<commit_message>
DA 16 | Day 6
</commit_message>
<xml_diff>
--- a/Batch/16/In_Class/Day_5.xlsx
+++ b/Batch/16/In_Class/Day_5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\16\In_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E88D0A-269F-4973-B83B-E80B169CE510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316311D9-D4E2-486D-99A2-5984892C90E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" tabRatio="748" activeTab="4" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" tabRatio="748" activeTab="3" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2002,18 +2002,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2053,8 +2053,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>19061</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
@@ -2073,7 +2073,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Ink 8">
@@ -2118,8 +2118,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>121694</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Ink 14">
@@ -2138,7 +2138,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="15" name="Ink 14">
@@ -2183,8 +2183,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>26959</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Ink 15">
@@ -2203,7 +2203,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Ink 15">
@@ -2248,8 +2248,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>131556</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="48" name="Ink 47">
@@ -2268,7 +2268,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="48" name="Ink 47">
@@ -2313,8 +2313,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>56676</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="53" name="Ink 52">
@@ -2333,7 +2333,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="53" name="Ink 52">
@@ -2378,8 +2378,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>47799</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="59" name="Ink 58">
@@ -2398,7 +2398,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="59" name="Ink 58">
@@ -2443,8 +2443,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>37719</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="72" name="Ink 71">
@@ -2463,7 +2463,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="72" name="Ink 71">
@@ -2508,8 +2508,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>28236</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="73" name="Ink 72">
@@ -2528,7 +2528,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="73" name="Ink 72">
@@ -2573,8 +2573,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>2234</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="75" name="Ink 74">
@@ -2593,7 +2593,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="75" name="Ink 74">
@@ -2638,8 +2638,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>36679</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="76" name="Ink 75">
@@ -2658,7 +2658,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="76" name="Ink 75">
@@ -2703,8 +2703,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9998</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="78" name="Ink 77">
@@ -2723,7 +2723,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="78" name="Ink 77">
@@ -2768,8 +2768,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>49517</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="79" name="Ink 78">
@@ -2788,7 +2788,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="79" name="Ink 78">
@@ -2833,8 +2833,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95875</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="81" name="Ink 80">
@@ -2853,7 +2853,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="81" name="Ink 80">
@@ -2898,8 +2898,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>141873</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="98" name="Ink 97">
@@ -2918,7 +2918,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="98" name="Ink 97">
@@ -2963,8 +2963,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>160716</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="120" name="Ink 119">
@@ -2983,7 +2983,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="120" name="Ink 119">
@@ -3028,8 +3028,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>181792</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="137" name="Ink 136">
@@ -3048,7 +3048,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="137" name="Ink 136">
@@ -3093,8 +3093,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>77793</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="138" name="Ink 137">
@@ -3113,7 +3113,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="138" name="Ink 137">
@@ -3163,8 +3163,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>48893</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Ink 7">
@@ -3183,7 +3183,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="8" name="Ink 7">
@@ -3228,8 +3228,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>160411</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="27" name="Ink 26">
@@ -3248,7 +3248,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="27" name="Ink 26">
@@ -3293,8 +3293,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>170054</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="33" name="Ink 32">
@@ -3313,7 +3313,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="33" name="Ink 32">
@@ -3358,8 +3358,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>105254</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="34" name="Ink 33">
@@ -3378,7 +3378,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="34" name="Ink 33">
@@ -3423,8 +3423,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>1857</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="43" name="Ink 42">
@@ -3443,7 +3443,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="43" name="Ink 42">
@@ -3488,8 +3488,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>17461</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="55" name="Ink 54">
@@ -3508,7 +3508,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="55" name="Ink 54">
@@ -3597,8 +3597,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>141100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="65" name="Ink 64">
@@ -3617,7 +3617,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="65" name="Ink 64">
@@ -3662,8 +3662,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>75992</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="74" name="Ink 73">
@@ -3682,7 +3682,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="74" name="Ink 73">
@@ -3727,8 +3727,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>162978</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="77" name="Ink 76">
@@ -3747,7 +3747,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="77" name="Ink 76">
@@ -3792,8 +3792,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>59098</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="86" name="Ink 85">
@@ -3812,7 +3812,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="86" name="Ink 85">
@@ -3857,8 +3857,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>67990</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="104" name="Ink 103">
@@ -3877,7 +3877,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="104" name="Ink 103">
@@ -3966,8 +3966,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>173242</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="122" name="Ink 121">
@@ -3986,7 +3986,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="122" name="Ink 121">
@@ -4031,8 +4031,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>170805</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="128" name="Ink 127">
@@ -4051,7 +4051,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="128" name="Ink 127">
@@ -4228,8 +4228,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>162820</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="144" name="Ink 143">
@@ -4248,7 +4248,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="144" name="Ink 143">
@@ -4293,8 +4293,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>74557</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="171" name="Ink 170">
@@ -4313,7 +4313,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="171" name="Ink 170">
@@ -4358,8 +4358,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>162839</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="172" name="Ink 171">
@@ -4378,7 +4378,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="172" name="Ink 171">
@@ -4423,8 +4423,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>1384</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="178" name="Ink 177">
@@ -4443,7 +4443,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="178" name="Ink 177">
@@ -4488,8 +4488,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>38988</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="188" name="Ink 187">
@@ -4508,7 +4508,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="188" name="Ink 187">
@@ -4553,8 +4553,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>150177</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId42">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="189" name="Ink 188">
@@ -4573,7 +4573,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="189" name="Ink 188">
@@ -4618,8 +4618,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>161583</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId44">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="190" name="Ink 189">
@@ -4638,7 +4638,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="190" name="Ink 189">
@@ -4683,8 +4683,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>131608</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="191" name="Ink 190">
@@ -4703,7 +4703,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="191" name="Ink 190">
@@ -4748,8 +4748,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>114050</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId48">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="193" name="Ink 192">
@@ -4768,7 +4768,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="193" name="Ink 192">
@@ -4813,8 +4813,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>141050</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId50">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="194" name="Ink 193">
@@ -4833,7 +4833,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="194" name="Ink 193">
@@ -4878,8 +4878,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>97376</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId52">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="195" name="Ink 194">
@@ -4898,7 +4898,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="195" name="Ink 194">
@@ -4943,8 +4943,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>77576</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId54">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="196" name="Ink 195">
@@ -4963,7 +4963,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="196" name="Ink 195">
@@ -5008,8 +5008,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>163010</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId56">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="197" name="Ink 196">
@@ -5028,7 +5028,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="197" name="Ink 196">
@@ -5073,8 +5073,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>150770</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId58">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="200" name="Ink 199">
@@ -5093,7 +5093,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="200" name="Ink 199">
@@ -5138,8 +5138,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>65696</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId60">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="211" name="Ink 210">
@@ -5158,7 +5158,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="211" name="Ink 210">
@@ -5203,8 +5203,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>144896</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId62">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="212" name="Ink 211">
@@ -5223,7 +5223,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="212" name="Ink 211">
@@ -5268,8 +5268,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>95115</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId64">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="215" name="Ink 214">
@@ -5288,7 +5288,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="215" name="Ink 214">
@@ -5333,8 +5333,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>93574</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId66">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="216" name="Ink 215">
@@ -5353,7 +5353,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="216" name="Ink 215">
@@ -5398,8 +5398,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>123555</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId68">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="218" name="Ink 217">
@@ -5418,7 +5418,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="218" name="Ink 217">
@@ -5463,8 +5463,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>116437</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId70">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="220" name="Ink 219">
@@ -5483,7 +5483,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="220" name="Ink 219">
@@ -5528,8 +5528,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>96555</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId72">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="222" name="Ink 221">
@@ -5548,7 +5548,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="222" name="Ink 221">
@@ -5593,8 +5593,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>105637</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId74">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="224" name="Ink 223">
@@ -5613,7 +5613,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="224" name="Ink 223">
@@ -5658,8 +5658,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>66050</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId76">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="225" name="Ink 224">
@@ -5678,7 +5678,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="225" name="Ink 224">
@@ -5723,8 +5723,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>36890</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId78">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="226" name="Ink 225">
@@ -5743,7 +5743,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="226" name="Ink 225">
@@ -5788,8 +5788,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>66050</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId80">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="227" name="Ink 226">
@@ -5808,7 +5808,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="227" name="Ink 226">
@@ -5853,8 +5853,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>65052</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId82">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="228" name="Ink 227">
@@ -5873,7 +5873,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="228" name="Ink 227">
@@ -5918,8 +5918,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>66770</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId84">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="232" name="Ink 231">
@@ -5938,7 +5938,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="232" name="Ink 231">
@@ -5983,8 +5983,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>85592</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId86">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="243" name="Ink 242">
@@ -6003,7 +6003,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="243" name="Ink 242">
@@ -6048,8 +6048,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>151717</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId88">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="244" name="Ink 243">
@@ -6068,7 +6068,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="244" name="Ink 243">
@@ -6113,8 +6113,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>57296</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId90">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="248" name="Ink 247">
@@ -6133,7 +6133,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="248" name="Ink 247">
@@ -6178,8 +6178,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>64578</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId92">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="252" name="Ink 251">
@@ -6198,7 +6198,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="252" name="Ink 251">
@@ -6243,8 +6243,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>163629</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId94">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="255" name="Ink 254">
@@ -6263,7 +6263,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="255" name="Ink 254">
@@ -6308,8 +6308,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>179109</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId96">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="266" name="Ink 265">
@@ -6328,7 +6328,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="266" name="Ink 265">
@@ -6373,8 +6373,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>57675</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId98">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="267" name="Ink 266">
@@ -6393,7 +6393,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="267" name="Ink 266">
@@ -6438,8 +6438,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>103118</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId100">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="272" name="Ink 271">
@@ -6458,7 +6458,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="272" name="Ink 271">
@@ -6503,8 +6503,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>66038</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId102">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="273" name="Ink 272">
@@ -6523,7 +6523,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="273" name="Ink 272">
@@ -6568,8 +6568,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>173203</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId104">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="277" name="Ink 276">
@@ -6588,7 +6588,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="277" name="Ink 276">
@@ -6633,8 +6633,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>85970</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId106">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="292" name="Ink 291">
@@ -6653,7 +6653,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="292" name="Ink 291">
@@ -6874,8 +6874,8 @@
       <xdr:row>47</xdr:row>
       <xdr:rowOff>65289</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId112">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="333" name="Ink 332">
@@ -6894,7 +6894,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="333" name="Ink 332">
@@ -6939,8 +6939,8 @@
       <xdr:row>47</xdr:row>
       <xdr:rowOff>17327</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId114">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="342" name="Ink 341">
@@ -6959,7 +6959,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="342" name="Ink 341">
@@ -7004,8 +7004,8 @@
       <xdr:row>42</xdr:row>
       <xdr:rowOff>164151</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId116">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="358" name="Ink 357">
@@ -7024,7 +7024,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="358" name="Ink 357">
@@ -7069,8 +7069,8 @@
       <xdr:row>42</xdr:row>
       <xdr:rowOff>170271</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId118">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="359" name="Ink 358">
@@ -7089,7 +7089,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="359" name="Ink 358">
@@ -7134,8 +7134,8 @@
       <xdr:row>42</xdr:row>
       <xdr:rowOff>66313</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId120">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="363" name="Ink 362">
@@ -7154,7 +7154,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="363" name="Ink 362">
@@ -7199,8 +7199,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>97556</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId122">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="367" name="Ink 366">
@@ -7219,7 +7219,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="367" name="Ink 366">
@@ -7264,8 +7264,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>30874</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId124">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="377" name="Ink 376">
@@ -7284,7 +7284,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="377" name="Ink 376">
@@ -7329,8 +7329,8 @@
       <xdr:row>44</xdr:row>
       <xdr:rowOff>135125</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId126">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="378" name="Ink 377">
@@ -7349,7 +7349,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="378" name="Ink 377">
@@ -7443,8 +7443,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114992</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="18" name="Ink 17">
@@ -7463,7 +7463,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="18" name="Ink 17">
@@ -7508,8 +7508,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>49162</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="19" name="Ink 18">
@@ -7528,7 +7528,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="19" name="Ink 18">
@@ -7617,8 +7617,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>26629</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="21" name="Ink 20">
@@ -7637,7 +7637,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="21" name="Ink 20">
@@ -7682,8 +7682,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>16841</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="22" name="Ink 21">
@@ -7702,7 +7702,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="22" name="Ink 21">
@@ -7747,8 +7747,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>86111</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="46" name="Ink 45">
@@ -7767,7 +7767,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="46" name="Ink 45">
@@ -7812,8 +7812,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>45349</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="47" name="Ink 46">
@@ -7832,7 +7832,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="47" name="Ink 46">
@@ -7877,8 +7877,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>154184</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="48" name="Ink 47">
@@ -7897,7 +7897,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="48" name="Ink 47">
@@ -7942,8 +7942,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>141517</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="54" name="Ink 53">
@@ -7962,7 +7962,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="54" name="Ink 53">
@@ -8051,8 +8051,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>114041</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="89" name="Ink 88">
@@ -8071,7 +8071,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="89" name="Ink 88">
@@ -8160,8 +8160,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>85154</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="97" name="Ink 96">
@@ -8180,7 +8180,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="97" name="Ink 96">
@@ -8225,8 +8225,8 @@
       <xdr:row>47</xdr:row>
       <xdr:rowOff>122066</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="111" name="Ink 110">
@@ -8245,7 +8245,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="111" name="Ink 110">
@@ -8290,8 +8290,8 @@
       <xdr:row>54</xdr:row>
       <xdr:rowOff>114213</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="163" name="Ink 162">
@@ -8310,7 +8310,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="163" name="Ink 162">
@@ -8355,8 +8355,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>27776</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="214" name="Ink 213">
@@ -8375,7 +8375,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="214" name="Ink 213">
@@ -8420,8 +8420,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>77538</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="220" name="Ink 219">
@@ -8440,7 +8440,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="220" name="Ink 219">
@@ -8485,8 +8485,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>161092</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="221" name="Ink 220">
@@ -8505,7 +8505,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="221" name="Ink 220">
@@ -8550,8 +8550,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>163500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="252" name="Ink 251">
@@ -8570,7 +8570,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="252" name="Ink 251">
@@ -8615,8 +8615,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>106990</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="253" name="Ink 252">
@@ -8635,7 +8635,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="253" name="Ink 252">
@@ -8685,8 +8685,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>171966</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -8705,7 +8705,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -8750,8 +8750,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>103648</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="4" name="Ink 3">
@@ -8770,7 +8770,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="4" name="Ink 3">
@@ -8815,8 +8815,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>106939</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Ink 4">
@@ -8835,7 +8835,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Ink 4">
@@ -8880,8 +8880,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>131798</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="10" name="Ink 9">
@@ -8900,7 +8900,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="10" name="Ink 9">
@@ -8945,8 +8945,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>171442</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Ink 15">
@@ -8965,7 +8965,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Ink 15">
@@ -9010,8 +9010,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>67724</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="41" name="Ink 40">
@@ -9030,7 +9030,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="41" name="Ink 40">
@@ -9251,8 +9251,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>74463</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="51" name="Ink 50">
@@ -9271,7 +9271,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="51" name="Ink 50">
@@ -9316,8 +9316,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>39625</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="61" name="Ink 60">
@@ -9336,7 +9336,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="61" name="Ink 60">
@@ -9381,8 +9381,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>27972</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="62" name="Ink 61">
@@ -9401,7 +9401,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="62" name="Ink 61">
@@ -9446,8 +9446,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28939</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="63" name="Ink 62">
@@ -9466,7 +9466,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="63" name="Ink 62">
@@ -9511,8 +9511,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>83463</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="64" name="Ink 63">
@@ -9531,7 +9531,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="64" name="Ink 63">
@@ -9576,8 +9576,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>170318</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="65" name="Ink 64">
@@ -9596,7 +9596,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="65" name="Ink 64">
@@ -9641,8 +9641,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>20564</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="68" name="Ink 67">
@@ -9661,7 +9661,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="68" name="Ink 67">
@@ -9706,8 +9706,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>10484</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="75" name="Ink 74">
@@ -9726,7 +9726,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="75" name="Ink 74">
@@ -9820,8 +9820,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>21117</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -9840,7 +9840,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -9885,8 +9885,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>58475</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="11" name="Ink 10">
@@ -9905,7 +9905,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="11" name="Ink 10">
@@ -9950,8 +9950,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>21883</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="12" name="Ink 11">
@@ -9970,7 +9970,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="12" name="Ink 11">
@@ -10015,8 +10015,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>49711</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="31" name="Ink 30">
@@ -10035,7 +10035,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="31" name="Ink 30">
@@ -10097,7 +10097,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">229 460 4210,'0'0'5997,"-16"-10"-5162,12 5 4016,3-24-3404,1 15-1224,-1 0 0,2 0 0,3-21 0,-4 31-223,1 1-1,0-1 0,0 1 1,0-1-1,1 1 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1 1 1,0-1-1,-1 1 1,1 0-1,4-3 1,-6 5-2,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1 0 0,11 22-68,-11-21 68,6 19-126,-1 1 0,-2-1 0,0 1 1,0 27-1,-3 54-691,0-100 783,3-58-67,3 0 0,2 0 0,24-84 1,-28 86 1150,-4 52-797,0 28-963,-2 45 777,0-36 36,2 0 0,6 56 0,-5-88-100,-1 0 1,1 0-1,0 0 1,0-1-1,0 1 1,0 0-1,1-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,1 0-1,0 0 1,0-1-1,-1 1 1,1-1-1,1 1 1,-1-1-1,0 0 1,1 0-1,-1-1 1,1 1-1,-1-1 1,8 3-1,-6-4-26,1 1 1,0-1-1,0 0 0,-1 0 0,1 0 1,0-1-1,-1 0 0,1 0 0,0 0 0,-1-1 1,1 0-1,-1 0 0,0 0 0,0 0 1,0-1-1,0 0 0,6-5 0,33-28-2129,14-11-6867,-42 40 4354</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="360.39">697 416 4002,'0'0'8881,"0"-10"-4479,9 151-3809,-9-130-777,0 1 0,-1 0 0,0-1 1,-1 1-1,-6 17 0,-18 23-5759,21-46 858</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1032.44">892 203 4370,'0'0'11016,"-14"-15"-8754,12 19-2192,0 0 1,1 1-1,0-1 0,0 1 0,0 0 1,0-1-1,1 1 0,0 0 0,0-1 1,0 1-1,2 9 0,-1 4-105,-1-16 29,1 0 0,-1 0 0,1 0 0,-1-1-1,1 1 1,0 0 0,0-1 0,-1 1 0,1 0-1,0-1 1,1 1 0,-1-1 0,0 0 0,0 1-1,1-1 1,-1 0 0,0 1 0,1-1 0,-1 0-1,1 0 1,0-1 0,-1 1 0,1 0 0,0 0-1,0-1 1,-1 1 0,1-1 0,0 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,3-1 0,0-40 163,-4-56 540,-1 96-169,0 4-696,2 35 88,2-1 0,2 0 0,2 0 0,13 38 0,-10-38 87,-2 1 0,-1 0 0,-2 0-1,1 42 1,-5-50-13,-1-21 5,-1-1 1,0 1-1,0-1 1,0 0-1,-1 1 1,0-1-1,-4 15 1,4-22 8,1 0 0,0-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1-1,1 1 1,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-2-2 31,1 1 1,-1-1-1,1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,1 1 1,-2-4-1,0-3-246,1 0 0,1 1 0,-1-1 0,2 0 0,-1 0 0,1 0 0,1 0-1,0 0 1,0 0 0,5-16 0,-2 13-771,1-1 1,1 1-1,0 0 1,1 1-1,0-1 1,16-19-1,15-16-3832</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1291.6">1189 11 5699,'0'0'7723,"0"0"-7709,0 0 0,-1-1-1,1 1 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,0-1 0,0 1-1,0 0 1,1 0 0,-1 0 0,0 0-1,0-1 1,0 1 0,1 0 0,1 0-10,0-1 1,1 1-1,-1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,3 2-1,39 24 311,-40-24-242,6 4-41,0 1-1,-1-1 0,0 1 1,-1 1-1,0 0 1,0 0-1,-1 0 0,0 1 1,-1 0-1,0 0 1,-1 1-1,0 0 0,0 0 1,-1 0-1,0 0 1,-1 1-1,-1-1 0,0 1 1,0 0-1,-1 20 0,-1-19-668,-1 0 0,0 1-1,-2-1 1,1 0-1,-2 0 1,1-1 0,-2 1-1,0-1 1,0 0-1,-1 0 1,-14 20-1,-26 27-5476</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1291.59">1189 11 5699,'0'0'7723,"0"0"-7709,0 0 0,-1-1-1,1 1 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,0-1 0,0 1-1,0 0 1,1 0 0,-1 0 0,0 0-1,0-1 1,0 1 0,1 0 0,1 0-10,0-1 1,1 1-1,-1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,3 2-1,39 24 311,-40-24-242,6 4-41,0 1-1,-1-1 0,0 1 1,-1 1-1,0 0 1,0 0-1,-1 0 0,0 1 1,-1 0-1,0 0 1,-1 1-1,0 0 0,0 0 1,-1 0-1,0 0 1,-1 1-1,-1-1 0,0 1 1,0 0-1,-1 20 0,-1-19-668,-1 0 0,0 1-1,-2-1 1,1 0-1,-2 0 1,1-1 0,-2 1-1,0-1 1,0 0-1,-1 0 1,-14 20-1,-26 27-5476</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1825.05">58 426 704,'0'0'15205,"-4"1"-14314,2 0-892,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,1-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,0-1-1,1 1 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 2 1,-8 56 121,6-38-34,-5 51 174,3 146 1,5-208-257,1-1 0,0 0 0,1 0 0,0 0 0,1 0 0,0-1 0,0 1 0,1-1 0,9 16 0,-10-20-58,1 1 0,-1-2 0,1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,0-1 0,1 1 0,-1-1 0,0 0 0,1-1 0,0 1-1,0-1 1,0 0 0,9 1 0,-2-1-526,1 0-1,0-1 1,-1-1-1,1 0 1,0-1-1,0-1 1,-1 0-1,22-6 1,-13-1-1437,0 0-1,20-14 1</inkml:trace>
 </inkml:ink>
 </file>
@@ -10186,12 +10186,12 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">550 1086 7603,'0'0'5710,"6"-2"-5318,26-9 95,1 1 0,37-6 0,19-6-337,-68 18-1002,-7 4-2506</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2172.72">1175 914 480,'0'0'10168,"-7"-5"-9566,3 3-488,0 0-1,0-1 0,0 1 0,0 0 0,0 1 0,0-1 1,-1 1-1,-8-2 0,11 3-80,-1 0 1,1 0-1,-1 1 0,1-1 1,0 1-1,-1-1 1,1 1-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,0 0-1,-1 2 0,-6 7-32,1-1 0,0 1 0,1 1 0,0-1 0,0 1 0,2 1 0,-1-1-1,2 1 1,0 0 0,0 0 0,-2 16 0,1-1 25,1 0 0,1 0 0,1 1 1,5 55-1,-2-78 15,1 1 1,-1-1-1,2 1 1,-1-1 0,1 0-1,0 0 1,0 0-1,1 0 1,0 0-1,0-1 1,0 1 0,1-1-1,-1 0 1,1-1-1,0 1 1,1-1-1,-1 0 1,1 0 0,0-1-1,0 1 1,0-1-1,0-1 1,0 1-1,12 2 1,6 1 163,1 0 0,0-2 1,1 0-1,-1-2 0,30-1 0,16-1-99,-1-4 0,77-13 0,31-19-180,144-19 310,-208 43-252,212-11-64,-305 23 78,1 1-1,0 1 0,0 1 1,0 1-1,29 9 0,-30-9 26,0-2 0,-1 0 0,1-1 0,0-1 0,0 0-1,22-5 1,-11-1-4,0-1 1,0-2-1,-1-1 0,-1-2 0,50-25 0,-75 34 2,-1 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,0-1-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 0,-1 1 1,1-1-1,-1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,2-8-1,0-10-8,0-1 1,-2 1-1,-1-28 0,0 24-159,-1 22 151,0 0 1,0 1-1,-1-1 0,1 0 1,-1 1-1,0-1 0,0 1 0,-1-1 1,1 1-1,-1 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,-5-4-1,-1-1-11,0 1-1,0 0 1,-1 1 0,-21-12 0,14 12-21,0 0 1,0 2 0,-1 0 0,0 1-1,-35-4 1,-98 4 37,117 4-22,-272 26-5,168-10 21,-325 31 17,291-26-13,95-10 0,-99 2-1,-65-13 89,240 0-131,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 1 0,0 1-914,0 1-1,1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,2 6 0,2-3-3898</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2172.71">1175 914 480,'0'0'10168,"-7"-5"-9566,3 3-488,0 0-1,0-1 0,0 1 0,0 0 0,0 1 0,0-1 1,-1 1-1,-8-2 0,11 3-80,-1 0 1,1 0-1,-1 1 0,1-1 1,0 1-1,-1-1 1,1 1-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,0 0-1,-1 2 0,-6 7-32,1-1 0,0 1 0,1 1 0,0-1 0,0 1 0,2 1 0,-1-1-1,2 1 1,0 0 0,0 0 0,-2 16 0,1-1 25,1 0 0,1 0 0,1 1 1,5 55-1,-2-78 15,1 1 1,-1-1-1,2 1 1,-1-1 0,1 0-1,0 0 1,0 0-1,1 0 1,0 0-1,0-1 1,0 1 0,1-1-1,-1 0 1,1-1-1,0 1 1,1-1-1,-1 0 1,1 0 0,0-1-1,0 1 1,0-1-1,0-1 1,0 1-1,12 2 1,6 1 163,1 0 0,0-2 1,1 0-1,-1-2 0,30-1 0,16-1-99,-1-4 0,77-13 0,31-19-180,144-19 310,-208 43-252,212-11-64,-305 23 78,1 1-1,0 1 0,0 1 1,0 1-1,29 9 0,-30-9 26,0-2 0,-1 0 0,1-1 0,0-1 0,0 0-1,22-5 1,-11-1-4,0-1 1,0-2-1,-1-1 0,-1-2 0,50-25 0,-75 34 2,-1 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,0-1-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 0,-1 1 1,1-1-1,-1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,2-8-1,0-10-8,0-1 1,-2 1-1,-1-28 0,0 24-159,-1 22 151,0 0 1,0 1-1,-1-1 0,1 0 1,-1 1-1,0-1 0,0 1 0,-1-1 1,1 1-1,-1 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,-5-4-1,-1-1-11,0 1-1,0 0 1,-1 1 0,-21-12 0,14 12-21,0 0 1,0 2 0,-1 0 0,0 1-1,-35-4 1,-98 4 37,117 4-22,-272 26-5,168-10 21,-325 31 17,291-26-13,95-10 0,-99 2-1,-65-13 89,240 0-131,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 1 0,0 1-914,0 1-1,1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,2 6 0,2-3-3898</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-942.12">616 106 4626,'0'0'5869,"-27"-4"-1605,292-39-4374,-262 40-1550,-10-3 681,-27-11 491,-46-16 1404,98 35-1273,-12-2 359,-1 0-1,0 1 0,0-1 1,0 1-1,1 0 1,-1 0-1,0 1 0,8 3 1,-9-3 11,0 0 1,0 1-1,-1 0 1,1-1 0,-1 1-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,-1 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,0 1 0,2 6-1,-3-5-109,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,-1-1 1,1 1-1,-1 0 1,0-1-1,-1 1 1,1-1 0,-1 0-1,-6 9 1,-10 13-2348,2 0-1822</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-368.55">530 541 5683,'0'0'7670,"-2"-3"-7011,2 2-648,0 1-1,-1-1 1,1 1 0,0 0 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,1 1 0,-1-1 0,0 1-1,0-1 1,0 1 0,1 0 0,-1-1 0,0 1-1,1-1 1,-1 1 0,0 0 0,1-1-1,-1 1 1,1-1 0,26-11 269,52-3 11,-50 10-252,11-4-37,-22 4-886,1 1 0,0 1 1,23-2-1,-33 3-6243,-18-5 4473,-20-6 1677,26 12 471,-33-12 711,2 2 1543,2-4 4114,32 14-4918,0-1-642,33 2-639,-30 0 352,1 0-1,-1 0 0,0 0 0,1 0 0,-1 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 1,0 0-1,0 0 0,0-1 0,2 7 0,-1-1-266,-1 1 1,0 0-1,0-1 1,-1 1-1,0 0 1,0 0 0,-1 0-1,0 0 1,-2 11-1,-1-1-2949</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4558.69">132 52 1409,'0'0'378,"0"17"113,0 98 771,0 22 3669,0-136-4782</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5204.68">1 643 496,'0'0'7908,"5"-14"-7078,21-42-340,-23 52-445,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,6 0 0,-9 2-45,0 0 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,0 1 1,-1 2-1,1 0 9,-2 29 133,-1 0 0,-1 0 1,-14 51-1,17-84-140,0 31 412,22-32-158,-14-2-81,1 0 1,0-1 0,-1 0 0,0 0-1,12-10 1,10-5 114,-26 18-402,-1 15-8369</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5752.47">38 1164 3265,'0'0'10021,"2"-4"-9663,4-5-286,1 1 0,0-1 0,1 1 0,0 1 0,0-1 0,1 1 0,-1 1 0,1 0 0,1 0 0,10-5 0,-9 9-75,-9 1-39,-2 34-6,-1-12 97,-1 0 1,0 0 0,-9 30-1,10-46-42,0-1-19,0 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0 1,-1-1-1,3 5 0,-2-5-17,0 0 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 0,-1-1 1,0 0-1,1 0 0,0 0 0,-1 0 0,8 0 1,-11-1 31,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,-1 1 0,-9 12 217,-17 6 106,-16 10-158,-7 5-308,16-16-2844,26-17-495,0-1-2476</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5752.46">38 1164 3265,'0'0'10021,"2"-4"-9663,4-5-286,1 1 0,0-1 0,1 1 0,0 1 0,0-1 0,1 1 0,-1 1 0,1 0 0,1 0 0,10-5 0,-9 9-75,-9 1-39,-2 34-6,-1-12 97,-1 0 1,0 0 0,-9 30-1,10-46-42,0-1-19,0 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0 1,-1-1-1,3 5 0,-2-5-17,0 0 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 0,-1-1 1,0 0-1,1 0 0,0 0 0,-1 0 0,8 0 1,-11-1 31,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,-1 1 0,-9 12 217,-17 6 106,-16 10-158,-7 5-308,16-16-2844,26-17-495,0-1-2476</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -10513,12 +10513,12 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">6845 749 2401,'0'0'8239,"0"-8"-6865,0-2-1918,0-25 4011,0 19-10,0 40-2738,0-8-717,-1 71 79,3 0 0,27 165 0,46 213 82,-75-369-101,-2-78-43,1-1 0,1 0 1,1 0-1,0 1 1,1-1-1,7 28 0,-14-53 152,0-1 0,0 2-1,-1-1 1,-10-10 0,5 6-181,1 0 1,0-1 0,-14-25 0,-14-49-370,66 140 354,2-1-1,3-2 1,65 78 0,-97-127 28,-1 0 1,1 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0-1 1,1 1 0,-1 0 0,0 0-1,0-1 1,1 1 0,-1-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,0-1 0,1 1-1,-1-1 1,0 0 0,0 1 0,2-2-1,2-3 28,-1 1 0,1-2 0,-1 1 0,0 0 0,-1-1 0,5-9 0,1 0-37,8-19 35,-1-1-1,-1-1 1,-2 0-1,8-39 1,-10 38-23,-8 20-1092,-3 16 836,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 1-1,1-1 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,1 0 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="982.52">6529 2350 880,'0'0'11200,"0"-8"-9559,0-32 2286,-6 42-3359,-6 24-413,2 1-1,1-1 0,1 2 1,1-1-1,-3 30 0,8-43-36,-1-1-63,0 0 0,1 0 0,1 1 0,0-1 0,1 0 0,1 1 0,2 16 0,-2-28-50,1 1 1,-1-1-1,1 0 0,0 1 1,-1-1-1,1 0 1,0 0-1,1 0 1,-1-1-1,0 1 0,0 0 1,1-1-1,-1 1 1,1-1-1,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0-1 1,0 1-1,-1-1 1,1 0-1,0 0 1,3 0-1,3 1 21,-1-1 1,1 0-1,0-1 0,-1 0 1,1 0-1,15-5 0,-15 3-194,-1-1 0,-1 0 0,1 0 0,-1-1 0,14-11 1,1-10-2845,-20 24 2397,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 1,-1-3-1,0-9-4897</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1209.25">6560 2492 3666,'0'0'10925,"0"0"-10887,-1 0 0,1 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0-1 1,0 1-1,-1 0 0,1-1 1,0 1-1,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 1,0-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,1-1-1,17-8 22,2 1 1,-1 1-1,23-6 1,30-11-1563,-29 1-2632,-34 14 1001,-7 1-1397</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1442.19">6564 2286 4258,'0'0'11133,"-1"-5"-10509,1 3-602,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 1,0 1-1,1-1 0,1-1 1,3-2 3,0 1 0,1-1 1,-1 1-1,1 0 1,12-5-1,-4 3-37,1 0 0,1 1 0,-1 0-1,34-3 1,-48 7-208,-1 1-1,1 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 1-1,-1-1 0,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,0 0-1,-1 1 0,1-1 1,-1 1-1,1-1 1,-1 3-1,6 14-4714</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1442.18">6564 2286 4258,'0'0'11133,"-1"-5"-10509,1 3-602,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 1,0 1-1,1-1 0,1-1 1,3-2 3,0 1 0,1-1 1,-1 1-1,1 0 1,12-5-1,-4 3-37,1 0 0,1 1 0,-1 0-1,34-3 1,-48 7-208,-1 1-1,1 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 1-1,-1-1 0,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,0 0-1,-1 1 0,1-1 1,-1 1-1,1-1 1,-1 3-1,6 14-4714</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4239.46">7010 2355 80,'0'-3'17958,"0"5"-16592,0 269-710,1-270-1265,1-1 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0-1-1,0 1 0,0-1 0,2 0 0,14-14-3963</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4850.92">7134 2358 2273,'0'0'8396,"0"-5"-7193,0-14 19,0 15 2150,0 22-3100,-1-7-98,0-1 0,-1 1-1,0-1 1,-1 0-1,0 0 1,-5 11-1,4-12-32,0 1-1,1-1 0,1 1 0,-1 0 0,2 0 0,-2 11 0,3-20-15,7-2-125,0 0 0,-1 0 0,1 0 0,0-1 0,-1 0-1,1 0 1,-1-1 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 1-1,1-1 1,-1-1 0,0 1 0,0-1 0,0 0 0,-1 0-1,0-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,-2 0-1,1 0 1,0 0 0,-1-1 0,-1 1 0,1-1 0,-1 0 0,0 1-1,0-1 1,-1-9 0,0 15 235,0 46-305,0 167 903,0-211-937,0 0 1,0 0-1,0 0 0,0 1 1,1-1-1,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,2 1 0,-2-2-328,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1-1 1,0 1-1,0 0 0,0 0 0,0-1 0,0 1 0,2-1 0,10-7-6847</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6162.87">7455 2182 1985,'0'0'9241,"0"-7"-7893,0-20 71,0 27-1362,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 1 1,-4 9 645,-18 295 312,23-219-854,-7 184 264,6-266-393,0 0-1,0 0 1,-1 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,-1 0 0,0-1 1,0 1-1,0 0 0,0-1 1,-1 1-1,1-1 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,-5 4 0,-2-2-12,0-1-1,-1 1 0,1-2 1,-1 1-1,0-2 0,1 1 1,-17-1-1,-212 18-27,-261 10-276,494-29 274,-1-1 1,1-1-1,0 1 1,-1-1-1,1 0 0,0 0 1,0-1-1,0 0 1,1 0-1,-1 0 0,1-1 1,-1 0-1,1 0 1,0 0-1,1-1 0,-1 1 1,1-1-1,0 0 1,-7-11-1,-5-10-9,0 0 0,-21-52 1,36 74 15,-14-36-51,2-1 0,2-1 0,-8-51 0,10 43 39,-27-84-1,29 115 27,1 0-1,1-1 1,0 0-1,1 0 1,-1-28-1,4 36-20,2 4-35,13 2-3,26-5 17,1 1 1,0 2 0,61-3-1,127 7 23,-148 5-2,139 10-121,1 1-780,-172-11 641,73-4-21,-109 2 297,-1-1 0,1 0 0,-1-1 0,0-1 0,0 0 0,0 0-1,17-10 1,-28 13 1013,3-1-3518</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8932.51">6315 2503 3025,'0'0'5723,"-5"-18"-2567,-10 11-2566,1 1-1,-1 1 0,0 1 1,-21-5-1,-8-1 47,-161-46 817,-262-85-825,157 8-365,32 13 122,109 56-76,61 26-123,-194-100 0,25-36 289,208 127-452,-1 4 0,-3 2 1,-147-58-1,188 85 40,-1-3 1,-52-35-1,8 5-77,18 17 19,-103-37 0,129 54 17,-7-2-230,40 40-78,-1 6 268,0-22 20,0 1 0,1-1 0,0 0 0,0 1-1,1-1 1,0 0 0,1 1 0,0-1 0,5 13-1,-4-19 13,-3-3 101,5-34 197,-2 18-316,1 0 0,0 0 0,1 1 0,1-1 0,14-25 0,-17 36-8,0 1-1,0-1 0,1 1 1,-1 0-1,1 0 1,0 0-1,1 1 0,-1-1 1,1 1-1,-1 0 1,1 0-1,0 1 0,0-1 1,0 1-1,0 0 1,1 1-1,-1-1 0,0 1 1,1 0-1,10-1 1,-9 2-24,1 0 1,-1 1 0,0-1 0,1 1 0,-1 0 0,0 1 0,0 0 0,0 0 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1 0 0,0 0 0,10 10 0,-9-7-761,0 0 1,0 1-1,-1 0 0,0 0 1,0 0-1,-1 1 1,5 11-1,1 8-3123</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9844.37">2233 1423 4386,'0'0'5957,"-3"-15"-5188,-13-47-89,15 57-540,-1 0 0,1 0 0,-1 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 1 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 0,-1 1 0,0-1 0,1 1 0,-1 1 0,0-1 0,0 0 0,-10-1 0,9 3-153,0-1 1,-1 1-1,1-1 1,-1 2-1,1-1 0,-1 1 1,1 0-1,0 0 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 1 1,1 0-1,-1 0 0,0 0 1,1 1-1,-6 5 1,3-1 11,0 0 0,1 0 0,1 1-1,-1 0 1,2 0 0,-1 1 0,1-1 0,0 1 0,1 0 0,-6 20 0,5-6 11,1-1-1,2 1 1,-1 46-1,3-67-8,0-1-1,0 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0-1 0,1 1 1,-1-1-1,1 1 1,-1-1-1,4 3 0,-1-1 7,0-1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 0 0,4 0-1,5 1-367,-1-2 0,0 0 0,0 0-1,0-2 1,1 1 0,13-5 0,41-23-5098,-37 14 1302</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9844.36">2233 1423 4386,'0'0'5957,"-3"-15"-5188,-13-47-89,15 57-540,-1 0 0,1 0 0,-1 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 1 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 0,-1 1 0,0-1 0,1 1 0,-1 1 0,0-1 0,0 0 0,-10-1 0,9 3-153,0-1 1,-1 1-1,1-1 1,-1 2-1,1-1 0,-1 1 1,1 0-1,0 0 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 1 1,1 0-1,-1 0 0,0 0 1,1 1-1,-6 5 1,3-1 11,0 0 0,1 0 0,1 1-1,-1 0 1,2 0 0,-1 1 0,1-1 0,0 1 0,1 0 0,-6 20 0,5-6 11,1-1-1,2 1 1,-1 46-1,3-67-8,0-1-1,0 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0-1 0,1 1 1,-1-1-1,1 1 1,-1-1-1,4 3 0,-1-1 7,0-1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 0 0,4 0-1,5 1-367,-1-2 0,0 0 0,0 0-1,0-2 1,1 1 0,13-5 0,41-23-5098,-37 14 1302</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9977.53">2246 1436 992</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10087.41">2246 1423 992,'26'-63'1759,"-23"57"-488,3-12 3982,-6 22-2262,-7 23-1755,-3 178 472,10-204-1909,0 1 0,-1-1 1,1 0-1,0 1 0,0-1 1,0 0-1,1 1 1,-1-1-1,0 0 0,0 1 1,1-1-1,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 1,0 1-1,0-1 0,2 1 1,11 0-4090</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10427.07">2353 1370 3570,'0'0'6419,"15"-15"-5937,47-45-111,-61 59-333,0-1 0,1 1 0,0-1-1,-1 1 1,1 0 0,0 0 0,0-1-1,-1 1 1,1 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 1 0,0 0 0,0-1-1,1 1 1,2 0 0,-3 0-14,-1 1 0,0-1-1,0 1 1,0-1 0,-1 1 0,1 0 0,0 0-1,0-1 1,0 1 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,1 2-1,0 5 178,0-1 0,-1 1 0,0 0 0,0 0-1,0 0 1,-2 7 0,-2-3 53,0-1-1,0 0 1,-1 0 0,-1 0-1,0-1 1,-10 15 0,9-15-34,0 0 0,1 1 0,0 0 0,0 0 0,1 1 0,-4 15 0,9-26-211,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 1,0 1-1,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,0 1 0,29-1 163,30-19-16,-24 5-237,32-15-2219,-62 26 1228,-1 0 0,0 0 0,0-1 1,0 0-1,7-8 0,1-3-5166</inkml:trace>
@@ -10650,7 +10650,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">188 186 7700,'0'0'9238,"-5"-8"-8643,2 1-604,-1 0 413,-1-1-1,2 0 1,-1 0-1,1 0 1,-4-16-1,7 21-363,0 0-1,-1 1 0,1-1 1,0 0-1,0 0 0,1 1 1,-1-1-1,1 0 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 1,1 0-1,0 0 0,-1-1 1,1 1-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,5-2-1,53-27 39,-56 30-84,0-1 1,0 0-1,1 1 1,-1 0-1,0 0 1,1 1-1,-1-1 0,1 1 1,-1 0-1,1 0 1,-1 0-1,1 1 1,4 0-1,-8 0 5,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,0-1-1,0 1 0,0-1 1,0 3-1,1 43 16,-2-35-13,0-4-3,0 0-1,0-1 1,-1 1 0,-1 0-1,1-1 1,-1 0-1,0 1 1,-1-1 0,0 0-1,0-1 1,0 1-1,-1-1 1,0 1-1,0-2 1,-7 7 0,-14 13-31,-57 41 0,75-60 25,-5 4-15,-49 32-258,59-40 256,0 0 1,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 0 0,0 1 0,-1-1 0,1-1 0,0 1 1,-1 0-1,-5-2 0,8 0-6,0 1 1,-1-1-1,1 1 0,1-1 1,-1 0-1,0 1 0,0-1 0,1 0 1,-1 0-1,1 0 0,-1 1 1,1-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1-1 0,-2 1 19,1 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,1 1 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,1 0 1,1-2-1,0 3-11,1-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1 0 0,7 3 0,-1 2-5,-1 1 1,1 0-1,-1 0 1,12 16 0,27 27 0,-44-49 22,1 1 1,0-1-1,-1 0 1,1 1 0,0-2-1,0 1 1,0 0-1,0-1 1,0 0 0,1 0-1,-1 0 1,0 0-1,9 0 1,-9-1 89,0 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 0 1,6-4-1,16-19 364,-9 4-3614,-2 3-2985,-6 7-3305</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="277.47">479 261 10261,'0'0'7107,"17"-6"-7043,-2 4 176,-1-2 160,4-2-128,-4 0-192,3 0 0,-6 2-80,0 0 0,-1 2-1280,-3 2-1569,0-2-1665,1 0-3650</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="277.46">479 261 10261,'0'0'7107,"17"-6"-7043,-2 4 176,-1-2 160,4-2-128,-4 0-192,3 0 0,-6 2-80,0 0 0,-1 2-1280,-3 2-1569,0-2-1665,1 0-3650</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="902.21">706 117 9060,'0'0'11083,"0"-4"-10955,0 121 1445,0-68-1382,0-38-381,0-15-243,0-226 1807,15 236-1830,-6 1 437,-1 1-1,0 0 1,0 0-1,-1 1 1,0 0-1,11 19 1,32 66 114,-39-71-118,-7-15 8,0 1 1,0 0-1,-1 0 0,0 0 0,-1 0 0,0 0 1,1 16-1,-3-23 14,1 1 0,-2-1 0,1 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1-1,-1-1 1,-8 3 95,1-1-1,0-1 0,0 0 0,-1-1 0,-13-1 1,22 1-158,1 0 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1-1 1,0 1-1,0-1 0,-1 0 1,1 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,0 0-1,0-4 0,0 3-126,0 1-259,-1 0 0,1 0-1,0 1 1,0-1-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 1 1,1-1-1,-1 0 1,1 0-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,3-1 1,13-8-7400</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1179.23">1147 208 10069,'0'0'10340,"-3"-4"-10340,3 0 0,11 0 0,3 0 64,11-4 16,-1 1-48,-2 1-32,2 0-832,-2 4-1201,-5 2-1472,-10 0-1602</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1397.31">1145 328 2401,'0'0'15815,"7"2"-15687,14-2 545,11-8-49,4-4-384,3 2-144,0 2-64,-7 0-64,-8 2-800,-2-1-993,-12 5-2369,1 0-1216</inkml:trace>
@@ -10661,7 +10661,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6831.23">3513 253 10805,'0'0'10605,"15"-10"-9541,62-10-722,32-7-336,-35 19-7837</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7046.06">3586 316 5138,'0'0'14663,"-4"0"-14551,22-2-48,7-6 80,3 0-128,4 0-16,0 2-96,0-2-944,-11 3-801,-3 3-1024,-11 0-1441</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7396.83">3623 101 10309,'0'0'10570,"-5"-3"-10407,-8-6-190,25 18-31,34 23 113,28 5 50,-55-30-103,0 2 1,-1 0-1,0 1 0,-1 1 0,0 1 0,28 25 0,-43-34-6,1 0 0,-1 0 1,0 0-1,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 0 1,0 1-1,-4 3 0,-7 9 50,0 0 0,0-2 0,-2 0-1,-24 20 1,36-31-256,-101 86 90,64-47-9026</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9622.3">4281 137 7876,'0'0'12053,"0"-3"-11778,-3 61 344,-13 76 1,-12 0-2852,15-106-4920</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9622.29">4281 137 7876,'0'0'12053,"0"-3"-11778,-3 61 344,-13 76 1,-12 0-2852,15-106-4920</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11364.01">4246 170 8820,'0'0'5776,"8"-12"-4477,23-36-701,-28 45-538,-1 1-1,1-1 1,0 1 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,1 1 0,-1 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,1 1 0,-1-1 0,1 1-1,-1 0 1,1 0 0,-1 0 0,1 0 0,0 1-1,3 0 1,-6 0-58,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,-1 1 1,1-1-1,0 0 0,-1 0 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 2-1,0 34 60,-1-26-31,0-3-31,0 0 0,0-1-1,-1 1 1,0-1 0,0 0 0,-1 1 0,0-1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,-1-1 0,0 0 0,0 0 0,-9 8 0,8-8-34,0 0 0,0-1 0,-1 0 1,1-1-1,-1 1 0,0-1 0,0 0 0,-1-1 1,1 0-1,-1 0 0,0-1 0,1 0 0,-1 0 0,-15 1 1,23-4 51,1 0 1,-1 0 0,1 0 0,-1-1 0,1 1-1,-1 0 1,1 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,2 0 0,0-1 2,1 1 0,0-1 0,0 1 0,0-1 1,1 2-1,-1-1 0,0 0 0,0 1 0,0-1 0,1 1 1,-1 0-1,0 1 0,0-1 0,1 1 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,6 3 0,-5-1 9,1 0 0,0 1 0,-1 0 0,0 0 0,0 0 0,0 1 0,-1 0 0,0-1 0,0 2 0,-1-1 0,4 8 0,9 9 44,-14-21-627,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,0-1-1,-1 0 0,1 1 1,4 0-1,-5-1 272,0-1 1,0 0-1,-1 0 0,1 1 0,0-1 0,0 0 0,-1-1 0,1 1 0,0 0 1,0-1-1,-1 1 0,1 0 0,0-1 0,-1 0 0,1 1 0,0-1 1,-1 0-1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 0 0,0-3 0,15-55 1635,-14 39 2384,-1 0 5686,-8 62-8911,2-19-333,2-1-1,0 1 0,0 31 0,3-52-174,0 0 1,1-1-1,-1 0 0,0 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 0 1,1 1-1,0-1 0,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 1,-1-1-1,1 1 0,0 0 1,-1 0-1,1-1 0,0 0 1,24-9 169,-22 6-154,1 0 1,-1 0 0,-1 0-1,1 0 1,0-1-1,-1 1 1,0-1 0,0 1-1,-1-1 1,1 0 0,-1 0-1,1-5 1,-1 7-32,-1 1-1,0 0 1,1 0 0,-1 0 0,0 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1-1 0,0 1 0,0 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 1-1,0 0 1,-3-2 0,0 0-90,-1 1-1,1 0 1,0 1-1,-1-1 1,1 1 0,-1 0-1,1 1 1,-9-1-1,32 7-951,-5-7 1032,0 0 1,-1-1 0,1-1-1,0 0 1,22-9 0,7-2-13,-36 14 52,-5 0-35,-1 17-60,-1-4 125,1-1-1,0 1 1,1 0-1,1-1 1,0 1-1,5 17 1,-7-29-46,1 0-1,-1 0 1,1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0-1,-1 0 1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,2 0-1,1-1 9,0-1-1,1 1 0,-1-1 0,0 1 0,-1-1 0,1 0 0,6-7 0,-7 7 6,0-1 0,0 0 0,0-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,0 0 0,0-8 0,0 13 302,0 25-422,-4 57 88,4-82 14,0 1 0,0-1 0,0 1 0,0-1-1,1 1 1,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0-1,-1 0 1,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,21-2-131,-18 0 82,0 1 0,0-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0-1 0,4-4-1,-3-2-27,0-1-1,-1 0 1,0 0-1,-1 0 1,0-1-1,0 1 1,-1-1-1,-1 0 0,0 0 1,0-11-1,-2 58 168,0-17 88,1 0 0,3 26 1,-3-44-173,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,1 0-1,-1-1 1,0 1 0,1 0 0,-1-1 0,0 1 0,1 0-1,-1-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0-1 0,-1 1 0,1 0-1,0-1 1,-1 1 0,1-1 0,1 0 0,31-25 181,-26 17-146,0 0 0,-1 0 0,0 0 0,-1 0-1,1-1 1,-2 0 0,1 0 0,-2 0 0,1-1 0,-1 1 0,-1-1-1,0 0 1,0 0 0,-1 0 0,-1-19 0,0 29-24,0 1 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,0-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1-1,0 0 1,-1-1-1,1 1 1,0 0-1,-1 0 1,1-1-1,-1 1 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,0 1 1,-1-1-1,1 0 1,-1 1-1,-23 15-167,23-15 95,0 1 0,0 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,1 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,2 1 0,4 3-407,1 0-1,-1-1 1,1 0-1,1 0 1,11 5-1,10 6-715,-28-15 1209,0 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1-1,0 0 1,1 4 0,-2-4 57,0-1 0,-1 1-1,1 0 1,0 0 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1 0-1,-1-1 1,1 1 0,-1 0 0,0-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,1 1-1,-1-1 1,0 0 0,0 1 0,0-1-1,1 0 1,-1 0 0,0 0-1,0 0 1,-1 1 0,-21 6 567,-20 8-35,17 0-7196</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11910.1">5312 406 7283,'0'0'6542,"0"-13"-4093,-18-368 1436,27 385-4128,-3 3 173,0 1 1,0-1 0,-1 1-1,0 1 1,-1-1 0,1 0-1,-1 1 1,-1 0-1,0 0 1,0 0 0,-1 1-1,0-1 1,-1 0 0,0 1-1,0-1 1,-1 1 0,0 0-1,-1-1 1,-2 13-1,3-19 41,-1-1 0,1 1-1,-1 0 1,0-1-1,0 1 1,0-1 0,0 0-1,-1 1 1,1-1-1,0 0 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,-1 0-1,1-1 1,0 1-1,0-1 1,-1 0-1,-3 2 1,-1-1-6,0-1 0,0 0 0,-1 0 1,1 0-1,0-1 0,-11-1 0,10 0 48,1 1 0,-1 0 0,1 1 0,-1-1 0,-14 5-1,20-5-10,1 1 0,-1 0-1,1 0 1,0 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,0 1-1,0-1 1,0 1 0,0-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 1 0,1 0-1,-1-1 1,1 1 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 2 0,0-1 0,0-1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 1-1,1-1 1,-1 0 0,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,1 1-1,-1 0 1,1 0 0,-1-1-1,4 3 1,-1-2 2,0 0 0,1 0 0,0-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1-1,1 0 1,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,0 0 0,-1 0 0,1 0 0,3-7 0,-5-2-3850</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12280.54">5656 269 5170,'0'0'11398,"-4"-4"-10707,4 2-666,-1 1 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,0 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1-1-1,1 1 1,0 0 0,-3 0 0,2 0-2,0 1 1,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,1 1-1,-1-1 1,0 1 0,0-1-1,1 1 1,-1 0 0,1-1 0,-1 1-1,0 2 1,-4 4 104,1 1 1,0-1-1,0 1 0,1 0 0,-5 16 1,7-20-108,1 0 0,-1 0 0,1 0 0,0 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,1 7 0,0-10-77,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1-1,0 0 1,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-2 0,0 1 0,1 0 0,2-1 0,1 1-710,1-1 0,-1 0 0,1 0 0,-1 0 1,0-1-1,0 0 0,1-1 0,7-3 1,9-12-3670,-4 0-195</inkml:trace>
@@ -10736,7 +10736,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1916.12">634 65 7139,'0'0'8388,"22"-8"-11141,-19 24 432,1 9-2850</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2929.89">767 247 6915,'0'0'7846,"7"4"-7349,-4-3-456,0 0 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 1 1,0-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0 0 1,-1-1-1,1 1 1,-1 0-1,0 0 1,0 0-1,0 0 1,-1 3 0,1 79 689,0-85-622,0-36 1484,1 30-1617,-1 1-1,1-1 1,0 1 0,0-1 0,0 1 0,1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0-1,1 1 1,5-7 0,-5 8 11,-1 0-1,1 0 1,-1 1 0,1-1-1,0 1 1,0-1-1,0 1 1,0 0 0,1 1-1,-1-1 1,1 0-1,-1 1 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 1 1,0-1 0,0 1-1,5 0 1,-8 0 8,1 1 0,0 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 2 0,2 59 11,-2-50 22,-5 17 205,12-50 172,2 1-434,1 1 1,0 0 0,2 1-1,0 0 1,1 1-1,0 1 1,2 0-1,16-14 1,-31 29 26,1-1 1,-1 1-1,1 0 1,-1-1-1,0 1 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,1 1 1,6 17 157,-7 40 405,-1-41-369,1 95-51,1-112-214,0 1-1,0 0 1,-1-1-1,1 1 0,0 0 1,0-1-1,0 1 1,0-1-1,0 0 1,1 1-1,-1-1 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,0-1 0,1 1 1,31-6-1423,-23 2 975,0-1-1,0 1 0,-1-1 1,1-1-1,-1 0 0,-1 0 1,14-13-1,-18 15 516,0 0 0,0-1 1,0 1-1,-1 0 0,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,0-1 1,0 0-1,0-5 0,-1 10 88,0 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,-1 1 0,1-1 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,0 0-1,1-1 1,-1 1 0,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,1-1 0,-1 1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 1 0,0-1 0,0 0-1,1 0 1,-1 1 0,-1-1 0,-1 1-3,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,0 1-1,-1 0 0,-3 2 0,-3 6 27,1 0-1,0 1 1,-13 21 0,18-26-100,0 0 0,1 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,2 0 0,-1-1 0,-1 12 0,4-18-40,-1 1 0,1-1 0,0 1-1,-1-1 1,1 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1-1,0 0 1,0 0 0,0-1 0,24-6-665,-13-1 426,-1 0-1,0-1 1,0 0-1,-1-1 1,0 0-1,10-13 1,-14 16 165,-5 5 612,10 51 2370,-11-46-2832,1 0 1,-1 0-1,1 0 0,0 0 1,-1 1-1,2-1 1,-1 0-1,0-1 1,0 1-1,1 0 0,0 0 1,0-1-1,-1 1 1,1-1-1,1 1 1,-1-1-1,0 0 0,3 3 1,0-3-720,0 0 0,0-1 0,1 1 0,-1-1 0,0 0 1,1 0-1,-1-1 0,0 0 0,11 0 0,12 0-7028</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4596.7">1706 205 6275,'0'0'7859,"-2"-6"-6799,2 4-1007,0 0 1,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,0 0 0,0-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,-3-1 0,2 2-41,0 0 1,0 1-1,0-1 0,1 0 0,-1 0 1,0 1-1,0-1 0,1 1 1,-1 0-1,0-1 0,1 1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 1-1,0-1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 1 1,-1 2-1,-5 6 23,1 1 0,0 0 0,1 0 0,0 1 1,1-1-1,0 1 0,0 0 0,2 0 0,-1 0 0,2 1 0,0-1 0,0 0 0,1 1 0,3 23 1,-3-34-53,1-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1 0,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,0 0 1,1 0 0,2-1-1,46-7-1424,-40 4 1088,1-2-1,-1 0 0,0 0 0,-1 0 0,1-1 0,-1-1 1,-1 0-1,1 0 0,-1-1 0,-1 1 0,8-13 0,-6 8 278,0 0 0,-1 0-1,-1-1 1,0 0 0,-1 0-1,-1-1 1,7-29-1,-10 3 2483,-2 26 800,-15 29-2847,5 7-279,1 2-1,0-1 1,2 1-1,1 0 1,1 1 0,1-1-1,1 1 1,0 37 0,3-60-77,0-1-1,0 0 1,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1-1,0-1 1,13-11 81,68-91 134,-77 105-138,-2 11-40,-1 13 304,-2-3-201,1-16-49,-1 0 0,1 0-1,0 1 1,1-1 0,0 0 0,2 8-1,-3-13-173,1 0-1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 1,1-1-1,-1 0 0,0 1 0,0-1 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 0 0,-1-1 1,1 1-1,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 1,-1 0-1,1 1 0,0-1 0,0 0 0,-1 0 0,4-1 1,5 2-804,0-2 1,0 1-1,0-2 1,0 1-1,-1-1 0,1-1 1,0 1-1,-1-2 1,0 1-1,18-11 1,-23 11 646,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 0 0,1 0 1,-1 0-1,3-7 0,-3 5 684,0 1 0,-1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1-9 0,-1 12-73,0 0 0,0 0-1,-1 0 1,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,-4-4 0,4 5-332,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-2 2 0,-5 6-34,0 0 0,0 0 0,1 1 0,0 0 0,1 0 0,0 0 0,0 1 0,1 0 0,1 0 1,0 0-1,0 0 0,1 0 0,1 1 0,-1 16 0,2-27-42,1-1 0,-1 1-1,0-1 1,1 0 0,-1 1 0,1-1 0,-1 0 0,0 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 1-1,1-1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1 0 0,1 0 0,0-1-1,19-6-501,-11-2 551,0 1 0,0-1 1,-1-1-1,0 1 0,-1-1 0,0-1 1,0 0-1,-1 0 0,8-22 1,-14 134 484,0-100-503,1-1-1,-1 0 1,0 1 0,0-1-1,0 0 1,0 1 0,1-1-1,-1 0 1,0 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,0 0 1,1 0-1,-1 0 1,0 1 0,1-1-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,1 1-1,-1-1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,0-1 1,1 1 0,15-10-111,-7 1 153,-6 6 34,0 0-1,0 1 0,0-1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,2-6 0,-4 9 327,0 40-378,-1-23 6,1-13-26,0 1 0,0 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,1 0 0,1 5 0,-1-8-19,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,0 0 0,-1 0 1,2 0-1,3-1 3,0 0-1,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 1,-1-1-1,0 0 0,0 1 0,-1-2 0,1 1 0,-1-1 0,1 1 1,-1-1-1,0 0 0,-1-1 0,1 1 0,-1-1 0,1 1 1,-1-1-1,-1 0 0,5-9 0,-8 17 48,0 0 1,1 0-1,-1-1 0,1 1 0,0 0 1,0 0-1,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1 0 1,0-1-1,0 1 0,0 0 0,0-1 1,1 1-1,2 4 0,-3-7-54,-1 1 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1-1,2 0 1,-2 0 22,1-1 1,-1 1-1,1 0 1,-1-1-1,1 0 0,-1 1 1,0-1-1,1 0 0,-1 0 1,0 0-1,0 1 1,1-1-1,-1-1 0,0 1 1,0 0-1,0 0 1,0 0-1,0 0 0,1-3 1,1-5 129,1 1 0,-2-1 0,1 0 1,-1 1-1,-1-1 0,1 0 0,-2 0 0,1 0 0,-1 0 1,0 0-1,-3-13 0,2-12-70,-2 17-93,3 17-47,0 1 0,0-1 1,0 0-1,0 0 0,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0 0-1,0 0 0,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0-1-1,0 1 0,-1 0 1,1 0-1,0-1 1,0 1-1,0-1 0,-6 15-5678</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5173.48">2631 247 9172,'0'0'7313,"-15"4"-7214,-48 15 13,60-19-108,1 1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,0 4 0,23-9-3131,26-27 212,-39 17 7823,-10 25-4727,-1-4-45,1-1 1,0 0-1,1 1 0,-1-1 0,1 0 0,4 14 0,-4-20-109,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,1 0 0,1 0 36,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,3-1 0,7-6 0,0-1 0,0-1-1,-1 1 1,0-2-1,-1 0 1,0 0-1,-1-1 1,0 0 0,-1 0-1,10-24 1,-9 18-76,-2-1 1,0 1 0,-2-1-1,0 0 1,-1-1 0,-1 1-1,1-33 1,-4 53 10,0-1-1,0 1 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,-1-1-1,1 1 1,0 0 0,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0-1,-1 0 1,1-1 0,-1 1-1,-15 8-206,-10 26-34,16-9 130,2 0 0,1 1 0,1 0-1,1 0 1,1 0 0,1 0 0,2 1 0,1 32-1,0-54-12,0 0 0,0-1 0,1 1-1,-1 0 1,1-1 0,0 1 0,0-1 0,1 1-1,-1-1 1,4 7 0,-3-9-244,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,4-1 0,9 1-6233</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5173.47">2631 247 9172,'0'0'7313,"-15"4"-7214,-48 15 13,60-19-108,1 1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,0 4 0,23-9-3131,26-27 212,-39 17 7823,-10 25-4727,-1-4-45,1-1 1,0 0-1,1 1 0,-1-1 0,1 0 0,4 14 0,-4-20-109,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,1 0 0,1 0 36,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,3-1 0,7-6 0,0-1 0,0-1-1,-1 1 1,0-2-1,-1 0 1,0 0-1,-1-1 1,0 0 0,-1 0-1,10-24 1,-9 18-76,-2-1 1,0 1 0,-2-1-1,0 0 1,-1-1 0,-1 1-1,1-33 1,-4 53 10,0-1-1,0 1 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,-1-1-1,1 1 1,0 0 0,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0-1,-1 0 1,1-1 0,-1 1-1,-15 8-206,-10 26-34,16-9 130,2 0 0,1 1 0,1 0-1,1 0 1,1 0 0,1 0 0,2 1 0,1 32-1,0-54-12,0 0 0,0-1 0,1 1-1,-1 0 1,1-1 0,0 1 0,0-1 0,1 1-1,-1-1 1,4 7 0,-3-9-244,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,4-1 0,9 1-6233</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -10768,7 +10768,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="201.75">746 193 12086,'0'0'3185,"65"-34"-4065,-47 26-1025,-7-2-608,-8 1-2530</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="387.39">502 110 9877,'0'0'3745,"62"-8"-14550</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="774.42">1073 240 7700,'0'0'9423,"-10"2"-7289,83-12-773,-29 3-3873,-13 5-6283</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1056.64">1080 339 11397,'0'0'8185,"22"0"-7937,-9-3-95,1-1-1,-1 0 1,0 0-1,13-7 1,-10 3-3529,-5 0-3514</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1056.63">1080 339 11397,'0'0'8185,"22"0"-7937,-9-3-95,1-1-1,-1 0 1,0 0-1,13-7 1,-10 3-3529,-5 0-3514</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1642.75">1105 144 5747,'0'0'11837,"-3"-5"-10508,-14-19 1341,56 38-3246,13 6 620,-40-16-54,1 0-1,-1 1 1,0 1-1,0 0 1,12 8-1,-23-12 1,1-1 0,-1 1-1,0 0 1,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 2-1,-27 59 121,18-43-124,-26 51 73,17-37-1868,-19 51 0,37-79-1737</inkml:trace>
 </inkml:ink>
 </file>
@@ -10838,7 +10838,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">464 120 4786,'0'0'6990,"-1"-3"-5963,0 2-953,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,-1 0-1,1 1 1,-1-1 0,1 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 1-1,-1-1 1,1 0 0,-1 1 0,1-1-1,0 1 1,-3 1 0,-2 1-78,1 1 1,0 0-1,0 1 0,0-1 0,1 1 1,0 0-1,-1 0 0,2 0 1,-1 1-1,1-1 0,-4 8 0,-29 72-42,23-45 25,2 0-1,1 1 0,3 0 0,1 1 1,2 0-1,1 46 0,3-85 12,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 1,0-1-1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1-1 0,2 1 0,-1 0 0,0 0 0,0-1 0,5 3 0,-2-2-61,0 0 0,1 0 0,0 0 0,0-1 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 0 0,8-1 0,-12 1 61,0-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,-1-1 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 0 1,-1 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,-1-1 0,1 1 0,-1 0 1,1-3-1,2-6 14,-2-1 0,1 0 0,-2-22 0,0 28 23,0 4-18,0 1-1,-1-1 1,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,0-1 0,1 1-1,-1-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,-1 1-1,0-1-30,1 0-1,-1 0 1,1 0-1,-1 1 0,1-1 1,0 1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,0 0-1,1 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,-1 3 0,1 33-5885,1-32 984</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="307.71">666 481 8356,'0'0'4578,"5"-2"-5010,4 10 160,1 11 256,0 4 16,-5-1 80,0 3 32,-5-3-96,0 1 32,0 2-48,0-6-497,-15-2-2112,0-9-3602</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="307.7">666 481 8356,'0'0'4578,"5"-2"-5010,4 10 160,1 11 256,0 4 16,-5-1 80,0 3 32,-5-3-96,0 1 32,0 2-48,0-6-497,-15-2-2112,0-9-3602</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="786.87">822 275 8324,'0'0'4647,"9"-18"-4567,34-56 46,-42 72-102,0 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,0 2 0,1-1 0,0 0 0,-1 0 0,1 1-1,-1 0 1,1-1 0,0 1 0,-1 0 0,5 1 0,0-1 15,-6 0-43,0 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,-1 1 0,0-1-1,1 0 1,-1 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,-1 1 0,0-1-1,1 1 1,-1-1 0,0 1 0,1-1-1,-1 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 1 0,0 1 0,0 20-57,0-19 63,0 181-120,4-183 99,0 0-1,-1 0 1,1 0 0,0 0-1,0-1 1,0 1-1,0-1 1,4 0 0,-3 0 6,0 0 1,0 1 0,0 0 0,1 0-1,-1 1 1,-1-1 0,1 1-1,0 0 1,0 0 0,-1 1-1,1 0 1,-1-1 0,0 1 0,0 1-1,0-1 1,0 1 0,3 3-1,-5-4 6,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 0 0,1 1 0,-4 3 0,-6 6-36,0-1 0,0-1 0,0 0 0,-2 0-1,1-1 1,-1-1 0,-24 12 0,28-18-2307</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1037.06">1303 9 9236,'0'0'3874,"126"-9"-3730,-97 35 112,1 1 48,-6 10-176,0 7-128,-9 9 0,-15 3-144,0 8-512,-10-3-1809,-24-8-2097</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1632.62">3 311 4898,'0'0'6489,"0"9"-6300,-1 58 104,-1-17 76,3 0-1,10 83 1,-8-120-343,0 1 1,0 0-1,1-1 0,0 0 0,2 0 1,-1 0-1,2-1 0,-1 0 0,2 0 1,0 0-1,0-1 0,1 0 0,0-1 1,16 14-1,-19-19-127,-1-1-1,1 0 1,1 0 0,-1 0 0,0-1 0,1 0 0,0 0-1,0-1 1,0 0 0,12 2 0,44-3-4837,-29-5-1964</inkml:trace>
@@ -10870,7 +10870,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">118 60 7700,'0'0'7011,"0"0"-6989,0 1 1,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-17 80 2009,-1 13-1151,9-36-2254</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="533.34">5 107 2561,'0'0'10941,"-1"0"-10698,1 0 1,-1-1-1,1 1 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 1,1-2-1,10-4-237,1 1 0,0 0 0,1 1 0,-1 0 0,1 0 0,15-1 0,-8 1 0,11-4 15,-16 3 15,1 1 1,-1 1 0,25-2 0,-39 5-163</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="533.33">5 107 2561,'0'0'10941,"-1"0"-10698,1 0 1,-1-1-1,1 1 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 1,1-2-1,10-4-237,1 1 0,0 0 0,1 1 0,-1 0 0,1 0 0,15-1 0,-8 1 0,11-4 15,-16 3 15,1 1 1,-1 1 0,25-2 0,-39 5-163</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="953.06">259 125 9428,'0'0'8903,"-2"-9"-7817,-2 12-1076,0 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 1 0,1 0 0,-1 0 0,1-1 0,0 2 0,0-1 0,0 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 10 0,2-13-17,0-1-1,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1-1-1,3 0 1,0 1 38,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 0-1,0 0 1,6-3 0,-8 1-5,1 1-1,0 0 0,-1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1-1-1,-1 1 0,0 0 0,0 0 1,-1 0-1,-1-7 0,1 10-85,-1 0 0,1 1 0,-1 0-1,1-1 1,-1 1 0,0 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1 0,-1 0-1,1-1 1,0 1 0,-1 0 0,-1 1-1,-10 20-2970,9-3-2270,4-7-976</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1925">491 158 9540,'0'0'10042,"-5"1"-9807,1 1-234,0-1 0,0 1 0,1 0 0,-1 1 1,0-1-1,1 0 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 1,-1 1-1,1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 0 1,1 0-1,-1 1 0,1-1 0,0 0 0,0 7 0,1-10-20,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,2 1 0,41-7-999,-39 5 776,0 0 1,-1 0-1,1 0 1,-1-1-1,0 0 1,0 1-1,0-2 1,0 1-1,0 0 1,-1-1-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,0 1 1,0-1-1,0 0 0,0 1 1,1-6-1,1-9 343,-1 0 0,-1 0 0,-1 0 0,-1-23-1,0 37 236,0 5-266,0 0 1,0 0 0,0 1-1,0-1 1,0 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1-1 1,1 1-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0-1 1,-2 22 526,0 0 1,-9 38-1,6-38-377,1 0 0,-2 40 0,7-60-215,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 1,0 0-1,-1 0 0,2-1 0,22-8 286,-16 3-224,0 0 0,-1-1 0,1 0 0,10-14 0,-6 7-47,-12 14-52,1 0 8,0 0-1,0 0 1,-1 1 0,1-1-1,0 0 1,-1 1 0,1-1-1,0 0 1,0 1 0,-1-1-1,1 1 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0 0,-1-1-1,0 1 1,1-1 0,-1 1-1,1 1 1,0-1 31,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0-1-1,0 1 1,-1 0-1,1-1 1,0 1 0,0 0-1,0-1 1,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,1 0 0,-1 0-1,1 1 1,2-1-12,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1-1 1,-1 0 0,1 1-1,-1-1 1,1-1-1,-1 1 1,0 0 0,1-1-1,-1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1-1 1,1 1-1,-1-1 1,1 1 0,-1-1-1,0 0 1,0 0-1,0 0 1,0-1 0,-1 1-1,1 0 1,-1-1-1,0 1 1,0 0 0,0-1-1,0 0 1,-1 1-1,1-1 1,-1 1 0,0-1-1,0-4 1,0 7-18,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 0,-1-2 0,0 3 10,1-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,-1 1 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 1-1,0 1 0,-2 3 15,0 2-1,1-1 0,-1 0 0,1 1 0,1-1 0,-1 1 1,1-1-1,1 1 0,-1 0 0,2 7 0,-1-14-73,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 1,0 1-1,1-1 1,-1-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,2-1 1,43-5-5547,-15-6 154</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2603.17">947 105 8116,'0'0'8510,"-8"7"-7608,-26 27-294,33-33-596,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,1 0 0,-1 1 0,0-1-1,1 0 1,-1 1 0,1-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,1 0 0,-1 1 0,0-1-1,1 1 1,-1-1 0,2 2-1,-1-1-18,1-1-1,-1 0 1,1 1-1,0-1 0,-1 0 1,1 0-1,0-1 1,0 1-1,-1 0 0,1 0 1,0-1-1,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,2 0 1,1-1-38,0 1-1,-1-1 1,1 0 0,0 0 0,-1 0 0,1-1-1,-1 0 1,0 0 0,1 0 0,-1 0-1,0-1 1,0 1 0,0-1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,-1-1 0,0 1 0,-1-1-1,1 0 1,-1 0 0,1 0 0,-1-1 0,2-5-1,1-4 186,0 1 0,-1-1-1,0 0 1,-1 0-1,-1 0 1,0 0-1,-1-18 1,-2 39-21,0 0 1,0-1-1,-1 1 0,0 0 1,0-1-1,-7 12 0,-5 19-68,9-18-51,1 1 0,0 0 0,-1 30 0,23-70 330,-12 14-212,8-8-116,0 0 0,0 0 0,1 2 0,1-1 0,0 2 0,1 0 1,0 2-1,26-12 0,-41 20-45,-27 10-128,-105 56 131,129-65 31,1 0 1,-1 0-1,0 0 0,1 1 0,-1-1 0,0 0 1,1 1-1,-1-1 0,0 1 0,1-1 1,-1 0-1,1 1 0,-1 0 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 1 0,1 0 1,0-1-1,-1 1 0,1 0 0,0 0 0,0-1 1,-1 2-1,15 10-328,30-1 135,8-6-913,84-1 0,-109-5-1116</inkml:trace>
@@ -10931,7 +10931,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">177 119 1377,'0'0'6024,"-3"-3"-4968,-5-6-676,5 7-170,1 0 0,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 0 0,1 1 1,0-1-1,-3-4 0,4 5-153,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0-1,-1 0 1,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,3-1 0,2-2-72,0 0 0,0 0 1,1 0-1,-1 1 0,1-1 1,0 2-1,0-1 0,0 1 1,0 0-1,0 1 0,0-1 1,1 2-1,-1-1 0,0 1 1,13 1-1,-18 0-28,-1 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,1 1 1,-1-1-1,0 1 0,1 0 0,-1-1 1,0 1-1,0 1 0,2 45-115,-2-44 147,1 10-36,-1 1 1,-1-1 0,0 0-1,-1 0 1,0 1-1,-1-1 1,-1-1-1,0 1 1,-6 13 0,-14 24-29,16-36 51,0 0 0,1 1 1,0 0-1,2 1 0,0 0 0,0 0 1,2 0-1,0 0 0,-1 22 0,4-39 16,0 1-1,0 0 0,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 1,0 1-1,1 0 0,-1-1 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,1 1 0,1-1 1,25-2 9,25-22 179,-47 21-142,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 0 0,0 0-1,0 0 1,0-1 0,0 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1-1,-1 0 1,0-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,-1 0 0,1-7-1,-3 13-41,1 1-1,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 2 0,-9 11 7,1 1 1,1 1-1,0 0 1,2 0-1,-1 1 0,-6 24 1,-23 114 24,13-48-18,-3 3 34,-22 190 0,11-31-78,37-263 36,0-1 0,-1 1 0,1 0-1,-1-1 1,0 1 0,0-1 0,-1 0 0,1 0-1,-1 0 1,0 0 0,-6 7 0,7-10 10,1 0 0,-1-1 0,1 1 0,-1 0 1,0-1-1,1 1 0,-1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0-1 0,0 1 1,0 0-1,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 1,-3-2-1,4 2-83,0 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1-1 0,1 1-1,0 0 1,-1 0 0,1-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,1 0-1,-1 0 1,0-1 0,1 1 0,-1 0-1,2-2 1,13-33-3442,5 3-1556</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="635.28">743 620 1409,'0'0'6941,"-32"76"-6516,23-59-406,1-1 0,1 1 0,1 0 0,0 1 0,1 0 0,1 0-1,1 0 1,-2 21 0,6-38-12,-1 0-1,1 0 0,0-1 0,0 1 0,-1 0 1,1-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 1,1-1-1,33-6 169,-29 4-621,-1 0 0,0 0 0,-1-1 0,1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,6-10 0,-6 5-1385</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="911.35">687 744 1665,'0'0'3954,"27"0"-3666,-10-6-176,1-1-96,-4 2-16,-2 0 0,0 2-80,-6-1 80,0 1-400,-3-1-993,-3 1-1216</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="911.34">687 744 1665,'0'0'3954,"27"0"-3666,-10-6-176,1-1-96,-4 2-16,-2 0 0,0 2-80,-6-1 80,0 1-400,-3-1-993,-3 1-1216</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1209.25">719 610 2401,'0'0'3554,"4"-2"-3448,5-2-676,7-5 1615,1 1 0,24-8 0,-10 12-6029,-25 6 1838</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1550.22">939 695 2321,'0'0'8553,"0"-1"-8427,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,-1 1 0,1-1-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 0 0,1 1-1,-2-2 1,-8 7-107,0 1 0,1-1 1,-1 1-1,1 1 0,0 0 0,1 0 1,0 1-1,-13 15 0,16-17-29,0-1-1,0 1 0,1 0 1,0 0-1,0 0 1,1 1-1,0-1 0,-4 12 1,2 14-5401</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1771.88">841 697 1121,'0'0'5960,"1"-1"-5936,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 1,0 0-1,2 1 0,25 49 2429,11 12-4023,-33-57-1311,2-1-798</inkml:trace>
@@ -10965,7 +10965,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">106 17 592,'0'0'7110,"0"-17"-453,-1 30-6670,-1 0 1,-1 0 0,0 0 0,-1-1 0,0 1 0,-9 16 0,-12 39 51,18-38-4,2-7 25,-1 0 0,-1 0 0,-16 35 0,23-58-17,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0-21 312,7-28-663,-3 35 243,5-16-243,1 0 0,2 1 0,0 0 0,26-41-1,-38 69 297,1 0-1,-1-1 1,1 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,1 1 1,-1-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,0-1-1,1 1 0,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 1 1,1-1-1,-1 0 0,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 0,0 0 1,1 0-1,1 2-13,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,-1 1 0,0-1 0,0 1 0,0-1 0,0 5 0,3 48 217,-4 79 1,-1-56-1530,0-70-1295,-4-4-1452</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="275.9">83 227 3105,'0'0'5523,"38"-22"-4963,-20 17-160,2-3-95,1 3-1,-1 0-128,1-2-96,-3 4-80,-4 1-192,-2 0-1569,-3 1-1809,-3-1-880</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="275.89">83 227 3105,'0'0'5523,"38"-22"-4963,-20 17-160,2-3-95,1 3-1,-1 0-128,1-2-96,-3 4-80,-4 1-192,-2 0-1569,-3 1-1809,-3-1-880</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="600.48">374 34 3314,'0'0'7768,"0"-3"-7502,0 9-358,-1 31 536,-3 0 1,0 1-1,-3-1 0,-1-1 1,-1 0-1,-3 0 0,0 0 1,-22 39-1,33-71-1242,-1 1 0,0-1 0,1 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,1 6 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="911.02">318 215 3794,'0'0'5421,"5"-7"-5232,-3 4-184,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0-1,3 1 1,-5-1-4,0 0 1,1 0-1,-1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,1 0 1,-1-1-1,0 1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,0 0-1,-1 1 0,3 2 0,-3-3 25,0 0-1,-1 1 1,1-1 0,0 0 0,-1 1-1,0-1 1,1 1 0,-1-1-1,0 1 1,0-1 0,1 1 0,-1-1-1,0 0 1,-1 1 0,1-1 0,0 1-1,0-1 1,-1 1 0,1-1-1,0 1 1,-1-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,-2 2-1,-3 2 127,0 0 0,0 0 1,-1 0-1,1 0 0,-1-1 0,0 0 0,0-1 0,-12 5 0,12-5-172,0-1 0,0 1 1,0 1-1,1-1 0,0 1 0,0 1 1,0-1-1,0 1 0,-5 6 1,9-6-1687</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1245.28">595 10 1553,'0'0'9159,"0"0"-9139,0 0 1,-1 0 0,1 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0-1-1,-1 1 1,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 1-1,0-1 1,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 1 0,-3 7 2,0 0 0,1 0 0,0 0 0,1 1 0,0-1 0,0 1 0,0 8-1,-1 13 257,-5 5 392,-2-1 0,-1 0 0,-2-1 0,-1 0 0,-2-1 1,-23 38-1,4-4-813,29-52-140,5-8-2246,17-25-8791</inkml:trace>
@@ -11102,9 +11102,9 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">80 151 2593,'0'0'9871,"0"0"-9732,1-1-1,-1 1 1,0-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,0 0 0,0-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,-1-1 1,1 1-1,0 0 1,-1 0 0,1-1-1,-1 1 1,-4 3-153,-1 1 0,1-1 0,0 1 0,0 0 0,1 1-1,-1-1 1,1 1 0,0 0 0,0 0 0,0 0 0,1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,1 0 0,-1 1 0,1-1 0,1 0 0,-1 12 0,2-17 9,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 1,-1 0-1,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,2-1 0,28 0 37,-26 0-35,1-1 0,0 1-1,-1-1 1,0 0 0,1 0-1,-1-1 1,0 0 0,0 0-1,0 0 1,-1 0 0,1-1-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,0 0-1,0-1 1,0 1 0,-1-1-1,2-8 1,-3 14 78,-14 40-801,13-39 716,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,0 0-1,-1-1 1,1 1 0,0 0-1,1 0 1,-1 0 2,1 0 1,0-1-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,3-2-1,-1 1-3,-1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,-1-1 1,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,-1-1 1,1 0-1,-1 0 1,1-3 0,-2 5 22,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,-1-1 0,-26 0-399,15 2-479,6 2-996,2 0-3141</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="311.14">298 5 5298,'0'0'5696,"0"17"-5914,-6 196 5919,6-212-5648</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="587.86">414 139 5186,'0'0'9434,"0"28"-8468,-10 5 277,0-1-1968,9-14-6892</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="587.85">414 139 5186,'0'0'9434,"0"28"-8468,-10 5 277,0-1-1968,9-14-6892</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="746.65">451 0 9428,'0'0'4274,"0"34"-12966</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1286.87">445 175 4834,'0'0'12086,"4"-2"-11822,-2 1-222,0-1 0,0 1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,1 0 1,2 0 0,-4 0-35,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,0 0-1,0 0 1,0-1 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,1 1 0,-1-1-1,0 0 1,-1 0 0,1 2 0,0 45 876,12-78-659,10-4-666,-21 33 410,0 0-1,-1 0 1,1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,1 1 0,-1-1-1,0 1 1,0-1 0,1 1 0,-1-1-1,0 1 1,1 0 0,-1 0-1,3 0 1,-2 4 32,-1 0 1,0 0-1,0 0 0,-1 1 0,1-1 0,-1 1 1,0-1-1,0 0 0,0 1 0,-2 5 0,2 0 233,0-8-210,-1 0 1,1 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 0 1,1 0-1,-1 0 0,1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,2 2-1,-2-4-171,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1-1,0-1 1,-1 0 0,1 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 1 0,1-3 0,9-8-4441</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1286.86">445 175 4834,'0'0'12086,"4"-2"-11822,-2 1-222,0-1 0,0 1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,1 0 1,2 0 0,-4 0-35,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,0 0-1,0 0 1,0-1 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,1 1 0,-1-1-1,0 0 1,-1 0 0,1 2 0,0 45 876,12-78-659,10-4-666,-21 33 410,0 0-1,-1 0 1,1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,1 1 0,-1-1-1,0 1 1,0-1 0,1 1 0,-1-1-1,0 1 1,1 0 0,-1 0-1,3 0 1,-2 4 32,-1 0 1,0 0-1,0 0 0,-1 1 0,1-1 0,-1 1 1,0-1-1,0 0 0,0 1 0,-2 5 0,2 0 233,0-8-210,-1 0 1,1 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 0 1,1 0-1,-1 0 0,1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,2 2-1,-2-4-171,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1-1,0-1 1,-1 0 0,1 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 1 0,1-3 0,9-8-4441</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2260.8">742 172 6643,'0'0'9095,"-6"-2"-8428,0 0-618,1 1 1,0 0-1,0 0 0,0 0 1,-1 1-1,1 0 1,0 0-1,-1 0 0,-7 2 1,11-1-48,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 1 1,1-1-1,-1 0 1,1 1-1,-1 0 1,1-1-1,0 1 0,0 0 1,0-1-1,0 1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,0 1-1,0-1 0,0 3 1,0-4-3,1 0-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0-1,-1-1 1,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 1-1,1-1 1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0-1,4-1 71,1 0 0,-1 0 0,0-1 0,1 0 0,7-5 0,-6 2-109,-1 1-1,0-1 0,-1-1 0,1 1 1,-1-1-1,0-1 0,-1 1 1,0-1-1,0 0 0,-1 0 1,6-12-1,-6 7 69,0-1 1,-1 0 0,0 0-1,-1 0 1,0 0-1,-1-23 1,-2 43-67,0 1 1,-1 0-1,0-1 1,0 1-1,0-1 1,-5 8-1,-5 21 85,11-35-45,-2 12 57,1-1 0,0 0 0,1 1-1,-1 20 1,2-31-60,0 1 0,0 0 0,1 0-1,-1 0 1,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1-1,0 1 1,0-1 0,0 1 0,0 0 0,0-1 0,0 0-1,0 1 1,0-1 0,1 0 0,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,0-1 0,-1 1-1,1 0 1,0-1 0,0 1 0,-1-1 0,1 0 0,0 0-1,0 1 1,0-1 0,2-1 0,-2 1 27,1 0 0,-1 0 0,1-1 0,0 0 0,-1 1 0,0-1 0,1 0-1,-1 0 1,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,2-4 0,-1 2-19,0 0 0,0-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,0 1 1,-1-1-1,1 1 0,-1-1 0,0 1 0,-1-1 0,0-5 0,1 10-6,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 1 1,-1-1 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,-22 21-11,19-15 19,0 0 0,0 0 0,1 1 0,0 0 0,0-1 0,1 1 0,0 0 0,1 0 0,0 1 0,0-1 0,0 12 0,1-20-44,0 1 0,0-1 0,0 1 0,1-1-1,-1 1 1,0-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,2 0 0,20 1-3608,-14-2 1492,15 1-2644</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2447.3">1050 81 11253,'0'0'6931,"-65"75"-6787,53-53-112,3-3-32,3-1-16,1-3-816,-1-5-1713,3-3-1281</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2630.72">928 113 7812,'0'0'9492,"35"40"-9380,-14-18 64,-1 0-64,1-2-96,5 0-16,1-1-352,-4-4-2625,-5-5-4259</inkml:trace>
@@ -11146,7 +11146,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5830.86">2552 811 272,'0'0'14289,"-4"2"-12429,-2 2 175,13-4-691,30-5-312,51-15-2698,-75 14-3539,-10 2 976</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6205.33">2565 626 7075,'0'0'11413,"-4"-1"-10999,-11 0-407,11 5-2,21 14 6,40 18 91,-26-22-62,-22-11-30,1 1 1,-1 0 0,-1 0 0,10 7-1,-16-10-9,0 1 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 1 1,0-1 0,0 0-1,0 1 1,-1-1-1,1 1 1,-1-1 0,1 1-1,-1 4 1,0 0 75,-1 0-1,1-1 1,-1 1 0,-1 0 0,0-1-1,1 1 1,-2-1 0,1 0-1,-1 0 1,0 1 0,-4 4-1,-5 7 449,0-1 1,-18 18-1,16-21-686,1 2 0,-19 29 1,26-41-5226</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7031.24">2999 670 4594,'0'0'13772,"0"-4"-12892,-8 15-50,-10 33-476,8-16-68,-13 50 0,22-73-271,0 0 1,1 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,1 0 0,0-1 0,2 10 0,-2-12-13,0-1 0,0 1 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1-1 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 1,0 1-1,0-1 0,0 0 1,1 0-1,-1 0 0,0 0 1,4 0-1,0 0 34,0 0 0,1-1 0,-1 0 0,0 0 1,0 0-1,0 0 0,10-4 0,5-13-2273,-20 16 1529,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,1 0-1,-1 0 1,1-1-1,-1 1 1,0-5-1,0-5-6716</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7229.47">2959 784 6931,'0'0'8788,"47"-22"-8628,-26 15-64,-1 0-96,-2 2-176,-6-2-1489,0 0-1424,-7 0-1681</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7229.46">2959 784 6931,'0'0'8788,"47"-22"-8628,-26 15-64,-1 0-96,-2 2-176,-6-2-1489,0 0-1424,-7 0-1681</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7463.19">2992 627 4882,'0'0'12310,"14"-25"-12134,10 21-48,-1 3-64,-2-1-64,-3 2 0,-7 0-32,-2 0-576,-3 0-1121,3 10-896,-3 2-161,0 4-3104</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7744.85">3383 732 9620,'0'0'9725,"-12"2"-9445,5-1-229,1 1 0,-1-1 0,1 2-1,-1-1 1,1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,1 0-1,-1 0 1,1 0 0,0 1 0,1 0 0,-8 9 0,6-7-92,-39 56 902,43-60-1089,0 1 0,0 0 1,0 0-1,1 0 0,0 1 1,0-1-1,0 0 0,0 0 1,0 6-1,16-7-16257</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7945.15">3256 749 10165,'0'0'9188,"41"40"-8580,-29-22-368,0 3-112,-3-1-96,-1-2-32,1-3 0,0-3-800,0 0-1713,3-5-2626,2-4-4913</inkml:trace>
@@ -11182,14 +11182,14 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">58 169 4562,'0'0'9180,"-16"-41"-856,13 93-8295,-2-1-1,-16 65 0,9-51 7,12-64-34,0 18 63,20-20-6,1-4 26,-1 0 0,0-2 0,36-17 0,-62 23-7391</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="637.09">213 251 5523,'0'0'9447,"0"0"-9158,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-2 0 0,0 2-281,-1 1 0,1 0 1,0 0-1,0 0 0,0 1 0,0-1 0,1 0 1,-1 1-1,0-1 0,1 1 0,0-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 0,0 6 1,-2 53 137,3-50-139,0-11-4,0 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0-1 1,-1 1-1,1-1 1,0 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,-1-1 1,2 0-1,39-19 125,-39 19-139,0-1-1,0 1 1,-1 0 0,1-1 0,0 0 0,-1 1-1,1-1 1,-1 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,-1-1 1,1 1 0,-1 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,0-1 0,-1 1 0,1 0-1,0 0 1,-1-1 0,0 1 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 1 0,-1-1-1,0 0 1,1 1 0,-1 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,0 1 0,-1-1-1,1 1 1,0 0 0,0 0 0,-1 0 0,-3 1-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1069.91">335 259 1745,'-1'1'15410,"-6"32"-13887,5-28-1427,0 1 0,1 0 0,-1-1 0,2 1 0,-1 0 0,0 0 0,1-1 0,0 1 0,2 10 0,-2-15-94,1-1-1,-1 1 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1-1 1,-1 1-1,1 0 0,0-1 1,0 1-1,-1-1 0,1 1 1,0-1-1,0 0 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1-1 0,0 1 0,0 0 1,0 0-1,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 1,-1 1-1,2-1 0,30-21-256,-31 21 190,1-1 0,-1 0 0,0 1 1,1-1-1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,0 0 0,1-4 0,-1 5 161,-1 0-1,1 0 0,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,-2 0 1,-36-10-3168,13 9-7680,33 2 4176</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1367.19">469 134 7251,'0'0'9538,"-8"10"-8751,3 9-376,1 0 1,1 0-1,1 1 0,1 0 0,0-1 0,3 23 1,-1-6 1,-1 20-850,12-63-14760</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1367.18">469 134 7251,'0'0'9538,"-8"10"-8751,3 9-376,1 0 1,1 0-1,1 1 0,1 0 0,0-1 0,3 23 1,-1-6 1,-1 20-850,12-63-14760</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2739.73">444 286 10293,'0'0'5989,"9"-7"-5853,-4 3-101,-1 1 2,-1 0 0,1 0 1,0 0-1,0 0 0,1 1 1,-1-1-1,0 1 1,1 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 1,0 1-1,6 1 1,-10 0-23,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 2 0,-7 32 476,2-27-447,0 0 0,-1-1 0,0 0 1,-1 0-1,1-1 0,-11 8 1,13-10-18,-1-1 0,1 1 0,-1-1 1,0 0-1,0-1 0,0 1 0,0-1 1,0 0-1,0 0 0,-1-1 1,-10 2-1,15-4-33,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 1-1,1-1 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1 0 0,1 0 1,0-1-1,0 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,-1 0-1,3-2 0,2 2 10,0 1 0,0-1 0,0 1 1,1 0-1,-1 0 0,0 0 0,0 1 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,0 0 0,-1 1 0,9 4 0,34 14 606,-44-20-592,-1-1 0,1 0 0,0 1 0,0-1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,2-4 0,1-3-30,0-1 1,0 1-1,-1-1 1,-1 0 0,0 0-1,0 0 1,0-13-1,-2 24 86,0 28-355,0-22 284,0 0 0,0 0 0,1 1 0,0-2 0,0 1 0,4 9 0,-5-14-2,0 0 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1-1 1,0 1 0,-1 0 0,1 0-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,-1 1 0,1-1-1,0 0 1,0 1 0,1-1 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,-1 0-1,2-1 1,2-1 3,0 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,-1 1 1,1-1-1,-1 1 0,0-1 0,0 1 0,-1-1 0,1-5 0,-1 9 12,34 22-316,-31-19 294,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,1-1 0,-1 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0-1 0,0 1 0,0-1-1,-1 0 1,1 1 0,0-1-1,-1 0 1,0 0 0,1-1-1,-1 1 1,0 0 0,0-1-1,0 0 1,0 1 0,-1-1-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0-4-1,3-4-8,-1-1 0,0 0 0,-1 1-1,-1-1 1,0 0 0,0 0 0,-1 0-1,-1 0 1,-3-20 0,6 51-22,-2 1 1,-2 29-1,0 6 153,2 169 770,0-223-812,0-26 358,-1 1-421,1 3-102,0-1-1,5-28 1,-5 45 18,1-1-1,1 1 1,-1-1-1,1 1 1,0 0 0,0 0-1,0 0 1,1 0-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 1-1,5-4 1,-6 7 40,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 1-1,0-1 1,0 0 0,0 1-1,-1-1 1,1 1 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,2 1 0,-3 0 20,0-1 1,0 1 0,1 0-1,-1 0 1,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 1-1,-1-1 1,1 0 0,-1 1-1,1-1 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0-1-1,0 0 1,0 3-1,-1 1 64,0 1-1,0 0 1,0 0-1,-1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,-1 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,-1-1 1,0 0-1,0 1 1,-1-2-1,1 1 0,-1 0 1,0-1-1,0 0 0,0 0 1,0 0-1,-1-1 0,1 0 1,-1 0-1,1 0 0,-1-1 1,-8 2-1,13-3-149,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 0 0,0-1-955,0-12-5480</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3561.84">1189 162 5234,'0'0'10392,"-3"-2"-9648,1 1-678,1 0 0,0 1-1,-1-1 1,1 0 0,-1 1 0,1-1 0,-1 1-1,1-1 1,-1 1 0,1 0 0,-1-1-1,1 1 1,-1 0 0,0 0 0,1 0-1,-1 1 1,1-1 0,-1 0 0,-3 1 0,3 1-25,0-1 1,0 0 0,0 1 0,1-1 0,-1 1 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,-1 4 0,-14 42 230,15-45-258,1-1 0,-1 1 0,0 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,0 0 0,-1 0-1,3 5 1,-2-7-39,0 0-1,1-1 0,-1 1 0,0 0 1,1 0-1,-1-1 0,0 1 0,1 0 1,-1-1-1,1 0 0,-1 1 0,1-1 1,-1 0-1,1 0 0,-1 1 0,1-1 1,-1 0-1,1-1 0,-1 1 0,1 0 1,-1 0-1,3-1 0,31-11-1046,-30 8 692,0 0 1,1 0-1,-2 0 1,1 0-1,0-1 1,-1 0-1,0 0 1,0 0 0,6-11-1,-3-15 3355,-19 46-2126,11-11-775,1-1 1,-1 1-1,1 0 1,0-1 0,0 1-1,0 0 1,0-1-1,1 1 1,1 5-1,-2-8-66,0-1 0,0 1 0,0 0 0,1-1 0,-1 1-1,0 0 1,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0-1,1 0 1,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,0-1 0,0 2-2,0-1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 1-1,0-1 1,0-1 0,0 1 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1-1 1,1 1 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1-1 0,0 1-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0-1,-1-1 1,1 1 0,0-1 0,-1 1-1,0-2 1,-1 1 0,1 1 0,-1-1-1,1 0 1,-1 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,-1-1 0,1 1 0,0-1-1,0 1 1,-1 0 0,-1 0 0,-3 0-415,-10 1 533,12 6-6941</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3902.04">1383 0 9316,'0'0'6822,"-9"51"-4866,5-6-713,4 62 0,1-48-672,-1-59-581,0 1 1,0 0-1,0-1 0,0 1 0,0 0 1,1-1-1,-1 1 0,0 0 1,0-1-1,1 1 0,-1-1 0,0 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,0-1 0,1 1 0,-1-1 1,1 1-1,-1-1 0,1 0 1,0 1-1,-1-1 0,1 0 0,-1 1 1,1-1-1,0 0 0,-1 0 1,1 0-1,0 0 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1-1 0,0 1 0,-1 0 1,2 0-1,15-9-4744,-10-1-2495</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4292.29">1446 134 7075,'0'0'8604,"0"6"-7318,0 107 3692,0-112-4972,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1-1,1-1 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1 0 0,-1-1-1,1 1 1,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1-1 1,2 1 0,20-8 117,-19 4-100,0 0 1,0 0 0,0 0-1,0 0 1,-1-1 0,0 1-1,0-1 1,0 0 0,2-6-1,-4 9-10,1 1-1,0-1 0,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 1 0,-1-1 0,1 1 1,-1-1-1,0 1 0,0-1 0,0 1 0,1 0 1,-1-1-1,0 1 0,-1 0 0,1 0 0,0 0 1,-2-2-1,-7 5-2627,7 14-5545,3-16 7916,0 12-8800</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4415.97">1446 134 976</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4415.96">1446 134 976</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4868.01">1446 134 976,'78'38'7657,"-54"-31"-864,-12-8-4570,-11 1-2193,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 2 0,1-1 20,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,2 1 0,-2-1-61,1-1 1,-1 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,-1 0 0,1-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1-1-1,-1 1 1,1-2 0,9-19-39,-3 20 48,-1 30 115,-6-25-91,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0-1-1,3 6 1,-4-8 13,3-2-49,-1 1-1,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 1,-1 0-1,2-5 0,-2 4 1,0 1-1,0-1 1,1 0 0,-1 1-1,1-1 1,-1 1 0,1 0 0,0-1-1,0 1 1,0 0 0,4-2 0,-6 4 15,1-1 1,-1 1-1,0 0 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,-1 0-1,0 1 1,1-1-1,-1 0 1,1 0-1,-1 1 1,0-1-1,1 0 0,-1 1 1,0-1-1,9 20 171,-5 22 17,-4-41-17,2 7-1969,6-6-6818,1-2-754</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5182.97">1795 143 7716,'0'0'8409,"2"5"-7366,0 1-1005,13 24 1790,-14-29-1799,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 0,0 0 1,0 1-1,0-1 0,-1 0 1,1 1-1,0-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1-1-1,0 1 1,0 0-1,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 1,-1-1-1,1 1 1,0-1-1,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,0 0 1,2-1-1,25-33 42,-22 27-64,1 0-1,0 0 1,0 0 0,1 1 0,-1 0 0,2 1-1,7-7 1,-14 14 8,0-1 0,-1 0 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1 0 0,0-1-1,1 1 1,-1-1 0,0 1 0,0 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 1 0,5 29 646,-4-25-540,-1-3-85,1 0 1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,3 4 0,-4-5-117,0-1-1,-1 1 1,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1-1 0,9-13-5291</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5182.96">1795 143 7716,'0'0'8409,"2"5"-7366,0 1-1005,13 24 1790,-14-29-1799,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 0,0 0 1,0 1-1,0-1 0,-1 0 1,1 1-1,0-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1-1-1,0 1 1,0 0-1,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 1,-1-1-1,1 1 1,0-1-1,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,0 0 1,2-1-1,25-33 42,-22 27-64,1 0-1,0 0 1,0 0 0,1 1 0,-1 0 0,2 1-1,7-7 1,-14 14 8,0-1 0,-1 0 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1 0 0,0-1-1,1 1 1,-1-1 0,0 1 0,0 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 1 0,5 29 646,-4-25-540,-1-3-85,1 0 1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,3 4 0,-4-5-117,0-1-1,-1 1 1,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1-1 0,9-13-5291</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -11283,8 +11283,8 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">24 569 1985,'0'0'9572,"0"5"-9876,0 4-896,0 10-1057,-4 0-721,-4 2-1120</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1354.41">0 742 512,'0'0'5043,"3"-38"292,3 3-4686,-1 0 0,-2 0 0,-3-63 0,-1 48-145,1 50-135,33 0-812,300 7 531,-233-10-359,0-4-1,123-26 1,88-16 207,-310 49 62,0 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,-1-1 0,1 1 1,0 0-1,0 0 0,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0 0 0,-1-1 0,1 1 0,0-1 1,-1 1-1,1-1 0,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-15-10-109,-44-6-83,51 15 191,-13-5 67,14 5-14,0 0 0,0 0 1,-1 0-1,1 1 0,0 0 0,-10-1 1,15 2-158,4 1-376,1-1 458,-1 1 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 1 1,3 1-1,11 4 10,7-3 36,-20-4-83,0 0-1,0 0 1,0 1 0,0 0-1,-1 0 1,1 0 0,0 0-1,4 2 1,-7-2 48,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 1 1,0-1 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0 0,-2 1-1,-2 5 55,-1 0 1,0 0-1,0 0 0,-1 0 1,-11 9-1,12-11-16,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 0,1 1 1,0-1-1,-4 10 0,8-7-1811,0-6-1331</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1862.18">1259 211 3009,'0'0'7476,"0"-4"-6775,4 185 967,-4-180-817,37-2-333,-1-4-297,-4 0-2427,-10 4-4491,-17 1 4032,-1-2 253</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2296.22">1477 303 1313,'0'0'7019,"1"0"-6972,-1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 0,0 0 0,0-1 1,-1 1-1,1-1 0,0 1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,-2 4 93,1 0 0,0 0 0,0 0 0,0 0-1,0 1 1,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0 6 0,-2 49 1347,3-53-1333,4-5-99,1 0 0,-1-1 0,1 1 0,-1-1-1,1 0 1,-1 0 0,1-1 0,-1 1 0,1-1-1,7-2 1,-10 1-55,1 0-1,-1 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,0-1-1,0 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,-1 0-1,1-1 0,0 1 1,-1 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-2-7 1,2 9-27,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,-2 0 0,-35-1-3889,28 1-1156</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1862.17">1259 211 3009,'0'0'7476,"0"-4"-6775,4 185 967,-4-180-817,37-2-333,-1-4-297,-4 0-2427,-10 4-4491,-17 1 4032,-1-2 253</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2296.21">1477 303 1313,'0'0'7019,"1"0"-6972,-1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 0,0 0 0,0-1 1,-1 1-1,1-1 0,0 1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,-2 4 93,1 0 0,0 0 0,0 0 0,0 0-1,0 1 1,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0 6 0,-2 49 1347,3-53-1333,4-5-99,1 0 0,-1-1 0,1 1 0,-1-1-1,1 0 1,-1 0 0,1-1 0,-1 1 0,1-1-1,7-2 1,-10 1-55,1 0-1,-1 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,0-1-1,0 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,-1 0-1,1-1 0,0 1 1,-1 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-2-7 1,2 9-27,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,-2 0 0,-35-1-3889,28 1-1156</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2686.78">1612 299 2545,'0'0'5259,"-3"6"-4339,0 3-639,-1-1 1,1 1-1,0 0 1,0 1-1,1-1 1,1 0-1,-1 16 1,2-25-271,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,1-1 0,27-9 157,-25 6-142,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 0-1,2-6 1,-3 9 6,-1-1 1,0 1-1,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 1,-1 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 1,-1 1-1,0 0 0,1 0 1,-3-4-1,2 5-78,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1-1 0,-4 2 0,-14 0-5801</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2827.95">1612 286 3121</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2965.2">1612 286 3121,'72'-77'2620,"-72"77"-2505,0 0-1,0-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,1-1 0,-1 1 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 1 0,0-1 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,5 22 2027,-4 37-2280,-2-48 910,1-4-759,0 1 1,1-1 0,0 1 0,0-1 0,0 0 0,4 10 0,-4-15-212,-1-1 0,1 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,0 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,0 0-1,1 0 1,1 1 0,-1-1-225,-1 0-1,1-1 1,0 1 0,-1-1-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,1 0 0,-1-1-1,3 0 1,8-7-2481</inkml:trace>
@@ -11321,16 +11321,16 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1966 443 5090,'0'0'10322,"0"-13"-9001,2 53-1113,-1-27-425,0-1-1,0 1 1,-2 0-1,1 0 1,-5 17-1,-2-23-7153</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-3558.62">0 22 4466,'0'0'6259,"18"0"-4805,43-10 718,-38 6-1434,0 1 0,24-1 0,-46 4-287,-27 19-10149,11-10 3388</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-3402.75">0 9 3009</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2720.37">0 9 3009,'55'44'2439,"-55"-43"-2305,0-1-1,1 0 1,-1 1 0,0-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,1 0-1,-1 1 1,0-1 0,1 0 0,-1 0-1,1 0 1,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0 2 1299,0 6-1502,3 46 556,-3 89 1,-3-63 503,-6 45 828,19-126-1525,78-17-125,-52 9-167,51-5 0,105 11-20,-128 3-543,-67-1 515,-1 1-1,0-1 1,0 0 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,1 0 1,0 1-1,0-1 1,-3-3 0,2 3 63,0-1 1,1 1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-6-1-1,14 7-11,0 1-1,0 0 0,0 0 0,0 0 0,-1 0 0,0 1 0,4 8 0,8 25-123,-16-37 95,0-1 1,1 0-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 0 1,0 1-1,0-1 1,-1 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,0 1 1,1-1 0,-1 0-1,-2 1 1,-6 5-111,0 0 0,0-1 1,-19 9-1,4-6-4291</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2050.39">694 361 3378,'0'0'7088,"-4"-3"-6722,2 2-335,0 0 1,1 1 0,-1-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,1 1-1,-4 2 1,0 1 130,0 0-1,1 0 1,0 0 0,0 0-1,0 1 1,1 0-1,-1-1 1,-3 9 0,4-7-50,0 0 0,0 0 0,1 1 0,0-1 0,0 1 1,1 0-1,-1 0 0,2-1 0,-1 1 0,1 0 0,0 11 0,0-16-167,0 0 0,1 1 0,-1-1 0,0 0-1,1 1 1,0-1 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1-1 0,0 1-1,1-1 1,-1 1 0,5-1 0,2 0-823,1 0 1,-1-1 0,0 0 0,0 0-1,0-1 1,0 0 0,0-1-1,0 0 1,0 0 0,13-8 0,-18 9 705,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0-1 0,0 0 0,4-7 0,3-16 2804,-7-7 3362,-7 62-5355,-1 12-242,5-39-393,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 1,1-1-1,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,1 0-1,2 0-36,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0-1-1,-1 1 0,6-4 0,-7 4 15,-1-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,0-4-1,0 4 16,1 0 0,-1 0-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,0 0 0,0 0 0,0-1-1,0 1 1,0 1 0,1-1-1,-1 0 1,-3 1 0,1-1-65,-1 1 0,1-1 0,0 1 1,-1 0-1,1 0 0,0 0 0,0 1 0,0-1 0,0 1 1,0 0-1,0 0 0,0 1 0,-4 3 0,0 5-2491,3 1-1391</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2720.38">0 9 3009,'55'44'2439,"-55"-43"-2305,0-1-1,1 0 1,-1 1 0,0-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,1 0-1,-1 1 1,0-1 0,1 0 0,-1 0-1,1 0 1,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0 2 1299,0 6-1502,3 46 556,-3 89 1,-3-63 503,-6 45 828,19-126-1525,78-17-125,-52 9-167,51-5 0,105 11-20,-128 3-543,-67-1 515,-1 1-1,0-1 1,0 0 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,1 0 1,0 1-1,0-1 1,-3-3 0,2 3 63,0-1 1,1 1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-6-1-1,14 7-11,0 1-1,0 0 0,0 0 0,0 0 0,-1 0 0,0 1 0,4 8 0,8 25-123,-16-37 95,0-1 1,1 0-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 0 1,0 1-1,0-1 1,-1 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,0 1 1,1-1 0,-1 0-1,-2 1 1,-6 5-111,0 0 0,0-1 1,-19 9-1,4-6-4291</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2050.4">694 361 3378,'0'0'7088,"-4"-3"-6722,2 2-335,0 0 1,1 1 0,-1-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,1 1-1,-4 2 1,0 1 130,0 0-1,1 0 1,0 0 0,0 0-1,0 1 1,1 0-1,-1-1 1,-3 9 0,4-7-50,0 0 0,0 0 0,1 1 0,0-1 0,0 1 1,1 0-1,-1 0 0,2-1 0,-1 1 0,1 0 0,0 11 0,0-16-167,0 0 0,1 1 0,-1-1 0,0 0-1,1 1 1,0-1 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1-1 0,0 1-1,1-1 1,-1 1 0,5-1 0,2 0-823,1 0 1,-1-1 0,0 0 0,0 0-1,0-1 1,0 0 0,0-1-1,0 0 1,0 0 0,13-8 0,-18 9 705,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0-1 0,0 0 0,4-7 0,3-16 2804,-7-7 3362,-7 62-5355,-1 12-242,5-39-393,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 1,1-1-1,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,1 0-1,2 0-36,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0-1-1,-1 1 0,6-4 0,-7 4 15,-1-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,0-4-1,0 4 16,1 0 0,-1 0-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,0 0 0,0 0 0,0-1-1,0 1 1,0 1 0,1-1-1,-1 0 1,-3 1 0,1-1-65,-1 1 0,1-1 0,0 1 1,-1 0-1,1 0 0,0 0 0,0 1 0,0-1 0,0 1 1,0 0-1,0 0 0,0 1 0,-4 3 0,0 5-2491,3 1-1391</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1682.45">961 274 5955,'0'0'5424,"-1"84"-3424,-7 171 396,8-254-2429,0 0 1,0 0-1,0-1 0,1 1 0,-1 0 1,0 0-1,0-1 0,0 1 0,1 0 0,-1-1 1,0 1-1,1 0 0,-1-1 0,0 1 0,1 0 1,-1-1-1,1 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 0,0 0 1,1 1-1,13 1-5221,-7-2-282</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1298.4">1034 500 5298,'0'0'5902,"0"17"-4944,0 55 520,0-71-1468,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 1-1,0-1 1,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0-1,2 0 1,-1 0 30,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1-2 0,2-7-9,-2 0-1,1 0 1,-1 0-1,-1 0 1,0 0-1,0 0 1,-1 0-1,-1-14 1,0-2-255,1 25-416,0 9-5456,0-6 5098,0 14-3322</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1298.41">1034 500 5298,'0'0'5902,"0"17"-4944,0 55 520,0-71-1468,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 1-1,0-1 1,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0-1,2 0 1,-1 0 30,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1-2 0,2-7-9,-2 0-1,1 0 1,-1 0-1,-1 0 1,0 0-1,0 0 1,-1 0-1,-1-14 1,0-2-255,1 25-416,0 9-5456,0-6 5098,0 14-3322</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-677.98">1186 445 2177,'0'0'7603,"1"1"-7500,0 0 0,0 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,0 1 0,0-1 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 1 0,0 2 0,8 68 1999,-9-73-2084,0 1 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,7-10 113,-5 5-75,19-41-537,-20 43 406,0 1 1,1-1-1,-1 0 0,1 1 1,-1 0-1,1-1 0,0 1 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,5-2 1,-7 4 62,1 0 1,-1 0-1,1 0 1,0-1-1,-1 1 1,1 0-1,-1 0 1,1 1-1,-1-1 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 1 1,-1-1-1,0 0 1,1 1-1,-1-1 1,1 1 0,-1-1-1,0 1 1,0-1-1,1 1 1,6 25-60,-4 35 365,-4-53-204,1-7 112,2-3-162,0 1 0,0-1 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1-3 1,3-5-34,6-9-92,-8 12 24,1 1 1,0 0-1,0-1 1,0 2 0,0-1-1,1 1 1,0-1 0,11-8-1,-16 14 58,1 0-1,-1 0 0,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 0 1,1 1-1,-1-1 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 1 1,1-1-1,-1 0 1,0 0-1,0 1 1,0-1-1,1 1 0,4 16 50,-4 27 88,-1-39-163,0 7-159,0 9-823,0-7-3929</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-278.9">1502 447 3890,'0'0'6613,"2"5"-5660,0 6-386,-2-4-301,1 0 1,1 1-1,-1-1 0,1 0 0,0 0 1,1 0-1,6 13 0,-8-20-178,1 0-49,0 0 0,-1 0-1,1-1 1,0 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,0 0 0,2-3 0,23-37 51,1-2-73,-26 42-86,2 4 114,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 1 1,-1-1 0,0 1 0,2 4-1,22 28 5,-17-26-3978,-5-1-191</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="154.95">2002 237 8580,'0'0'2289</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="545.79">2064 402 7571,'0'0'4944,"1"15"-3610,6 145 1894,-4-160-3218,0-1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,0-1 1,1 1 0,-1-1 0,4-3 0,20-26-67,-22 24 75,1 0-1,1 1 0,-1 0 0,1 0 0,0 0 0,8-5 1,-13 10 315,1 4-325,-1 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 1 0,0 2 1,-1-3-69,1 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,0 0 0,1 0-1,3 3 1,0-3-695,0 0 0,-1-1 0,1 0 0,0 0 0,0-1 0,0 1 0,0-1-1,0-1 1,0 1 0,8-2 0,14-6-3770</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1129.98">2392 464 496,'0'0'13847,"-2"-10"-12634,-7-29-508,9 39-695,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 1-1,0-1 0,0 0 1,-10 10 250,-3 12 24,8 3-224,39-27 169,-26-1-262,-1 0 0,0-1-1,0 0 1,-1 0 0,1 0 0,-1-1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0-1,0 0 1,-1-1 0,1 1 0,-1-1 0,-1 0 0,1 0 0,-1-1 0,-1 1 0,3-11 0,3-7 5,-2-1 0,-1 0 1,2-37-1,-6 56 221,-5 40-120,2-21-46,0 0 0,1 0 0,0 0 0,1-1 0,0 1 0,4 20 0,-3-29-17,0 0 1,1 0-1,-1 0 0,0 0 1,1-1-1,0 1 0,-1 0 1,1-1-1,0 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1-1 0,0 1 1,-1-1-1,1 0 0,0 1 1,0-1-1,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 0-1,0 0 0,1 0 1,2-1-1,1 1 24,0 0 0,0 0 1,-1-1-1,1 0 0,0 0 0,-1-1 0,1 0 0,-1 0 1,1 0-1,-1-1 0,7-4 0,-10 5 1,0 0 0,0-1 0,0 1 0,-1-1-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,-1 0 0,1 0 0,0-1-1,-1 1 1,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,0 0-1,0-6 1,1 9-9,-1 0-1,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,-1 0 0,1 1 0,0-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,-1-1-1,1 1 0,0-1 0,-1 1 1,1 0-1,-1-1 0,1 1 1,0-1-1,-1 1 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,0-1-1,1 1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 1,-1-1-1,0 0 0,1 0 1,-1 0-1,1 0 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,1 1 0,-1-1 0,1 0 1,0 1-1,-1-1 0,1 1 1,-30 28 0,25-21-54,1-1 0,1 1 0,-1 0 0,1 0-1,1 0 1,-1 0 0,1 0 0,1 1 0,0-1 0,0 1 0,0 14 0,1-22-37,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0-1 1,0 1 0,0 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,1 1 1,46 0-2589,-38-2 1729,-3 1 77,0-1-1,1 0 1,-1 0-1,0 0 0,0-1 1,0 0-1,0-1 0,12-5 1,14-12-3967</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1289.1">2893 306 3169,'0'0'13879,"-12"-7"-13767,-1 28 416,1 2-352,4-2-96,-5 3-64,9 2-16,-4-8-800,4 1-1009,4-9-2753</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1289.09">2893 306 3169,'0'0'13879,"-12"-7"-13767,-1 28 416,1 2-352,4-2-96,-5 3-64,9 2-16,-4-8-800,4 1-1009,4-9-2753</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1485.6">2844 271 8148,'0'0'7779,"107"84"-7363,-78-46-191,4 4-113,-1-2-112,-3-8-385,-4-3 209,-9-11-2305,-4-4-1425</inkml:trace>
 </inkml:ink>
 </file>
@@ -11369,7 +11369,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3454.12">1699 678 2145,'0'0'7694,"-24"63"-4786,16-29-1598,8-33-806,0-8 43,1-7-709,0-1 0,2 1 0,0-1 1,0 1-1,1 0 0,1 0 0,0 0 0,8-13 0,-11 23 125,4 1-395,-1 12 306,1 11 159,-3 4 193,0 0 0,-2 1 0,-3 32 0,1-8-487,-1-17-1720,-1-23-3580,0-9 1692</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3611.75">1663 798 3650,'0'0'8019,"24"-18"-8051,-7 18-624,-1 0-833,-4 0-2144,1 0-929</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3913.82">1663 785 1889,'94'-53'4989,"-93"53"-4864,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 0,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 3 0,15 37 498,-12-1 932,-3-40-1501,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-4-22 736,3 18-890,0-1 0,1 1 0,0 0 0,-1 0 0,2 0 0,-1 0 0,0 0-1,1 0 1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,3-5 1,-3 6-464,1 0 0,0 1 0,-1-1-1,1 1 1,0-1 0,1 1 0,-1 0-1,0 0 1,1 0 0,6-2 0,3-1-4393</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4729.94">1879 721 2801,'0'0'7118,"4"3"-6742,-2-2-303,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 4 0,2 42 1878,-3-38-1477,0-10-438,0 0-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-4-12 429,4 10-639,0-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,1 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,0 0-1,-1 1 1,1-1 0,0 0-1,0 1 1,0 0-1,3-2 1,7-4-1399,0 2 0,0 0 1,16-5-1,15-10 4812,-44 19-3152,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1-1,0 0 1,-1 0 0,1-1 0,0 1 0,0 0 0,-1 1 0,1-1 0,0 0-1,-1 0 1,1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,-1 2 0,0 0-21,0 0-1,1 1 0,-1-1 1,1 0-1,0 1 0,0-1 1,0 1-1,0 0 0,0-1 1,1 1-1,-1 0 0,0 3 1,1-5-64,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,1 1 0,-1 0-1,0 0 1,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1-1 0,0 0 0,0 1-1,-1-1 1,1 1 0,0-1-1,0 0 1,0 0 0,-1 1 0,1-1-1,2 0 1,-1 0-78,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1-1 1,0 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,1-1 0,-2-1 64,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0-4 0,46 8-141,-44 0 192,1-1 0,-1 0 0,1 0-1,-1 0 1,1-1 0,-1 1 0,1 0 0,-1-1-1,0 0 1,1 0 0,-1 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,0-4 0,-1 6 509,3 11-268,-2-1-237,4 22 158,-1 0 0,-2 1 0,-2 0 0,-5 50-1,4-80-111,0 1-1,-1-1 0,0 1 1,1-1-1,-1 1 0,-1-1 1,1 0-1,0 0 0,-1 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,-1 1 0,1-1 1,0 0-1,0 0 0,-1-1 1,0 1-1,1-1 1,-1 1-1,0-1 0,1 0 1,-1-1-1,0 1 0,0-1 1,0 1-1,0-1 0,1 0 1,-1-1-1,0 1 0,0-1 1,0 0-1,-4-1 0,6 1-347,0-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,0 0 1,-1 1-1,1-1 0,0 0 0,0 0 1,0 0-1,-2-4 0,2 3-281,-8-20-3436</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4729.93">1879 721 2801,'0'0'7118,"4"3"-6742,-2-2-303,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 4 0,2 42 1878,-3-38-1477,0-10-438,0 0-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-4-12 429,4 10-639,0-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,1 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,0 0-1,-1 1 1,1-1 0,0 0-1,0 1 1,0 0-1,3-2 1,7-4-1399,0 2 0,0 0 1,16-5-1,15-10 4812,-44 19-3152,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1-1,0 0 1,-1 0 0,1-1 0,0 1 0,0 0 0,-1 1 0,1-1 0,0 0-1,-1 0 1,1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,-1 2 0,0 0-21,0 0-1,1 1 0,-1-1 1,1 0-1,0 1 0,0-1 1,0 1-1,0 0 0,0-1 1,1 1-1,-1 0 0,0 3 1,1-5-64,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,1 1 0,-1 0-1,0 0 1,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1-1 0,0 0 0,0 1-1,-1-1 1,1 1 0,0-1-1,0 0 1,0 0 0,-1 1 0,1-1-1,2 0 1,-1 0-78,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1-1 1,0 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,1-1 0,-2-1 64,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0-4 0,46 8-141,-44 0 192,1-1 0,-1 0 0,1 0-1,-1 0 1,1-1 0,-1 1 0,1 0 0,-1-1-1,0 0 1,1 0 0,-1 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,0-4 0,-1 6 509,3 11-268,-2-1-237,4 22 158,-1 0 0,-2 1 0,-2 0 0,-5 50-1,4-80-111,0 1-1,-1-1 0,0 1 1,1-1-1,-1 1 0,-1-1 1,1 0-1,0 0 0,-1 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,-1 1 0,1-1 1,0 0-1,0 0 0,-1-1 1,0 1-1,1-1 1,-1 1-1,0-1 0,1 0 1,-1-1-1,0 1 0,0-1 1,0 1-1,0-1 0,1 0 1,-1-1-1,0 1 0,0-1 1,0 0-1,-4-1 0,6 1-347,0-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,0 0 1,-1 1-1,1-1 0,0 0 0,0 0 1,0 0-1,-2-4 0,2 3-281,-8-20-3436</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -11430,9 +11430,9 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">75 134 10325,'0'0'7334,"-20"66"-7588,2-13 356,-17 57-2346,34-93-2965,1-13 2342</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="200.21">50 160 7363,'0'0'5763,"41"25"-5875,-21-3 784,-3-1-256,3-3-175,-8 1-209,5 0-16,3-3-16,-7-6-1393,3-6-1408,-8-4-3730</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="200.2">50 160 7363,'0'0'5763,"41"25"-5875,-21-3 784,-3-1-256,3-3-175,-8 1-209,5 0-16,3-3-16,-7-6-1393,3-6-1408,-8-4-3730</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="403.89">304 61 10453,'0'0'3537,"0"99"-2864,0-69-17,0 3-400,0-5-192,0-2-64,0-3-992,0-6-1938,4-10-1744</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="711.34">398 232 7940,'0'0'5127,"-6"13"-5041,-18 40-89,23-52 6,1 0-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,0 0 1,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 1,-1 0-1,1 1 1,-1-1 0,1 0-1,0 1 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 0 1,0 0-1,-1 0 1,2 0-1,35-3 387,-35 2-365,3 0 11,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,-1 1-1,1-1 0,-1 0 1,0-1-1,0 1 1,0-1-1,0 0 0,5-6 1,-7 7 3,1 0 1,-1-1 0,0 1-1,0-1 1,0 1-1,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,-1-7-1,0 10-29,1 0-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1 0,-1 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,0 0 0,-1-1-233,0 1 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,1 1 1,-1-1-1,0 1 1,1-1 0,-3 4-1,-3 12-2681,6 2-1884</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="711.33">398 232 7940,'0'0'5127,"-6"13"-5041,-18 40-89,23-52 6,1 0-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,0 0 1,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 1,-1 0-1,1 1 1,-1-1 0,1 0-1,0 1 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 0 1,0 0-1,-1 0 1,2 0-1,35-3 387,-35 2-365,3 0 11,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,-1 1-1,1-1 0,-1 0 1,0-1-1,0 1 1,0-1-1,0 0 0,5-6 1,-7 7 3,1 0 1,-1-1 0,0 1-1,0-1 1,0 1-1,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,-1-7-1,0 10-29,1 0-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1 0,-1 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,0 0 0,-1-1-233,0 1 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,1 1 1,-1-1-1,0 1 1,1-1 0,-3 4-1,-3 12-2681,6 2-1884</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1503.66">813 220 9636,'0'0'6611,"-3"6"-6643,2-5 27,-1 4-30,0-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,1 0 0,0 0 0,0 0 0,1 9 0,0-13 19,-1-1 1,0 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1-1-1,1 0 1,0 0-21,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 0,1-1 1,-1 1-1,1 0 1,-1-1-1,1 0 1,-1 1-1,0-1 1,2-3-1,-2 3 49,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,-1 0-1,-1-4 1,2 5 23,-1 0-1,0 0 0,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 0,0 0 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,0-1 0,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,-2 1 1,2-1-44,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1-1,0 1 1,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1-1,1 1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 1 0,-3 29-900,3-28 705,1-2 105,0 0 0,-1-1 0,1 1 1,0 0-1,-1 0 0,1-1 0,0 1 0,0 0 1,0-1-1,0 1 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,1-1 0,37 0-502,-38 0 584,6 0-14,-1 0 1,1-1-1,0-1 0,-1 1 0,0-1 1,1 0-1,-1 0 0,0-1 0,0 0 1,-1 0-1,1 0 0,-1-1 0,0 0 1,0 0-1,5-7 0,-2 2 338,0 0 1,-1 0-1,0-1 0,-1 0 0,0-1 1,-1 0-1,6-18 0,-3 9 509,2-16 1232,-10 36-1438,3 29-1318,-5 255 1292,-4-106-229,6-176-355,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,0-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0-1 1,10-8 139,-7 4-155,1-1 1,-1 0-1,0 1 1,0-2-1,-1 1 0,1 0 1,-2 0-1,1-1 0,-1 1 1,1-1-1,-2 1 0,1-1 1,-1 0-1,0 1 0,0-1 1,-1 1-1,0-1 1,0 1-1,-1-1 0,1 1 1,-1-1-1,-1 1 0,1 0 1,-1 0-1,0 0 0,-1 1 1,1-1-1,-1 1 1,0-1-1,0 1 0,-1 0 1,0 1-1,0-1 0,0 1 1,0 0-1,-1 0 0,1 1 1,-12-6-1,17 9 10,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,0 1 1,-1 0-1,1 0 1,0 0-1,0 0 0,0-1 1,0 1-1,-1 0 1,1 0-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,-1 0-1,1 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,1 0 1,-1 0-1,0-1 0,14-5-559,35-3-1102,-39 8 1077,26-6-1918,1 0-1419</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4016.56">1573 207 2305,'0'0'13369,"-1"-1"-13296,1 0 0,-1 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,0-1 1,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 0-1,-3 0 1,-2 2-41,1 0-1,-1 1 0,0 0 1,0 0-1,1 0 1,0 0-1,0 1 0,0 0 1,0 0-1,0 0 1,1 0-1,0 0 0,-1 1 1,2-1-1,-1 1 1,0 0-1,1 0 0,0 0 1,0 0-1,1 1 1,0-1-1,-1 0 0,2 1 1,-1-1-1,0 11 1,2-15-65,-1 0 1,1 0-1,-1 0 1,1 0-1,-1-1 1,1 1 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,2 0-1,37 2-1221,-35-2 1067,9-2-468,-1 0 0,0-1-1,1 0 1,-1-1 0,0 0-1,-1-1 1,1-1 0,-1 0 0,0 0-1,0-2 1,-1 1 0,0-1-1,0-1 1,-1 0 0,13-14-1,-11 1 1470,-10 6 7238,-2 46-8100,0-15 140,-1-11-75,1-1 0,0 0 0,0 1 0,0-1 0,0 0 1,1 1-1,-1-1 0,1 0 0,0 1 0,2 5 1,-1-8 5,0 1 0,-1-1 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,1-1-1,-1-1 1,0 1-1,2 0 0,-1-1-13,0 1 0,0-1 0,0 1-1,-1-1 1,1 0 0,0 0-1,0 0 1,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0-1 0,-1 1 0,1 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,0 1 0,0-1-1,0 0 1,1-4 0,-2 6-16,1-1-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,-1 0 1,1 0 0,0 1-1,-1-1 1,1 0 0,-1 0-1,1 0 1,-1 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1 0 0,0 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,1 0 0,-1 0-1,0 0 1,-3 0 0,2 0-6,1 0 1,-1 0 0,0 0 0,0 1-1,0-1 1,0 1 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,1 1 0,-1-1-1,1 1 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,1 0 0,0 0 0,-1-1-1,1 1 1,0 0 0,1 0-1,-1 0 1,1 6 0,0-9-7,-1 1 1,1 0-1,-1-1 1,1 1-1,0 0 1,-1-1-1,1 1 1,0-1 0,0 1-1,-1-1 1,1 1-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,1-1-1,27 1-287,-22 0 193,3-1-14,0 0 0,0 0 0,0-1 0,0 0 0,-1-1 0,1 0 0,-1-1 0,0 0 0,0 0 0,0-1 0,-1 0 0,1 0 1,-1-1-1,11-10 0,-12 10 123,-1 0 1,0-1-1,0 1 1,-1-1-1,0 0 1,0 0-1,-1 0 1,0-1-1,0 0 1,-1 0-1,0 0 1,0 0-1,-1 0 1,0-1-1,0 1 1,1-16-1,-7-46 2853,-3 73-2914,1 8-145,-5 18 551,2 1-1,1 0 0,1 0 0,1 0 0,2 1 0,0 37 0,4-61-267,-1 0 0,2-1-1,-1 1 1,1 0 0,0 0-1,1 0 1,-1-1 0,5 12-1,-4-16-55,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1-1 0,1 1 0,4-1-1,-3 0 8,1-1-1,-1 1 0,0-1 0,1 0 0,-1 0 1,0 0-1,0-1 0,0 1 0,-1-1 0,1 0 1,-1 0-1,1 0 0,-1-1 0,0 1 0,0-1 1,3-6-1,3-2-71,-1-1 0,-1 0 0,0 0 0,5-14 0,-6 12-11,8-31 51,-14 45 178,-1 35-734,1-33 564,-2 3 9,1 1-1,0 1 1,0-1 0,0 0 0,0 0 0,1 0 0,0 0 0,1 9-1,0-13-13,0 1-1,0-1 1,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0-1-1,2 1 1,6 0-102,0-1-1,0 0 1,0 0 0,0-1 0,-1 0-1,1 0 1,0-1 0,-1 0 0,0-1-1,15-8 1,-19 9 144,-1 0-1,0-1 1,0 1 0,0 0-1,0-1 1,-1 0-1,1 0 1,-1 0-1,0-1 1,0 1 0,-1-1-1,1 1 1,-1-1-1,0 0 1,0 0 0,-1 0-1,0 0 1,1 0-1,-2 0 1,1-1 0,0 1-1,-1-6 1,0 17 685,-1 10-606,0 0 0,2 0 0,0 0 0,1 0 0,0-1 0,1 1 0,7 18 0,-9-32-111,1 0 1,0 0-1,-1-1 0,1 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 0 0,0 1 1,1-1-1,-1 0 0,0 0 0,1-1 1,-1 1-1,0 0 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1-1 0,4 0 1,3-1-103,0 0 1,0-1 0,0 0-1,-1 0 1,17-10 0,-18 9-166,1-1 0,-1-1 1,0 1-1,-1-1 0,1 0 1,-1 0-1,0-1 0,-1 0 1,1 0-1,-2 0 1,1-1-1,-1 0 0,0 1 1,3-11-1,-4 10 469,-1 0 1,0 0-1,-1 0 0,0 0 1,0-13 1349,-1 59-1145,-1-25-230,0-1 0,-1 0 0,0 0 0,-1 0 0,0-1 0,-6 14 0,13-39 829,-3 8-1017,0 0 1,0 0-1,1 1 1,0-1 0,0 1-1,1-1 1,3-4-1,-6 9 3,24-28-277,-23 28 248,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 1,0 0-1,-1 0 0,2 1 0,-1-1 17,-1 1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,-1 1-1,1-1 1,0 0-1,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 1,0 1-1,0-1 0,0 0 1,1 1-1,-1-1 1,-1 2-1,2 37 69,-1-33-24,-8 73 1645,8-80-1220,2-28-16,1 20-560,0-1-1,0 1 0,1 0 1,1 0-1,-1 0 0,2 1 1,-1 0-1,0 0 0,13-12 1,-13 14-38,0 1 1,0 0 0,0 0 0,0 0 0,0 1 0,1 0-1,0 0 1,0 0 0,0 1 0,0 0 0,0 0-1,0 0 1,0 1 0,0 0 0,8-1 0,-14 3 141,1-1 0,0 1 0,0 0 1,-1-1-1,1 1 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,-1 2-1,1 35 292,0-30-102,0 63 1602,3-71-1737,-1 0 0,1 0 0,0-1-1,0 1 1,0 0 0,0-1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,5-2 0,1-3-9,0-1-1,-1 1 1,0-1 0,-1-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,0-1-1,-1 0 1,0 0 0,0 0 0,-1 0 0,0 0 0,-1-1 0,0 1 0,0-1 0,-1 0-1,0-15 1,-1 25-16,-1-1 0,1 1 0,0-1 0,-1 1-1,1-1 1,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0-1,-1 1 1,1-1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1-1,-1-1 1,-23 12-111,22-10 66,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0-1,1 0 1,-1-1 0,1 1 0,0 0 0,0 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,3 2-1,1 2-126,1 0 0,0-1 0,0 1 0,0-1 0,1-1 0,0 1 0,7 4 0,-5-3 60,-8-7 99,0 0 0,1 1 0,-1-1-1,0 0 1,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1-1,0 1 1,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0-1,1 0 1,-2 0 0,-39 11 307,31-8-346,-69 17-2096,31-10-2404</inkml:trace>
 </inkml:ink>
@@ -11585,13 +11585,13 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13771.33">1909 527 4098,'0'0'6227,"3"-11"-5408,2-2-426,-3 9-100,0-1 1,-1 0 0,0 1-1,1-1 1,-2 0 0,1 0-1,0 0 1,-1-8 1038,0 19-1653,-2 72 1443,-17 121 0,9-132-887,-48 426 1710,52-391-1776,-4-1 0,-33 149 0,-18 62 87,18-75 1043,30-195-1063,11-37-272,0 1-1,0 0 0,0 0 0,1 0 0,0 0 1,-1 8-1,2-48-19964</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15879.65">350 934 4162,'0'0'6688,"-10"-8"-3441,37 16-1567,-6-1-927,1-1 0,0-1 0,0-1 0,40 2 0,-62-6-766</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16269.13">474 899 1201,'0'0'8961,"-13"-10"-1739,127 5-7694,-113 38 378,-1-29 107,0-1 0,-1 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0-1,0-1 1,-1 1 0,1-1 0,-1 0 0,-4 4-1,-59 34 194,43-28-209,19-7-1066</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18906.6">289 1473 6435,'0'0'6360,"39"4"-2902,-9-4-3226,-3 1-155,0 0-1,0-2 1,1-2 0,-1 0-1,0-1 1,0-2 0,29-10-1,-55 16-73,-1-1 0,1 1-1,0 0 1,0-1 0,0 1-1,-1-1 1,1 1 0,0-1-1,-1 0 1,1 1-1,0-1 1,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0 0,0 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,0-1-1,1 0 1,-1 1 0,1-1-1,-1 1 1,0-1 0,-1 0-1,-40-32 131,42 33-132,-1 0 0,-1-1 1,1 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1-2 0,1 2-24,20 7-533,11 5 544,9 5 39,-39-16-35,1 1 0,-1 0 1,0 1-1,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 1,0-1-1,0 1 0,0 2 0,0 0 18,-1-1 0,0 1 0,0-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,-7 3 0,-26 22-2753,34-27 335</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18906.59">289 1473 6435,'0'0'6360,"39"4"-2902,-9-4-3226,-3 1-155,0 0-1,0-2 1,1-2 0,-1 0-1,0-1 1,0-2 0,29-10-1,-55 16-73,-1-1 0,1 1-1,0 0 1,0-1 0,0 1-1,-1-1 1,1 1 0,0-1-1,-1 0 1,1 1-1,0-1 1,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0 0,0 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,0-1-1,1 0 1,-1 1 0,1-1-1,-1 1 1,0-1 0,-1 0-1,-40-32 131,42 33-132,-1 0 0,-1-1 1,1 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1-2 0,1 2-24,20 7-533,11 5 544,9 5 39,-39-16-35,1 1 0,-1 0 1,0 1-1,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 1,0-1-1,0 1 0,0 2 0,0 0 18,-1-1 0,0 1 0,0-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,-7 3 0,-26 22-2753,34-27 335</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20627.12">340 1804 1169,'2'-3'17365,"11"-9"-17277,18 3-81,0 0 1,1 2 0,0 1-1,0 2 1,60-1-1,-91 5-45,-1-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1-1,0 1 1,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0-1,0-1 1,-1 1 0,0-1-1,0 0-24,-4-3-61,-1 0 0,1 1 0,-1 0 0,1 0 0,-1 1 1,0-1-1,0 1 0,-12-2 0,35 11 75,3 2 111,0-1 1,25 6 0,-44-14-64,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 1 0,-1 0 7,0-1-1,-1 0 1,1 1-1,-1-1 0,1 0 1,-1 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,-1 1 1,-52 34 251,50-34-241,-52 28-121,32-18-3141,9-5-1247,4-1-1029</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22607.28">333 2068 176,'0'0'10885,"-12"0"-3754,35 0-6546,9 1-405,1-1-1,0-2 1,0-2 0,33-7 0,-65 11-169,-1 0 0,1 0-1,0 0 1,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,1 0 0,-13-12-24,-33-7-152,42 19 212,-2-2-77,-19-8 131,20 8-198,13 7-250,131 43 544,-139-46 6,-1-1-144,-1 3-59,-1 1 0,0-1 1,1 0-1,-1 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,-1-1 0,0 1 0,1-1 1,-1 0-1,0 0 0,-6 3 0,-11 11-6,6-1-267,-34 41-3474,45-52 3330,0 0 0,1 0-1,-1 1 1,1-1-1,0 1 1,0 0 0,1 0-1,-1-1 1,1 1 0,0 0-1,0 9 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27230.95">2768 502 464,'0'0'7446,"-3"-4"-6539,-10-14-292,4 13 7558,2 38-7922,-32 149 1146,-6 25-537,-1-59-636,11-39 29,-37 207 1,36-155 127,22-109-156,-11 83-1,18-84-29,-17 60-1,-8 39 988,30-140-1082,0 0-1,0 0 0,0 21 1,-15-70-8696,10-1-4178</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28136.9">31 701 4002,'0'0'8169,"-3"-7"-6667,-2-4-1528,-2-4 2938,4 37-1412,3 12-1516,-2-1 0,-6 36 0,7-60-182</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28520.06">2 790 256,'0'0'11128,"0"-1"-10990,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 1,0-2-1,9 0-16,0 0 0,0 0 0,1 1 0,20-2 0,22-5-5617,-53 8 5123,1 1 0,0-1 1,0 1-1,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 0 1,1 0-1,-1 1 0,1-1 1,-1 0-1,0 0 0,1 0 1,-1 1-1,0-1 0,1 0 1,-1-2-1,4-40 3674,-4 24 3309,-1 49-5100,1 71-68,0-59-5594</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28930.61">204 672 5491,'0'0'8425,"0"-6"-6907,-17 147-339,56-139-862,-33-2-300,1-1 1,0-1-1,0 1 0,-1-1 0,1 0 0,-1-1 0,1 0 0,-1 0 0,9-5 0,13-15-6583</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28930.6">204 672 5491,'0'0'8425,"0"-6"-6907,-17 147-339,56-139-862,-33-2-300,1-1 1,0-1-1,0 1 0,-1-1 0,1 0 0,-1-1 0,1 0 0,-1 0 0,9-5 0,13-15-6583</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29875.73">2733 81 4082,'0'0'8617,"27"51"-6920,-26-50-1678,0 5 18,1-1 1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,1-1 0,-1 1 0,8 7 0,-11-12 39,1 0 0,0 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,-1-1 0,1 1 0,-1 0 1,0-1-1,1 1 0,-1-1 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 1 0,0-1 1,0 1-1,0-1 0,1 1 0,-1-1 1,0 0-1,11-24 138,-8 18-89,5-11-131,-3 10-135,-1-1-1,0 0 1,-1-1 0,0 1-1,0 0 1,2-16 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30078.97">2949 93 6547,'0'0'5491,"0"-9"-7668</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30421.69">3054 0 3249,'0'0'6700,"0"5"-6551,0 124 3885,36-127-2151,-25-4-1697,-1 0 0,1 0 0,-1-1-1,1 0 1,-1-1 0,16-9-1,21-6-930,0 10-3734</inkml:trace>
@@ -11767,7 +11767,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">34 111 3570,'0'0'6939,"-1"-7"-6304,-6-37 1456,4 32 1205,-2 21-1963,-3 23-1101,-1 269 283,9-299-496,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 0,0 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1-1-1,0 1 1,0 0-1,0-1 1,1 1-1,1 0 1,3 0 37,0 0 0,0 0-1,0 0 1,0-1 0,1 0 0,5-1 0,11 0-43,-9 0 265,0 0 0,0-2 0,20-4 0,10-2-3320,-13 6-6852,-22 3 3843</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="484.12">366 262 3394,'0'0'8977,"-1"-4"-8043,1 2-821,0 0 1,0 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 1 1,-1-1 0,0 1-1,1-1 1,-3-2 0,2 4 491,-19 24 372,17-17-871,-1 0 0,2 0 0,-1 1 0,1-1 1,0 1-1,1-1 0,0 1 0,0 0 0,1 0 0,0-1 0,0 1 1,0 0-1,4 13 0,-3-19-98,0 0 1,0-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,3-1-1,0 1 10,0 0-1,-1 0 1,1-1 0,0 0-1,-1 0 1,0 0 0,1-1-1,-1 1 1,0-1-1,0 0 1,6-6 0,-8 7-2,0 0 0,0-1 0,0 1 0,-1 0 1,1-1-1,-1 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 1-1,-1-1 0,-1-3 0,0 2-35,0 1 0,0 0 0,0 0 0,-1 0 1,1 1-1,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 1 0,1-1 0,-6 1 0,9 1-193,1-1-1,-1 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,1-1 1,-1 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,1-1 1,-1 1-1,0-1 0,0 1 0,1-1 1,-1 1-1,0-1 0,1 1 0,13 6-4191</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="934.97">666 248 2753,'0'0'10554,"-6"-2"-9452,3 0-1042,1 1 6,0 0 0,1 0-1,-1 0 1,1 1-1,-1-1 1,0 0-1,0 1 1,0-1 0,1 1-1,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0 0,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,0 0 1,-3 3 0,-1 2 61,0 0 1,0 1-1,1 0 1,-1 0-1,2 0 1,-1 0-1,1 1 1,0 0-1,-4 15 1,7-21-115,0 0 1,0 0-1,0 0 0,-1 0 1,2 0-1,-1 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 0,0-1 1,0 1-1,0 0 0,2 1 1,-1-1-4,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 1,0 1-1,0-1 0,3-1 0,0 1 7,1 0 0,-1 0 1,1-1-1,-1 0 0,0 0 1,1-1-1,-1 0 0,0 0 1,0 0-1,11-7 1,-14 7-6,0 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,0 0 1,0-1-1,0 1 0,0-1 0,-1 1 0,0-1 0,1-7 0,-2 3 25,1-1-1,-1 0 1,0 1 0,-5-16-1,6 22-32,-1 0 0,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 1 1,0-1 0,0 1-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1-1 1,0 1-1,0 0 1,1 1-1,-1-1 1,0 0 0,0 0-1,0 1 1,0-1-1,-3 0 1,4 1-175,1 1-821,1 0 592,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 1,1 1-1,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1-1 0,0 1 0,0-1 0,0 1 0,1 0 1,17 0-4257</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1275.13">900 79 4514,'0'0'9458,"-4"-6"-8431,-9-19-336,9 19-347,4 9-203,-7 45 792,2 1-1,2 0 0,5 60 1,-1-27-877,-1-81-167,0-1 1,0 1-1,0-1 0,1 1 0,-1 0 1,0-1-1,0 1 0,0-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,1 1 0,-1-1 1,1 0-1,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,1 0-437,-1 0 1,1 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 1 0,3-3 1,8-11-4960</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1275.12">900 79 4514,'0'0'9458,"-4"-6"-8431,-9-19-336,9 19-347,4 9-203,-7 45 792,2 1-1,2 0 0,5 60 1,-1-27-877,-1-81-167,0-1 1,0 1-1,0-1 0,1 1 0,-1 0 1,0-1-1,0 1 0,0-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,1 1 0,-1-1 1,1 0-1,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,1 0-437,-1 0 1,1 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 1 0,3-3 1,8-11-4960</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2640.65">985 205 1985,'0'0'9594,"-5"3"-8036,1 2-1292,1 0 1,-1 0 0,-1 0 0,1-1 0,-1 0-1,1 0 1,-1 0 0,0 0 0,-1-1 0,-9 5 1870,17-5-2119,0 0 1,0-1 0,0 1-1,1 0 1,-1-1 0,1 0-1,0 1 1,0-1 0,0 0-1,0-1 1,6 4 0,2 2 138,-3 0-123,1-1-1,-1 1 1,1-1-1,0-1 1,1 0-1,-1 0 1,1-1-1,0 0 1,0-1-1,0 0 1,0-1 0,1 1-1,19 0 1,-29-3-40,0-1-1,0 1 1,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1-1 0,6-44-3,-3 19 40,-2 33 83,-1 1 0,1-1 1,0 1-1,0-1 1,1 1-1,2 6 1,-3-10-100,0-1 1,-1 1-1,1-1 1,1 1 0,-1-1-1,0 1 1,1-1-1,-1 0 1,1 0-1,-1 1 1,1-1 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,1-1-1,-1 0 1,0 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,1 0-1,0-1 1,4 1-1,-5-1-14,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 1 0,0-2 0,2-2 0,-1 0 1,0 0 0,0-1 0,0 1 0,-1 0 0,1-9 0,1-24 5,-4 31-5,1 14-2,-1-3 3,1 0-1,0 1 1,1-1 0,-1 0-1,1 0 1,0 1 0,0-1-1,0 0 1,1 0 0,-1 0-1,4 7 1,-3-9-1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,0 0 0,1-1 1,0 1-1,-1-1 1,1 1-1,-1-1 1,1 0-1,0 0 1,2 0-1,-1 0-10,1 0 0,-1 0-1,0 0 1,1-1 0,-1 1-1,0-1 1,1 0 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,-1-1 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,-1 1 0,0-1-1,1 0 1,-1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0-8-1,2-3-15,-1 0-1,0-1 0,-2 1 1,0 0-1,0-1 0,-2 1 1,-2-25-1,3 40 26,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 1 1,1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,-6 21-50,-3 28-2,5-19 133,2 1 0,1 0 0,1-1 0,2 1 0,1 0 1,11 49-1,-5-58 597,-9-50 721,1-11-1494,0 29 74,1 0 1,0 1-1,1-1 0,0 1 1,0-1-1,1 1 1,1 0-1,7-12 0,-10 17-14,1 1-1,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,1 1 1,0-1-1,0 1 0,0 0 1,0 0-1,0 1 1,0-1-1,1 1 0,-1 0 1,0 0-1,1 0 1,-1 1-1,5-1 1,-8 1 32,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 0 0,0 1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 1,1 0-1,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 1,-1 0 9,1 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 1,-1-1-1,-1 3 0,-5 0 54,1 0 0,-1 0 0,0-1 0,0 0 0,-1 0-1,1-1 1,0 0 0,-1 0 0,1-1 0,-13 0 0,21-1-392,12 0-14913</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4247.33">1929 327 2081,'1'-3'15081,"-1"3"-15073,0-1 1,0 1 0,0-1-1,0 1 1,1 0 0,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1 0,0 1-1,1 0 1,-1-1 0,0 1-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1 0 0,-1-1-1,1 1 1,0 0 0,611-14 1052,-392 16-1002,-220-1-58,1-1 1,0 0-1,0 0 0,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0-1-1,0 1 0,0 0 1,-1-1-1,1 1 0,0 0 0,0-1 1,-1 1-1,1-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1-1 1,-1 0-1,1 1 0,-1-1 0,1 0 1,0 0-1,-2-1-24,0 1 0,1-1 0,-1 1 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,-1-2 0,-4-2 33,1 1 17,0 1 1,0-2-1,1 1 0,0-1 1,-1 1-1,1-2 1,-7-6-1,12 10 144,38 17-546,-19-6 371,-14-9-25,0 0 1,0 1-1,0 0 0,-1 0 1,1 1-1,-1-1 0,6 5 0,-10-7 21,0 0-1,1 0 0,-1 1 1,0-1-1,0 0 0,1 0 0,-1 1 1,0-1-1,0 0 0,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 1,-1 1-1,-23 12-299,-38 7-2461,-1-3-3746,29-8 320</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4869.14">1905 228 2209,'0'0'7214,"2"-2"-6360,9-9-174,-8 8 43,-3 29 534,-1-18-1112,0 0 0,0 1 0,-1-1 0,0-1 1,-1 1-1,1 0 0,-2-1 0,1 1 0,-8 12 1,-7 15-3,17-34-136,1 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,0 0 0,23 9 133,41-9 5,-51-2-122,29 0-17,44 2-1002,-87-1 884,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 1 0,0-1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,1 0-1,-1 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1-345,0 7-6119</inkml:trace>
@@ -12171,14 +12171,14 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">0 57 3458,'0'0'7776,"0"-5"-7253,0-16 299,0-9 5226,4 56-6507,4 13 479,-3-1 0,1 44 0,-1-6 0,-3-58-16,1 45 104,43-63 314,-34 0-300,-8 1-93,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,-1-1 0,1 0 0,0 1 0,5-3 0,-8 2-16,-1-1-13,0 2-88,1 0-538,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1-1 0,7-7-4649</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="619.68">251 85 3986,'0'0'6627,"-1"-5"-5957,0-4-947,-1-3 2038,2 31-570,4 273 933,-4-291-2423,1 0-1,-1-1 0,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,1-1 1,1 1-1146,6 0-3520</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1115.14">403 86 3410,'0'0'6563,"0"-4"-5707,0-15-112,0 14 1679,-24 20-2359,-4 17 243,19-21-655,17-20-2276,4-2-687</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1115.13">403 86 3410,'0'0'6563,"0"-4"-5707,0-15-112,0 14 1679,-24 20-2359,-4 17 243,19-21-655,17-20-2276,4-2-687</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2059.1">419 50 1121,'0'0'8243,"-8"-12"-4115,0 12-3957,1 0 0,-1 1 1,0 0-1,0 0 0,-15 4 1,21-4-141,-1 0-1,0 1 1,1-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,-2 4 0,-25 74 854,22-40-449,0-1 1,3 1-1,2 52 0,1-86-425,0-5-7,1-1 0,0 1 1,-1 0-1,1 0 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,-1 0 0,1-1 0,0 1 1,0-1-1,0 0 0,-1 0 1,1 1-1,0-1 0,0-1 1,2 1-1,63-2 210,-67 2-213,6-1 103,-1 0-1,1 0 1,-1-1-1,1 0 0,-1 0 1,0 0-1,0-1 1,0 0-1,0 0 1,-1 0-1,1 0 0,-1-1 1,0 0-1,0 0 1,0 0-1,4-6 0,-7 9-203,-1 1-1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 0,0 0 0,-5 4-5533</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2506.69">797 157 2945,'0'0'10947,"-6"-3"-6577,62-1-3889,-1-3 1,85-20 0,-132 25-468,6-1-115,-1 0 0,0-1 0,0-1 1,16-7-1,-28 11-702</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2845.8">953 267 4930,'1'0'11247,"8"2"-10766,9-2-157,0-2 0,-1 0-1,1-1 1,-1-1-1,1 0 1,-1-1 0,-1-1-1,1-1 1,21-11-1,-37 14-120</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3456.17">866 45 5923,'0'0'11109,"-6"-3"-10031,-18-9-393,17 9-375,45 4-310,-1 8 84,0 1-1,40 17 1,14 5-52,-72-26-20,11 4 11,0-2-1,0 0 1,1-2-1,62 3 1,-93-9 281,-1 4-303,-1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1-1 0,-1 1 1,0-1-1,0 0 0,-1 0 0,1 0 0,-5 3 0,-13 14 0,-118 164 709,138-184-764,1 0 1,-1 1 0,1-1-1,-1 0 1,1 1-1,0-1 1,-1 0 0,1 1-1,-1-1 1,1 0-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1-1,0-1 1,-1 0 0,1 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1-1,-1 1 1,1 0 0,0-1-1,0 1 1,1-1-1,-1 1 1,0-1 0,0 1-1,0-1 1,0 1-1,22-5-4474,2-7-53,1-3-2092</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4214.46">1610 172 3490,'0'0'11762,"0"-4"-10500,11 206 2257,-10-176-3016,-1-20 312,0-17-329,-1-20-525,2-1 1,1 1-1,1-1 1,2 1-1,1 0 0,1 0 1,2 1-1,13-31 1,-20 57 24,0 1 0,1-1 1,-1 1-1,1 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 1 1,1-1-1,-1 1 0,0 0 0,1 0 1,0 0-1,-1 0 0,1 1 0,0 0 1,0-1-1,0 1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 1,6 1-1,-8 0 5,-1-1 0,1 1 0,-1-1-1,0 1 1,0-1 0,1 1 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-2 0 0,1 0 0,0 0-1,0 0 1,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1-1,0-1 1,1 1 0,-2 1 0,2 3-1,0 1 0,-1-1 0,0 0-1,-1 1 1,1-1 0,-2 7 0,-1-6-8,0 0-1,-1-1 0,0 1 1,1-1-1,-2 0 0,1 0 1,-1-1-1,0 1 0,0-1 1,-1 0-1,-8 6 1,-2 1-389,-1 0 0,-34 18 1,49-30 349,1 1 1,0 0-1,0-1 0,0 1 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 0 1,-1 0-1,-1-1 0,3 1 39,-1-1 0,1 1 1,-1 0-1,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 3,0-1 0,0 1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 1,0-1-1,0 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,3 0 0,37 2-72,-36-1 107,0 0 0,0 1 1,-1 0-1,1 0 0,-1 0 0,1 1 1,-1-1-1,0 1 0,0 0 0,6 6 1,39 42 604,-24-23-99,-22-26-776,41 39 1499,-18-23-2319,-2-11-5017,-15-7-710</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4387.93">2036 299 9476,'0'0'8900,"0"-29"-9172,8 29-1505,-4 0-2801,9 0-2769</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4749.98">2381 71 6259,'0'0'8969,"-2"-4"-8398,2 4-565,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 1 0,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0-1,0-1 1,-1 1 0,1 0-1,-1-1 1,1 1-1,-1 0 1,1-1 0,-1 1-1,1 0 1,0 0-1,-1 0 1,0-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1 0,-1-1-1,-28 33 281,-18 50 587,41-70-716,1 0 1,0 1-1,1 0 0,1 0 0,0 0 0,1 0 0,0 1 1,1-1-1,1 1 0,3 27 0,-2-38-138,0-1 1,0 1-1,1-1 1,0 1-1,-1-1 0,1 1 1,1-1-1,-1 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,0-1 0,0 1 1,0-1-1,0 0 1,1 1-1,-1-2 0,1 1 1,-1 0-1,1-1 0,-1 1 1,1-1-1,0 0 1,0 0-1,-1-1 0,1 1 1,6-1-1,1 1 17,-1 0-1,1-1 1,-1 0-1,1-1 1,-1 0 0,1 0-1,-1-1 1,0-1-1,16-5 1,-12 2-66,0 0-1,-1-1 1,0-1 0,-1 0 0,1-1-1,-2 0 1,1-1 0,13-15 0,-20 17-748,-7 2-2521,-8 4-3832</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4387.92">2036 299 9476,'0'0'8900,"0"-29"-9172,8 29-1505,-4 0-2801,9 0-2769</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4749.97">2381 71 6259,'0'0'8969,"-2"-4"-8398,2 4-565,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 1 0,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0-1,0-1 1,-1 1 0,1 0-1,-1-1 1,1 1-1,-1 0 1,1-1 0,-1 1-1,1 0 1,0 0-1,-1 0 1,0-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1 0,-1-1-1,-28 33 281,-18 50 587,41-70-716,1 0 1,0 1-1,1 0 0,1 0 0,0 0 0,1 0 0,0 1 1,1-1-1,1 1 0,3 27 0,-2-38-138,0-1 1,0 1-1,1-1 1,0 1-1,-1-1 0,1 1 1,1-1-1,-1 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,0-1 0,0 1 1,0-1-1,0 0 1,1 1-1,-1-2 0,1 1 1,-1 0-1,1-1 0,-1 1 1,1-1-1,0 0 1,0 0-1,-1-1 0,1 1 1,6-1-1,1 1 17,-1 0-1,1-1 1,-1 0-1,1-1 1,-1 0 0,1 0-1,-1-1 1,0-1-1,16-5 1,-12 2-66,0 0-1,-1-1 1,0-1 0,-1 0 0,1-1-1,-2 0 1,1-1 0,13-15 0,-20 17-748,-7 2-2521,-8 4-3832</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -12238,7 +12238,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="109.56">344 73 5122</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="479.54">344 73 5122,'2'-38'2639,"-2"39"-2537,0-1 1,-1 0-1,1 0 1,0 1 0,0-1-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,-15 18 536,7 1-459,0 0 1,1 0 0,1 1-1,1 0 1,1 0-1,1 0 1,0 0-1,0 31 1,6-49-167,-1 0 0,1-1-1,-1 1 1,1 0 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,5-1 0,-2 1 34,-4 0-31,5 0-6,0-1 0,0 1 0,0 1 0,0 0 0,0-1 0,0 2 1,11 2-1,-16-3-38,1 0 1,-1 1 0,1-1 0,-1 0 0,0 0-1,0 1 1,1-1 0,-1 1 0,0-1 0,0 1 0,0 0-1,0-1 1,-1 1 0,1 0 0,0-1 0,-1 1-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,0 1 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,0 2 0,0-2 57,0 1 0,0 0 1,0 0-1,0-1 0,-1 1 0,1-1 0,-1 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0-1 0,-5 4 1,-46 25 319,33-19-340,19-11-470,-10 5 1022</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="792.7">638 72 7988,'0'0'9788,"0"-5"-9390,3-16-184,3 21-176,3 12-26,-2-1 58,-1 1-1,1 0 1,-2 0 0,0 0 0,0 1 0,-1 0-1,0 0 1,2 21 0,-5-27-180,-1 1 0,1-1 1,-1 1-1,-1-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,0-1 0,0 0 0,-1 0 1,0 0-1,0-1 0,0 1 0,-1-1 1,-9 12-1,1-5-1166,0 0 1,0-1-1,-1-1 0,-1 0 1,0 0-1,-21 10 0,-7-1-5377</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1203.62">131 25 8660,'0'0'5944,"-10"15"-5664,0-1-163,0 0-2,1 1 1,1-1 0,0 1 0,0 1-1,-4 16 1,0 0-46,1 1 0,2 0-1,2 0 1,0 1 0,3 0 0,-2 54-1,7-82-312,-1-1 0,1 1 0,0 0 0,0-1 0,1 0 0,-1 1 0,1-1 0,1 0 0,-1 0 0,6 9 0,-5-9-290,0-1 0,1-1 1,-1 1-1,1 0 0,0-1 1,0 0-1,0 0 0,0 0 1,1 0-1,-1-1 1,10 4-1,18 4-5336</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1203.61">131 25 8660,'0'0'5944,"-10"15"-5664,0-1-163,0 0-2,1 1 1,1-1 0,0 1 0,0 1-1,-4 16 1,0 0-46,1 1 0,2 0-1,2 0 1,0 1 0,3 0 0,-2 54-1,7-82-312,-1-1 0,1 1 0,0 0 0,0-1 0,1 0 0,-1 1 0,1-1 0,1 0 0,-1 0 0,6 9 0,-5-9-290,0-1 0,1-1 1,-1 1-1,1 0 0,0-1 1,0 0-1,0 0 0,0 0 1,1 0-1,-1-1 1,10 4-1,18 4-5336</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -12327,7 +12327,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">79 67 2497,'0'0'10042,"-1"-8"-8759,-2-42 2220,-15 107-3511,-1 9 115,10-38-80,1 0 0,2 0 1,0 0-1,-2 53 0,8-81 104,0-15 7,2-5-160,1-1-1,0 1 1,2 0-1,1 0 0,10-27 1,2-5-96,-17 46 99,2-4-3,-1 0-1,2 0 0,-1 1 0,1-1 0,1 1 0,-1 0 0,2 0 0,-1 0 0,8-7 0,-13 16 17,0-1 1,1 1 0,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1-1,0-1 1,1 0 0,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 1 1,1-1-1,-1 0 1,0 1 0,0-1-1,1 1 1,-1 0-1,11 17 0,1 14-144,0 0-1,-3 1 1,0 0-1,-2 1 0,-2-1 1,3 69-1,-9-101-125,1-1 1,0 1-1,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,0 1-1,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1-1-1,0 1 0,-1 0-174,-7-2-3614</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="273.93">67 217 2785,'0'0'8039,"-4"-3"-7279,1 1-789,-9-8 998,12 10-949,0-1 0,0 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,1-1-1,-1 1 0,0 0 1,0 0-1,0-1 1,1 1-1,-1 0 0,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 1,1 0-1,-1 0 0,1 0 1,12-1 157,1-1 1,-1-1-1,0-1 1,0 0-1,0 0 1,-1-1-1,1-1 1,-1 0-1,22-15 1,-29 16 9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="273.92">67 217 2785,'0'0'8039,"-4"-3"-7279,1 1-789,-9-8 998,12 10-949,0-1 0,0 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,1-1-1,-1 1 0,0 0 1,0 0-1,0-1 1,1 1-1,-1 0 0,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 1,1 0-1,-1 0 0,1 0 1,12-1 157,1-1 1,-1-1-1,0-1 1,0 0-1,0 0 1,-1-1-1,1-1 1,-1 0-1,22-15 1,-29 16 9</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -12506,7 +12506,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">33 223 2785,'0'0'8708,"-4"-11"-7344,-20-49 1023,23 58-2068,-2-10 1545,3 16-943,3 26-773,9 372 429,-11-401-575,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,1 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,2-1-1,34 1 68,-33 0-62,8-2 55,0-1 0,0 0 1,0-1-1,0 0 0,-1 0 0,1-1 1,-1-1-1,-1 0 0,1-1 0,-1 0 1,0 0-1,12-13 0,-2 5 334,-9 10-2072,-2 5-7140</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="185.84">356 386 1105,'0'0'16455,"0"-43"-16455,0 53-4434,0-3-16</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="659.92">783 279 5795,'0'0'6998,"0"-13"-5424,1-2-1204,-1 2 5,1 0 1,-2 1 0,0-1-1,-4-24 1,4 35-331,1-1-1,-1 0 1,0 0-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,-1-1 1,1 1-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 1 1,0-1-1,0 1 1,1-1-1,-6 1 1,2 1-39,1 0 0,-1 1 0,1 0 1,-1 0-1,1 0 0,0 0 0,0 1 0,0 0 0,0 0 1,1 0-1,-1 1 0,1-1 0,0 1 0,0 0 0,0 0 1,1 1-1,-1-1 0,1 1 0,-5 9 0,0 0 4,0-1 0,1 1 0,1 1 0,0-1-1,1 1 1,-4 19 0,7-24-15,0-1 1,1 1-1,1 0 0,-1-1 0,1 1 1,1-1-1,0 1 0,4 16 1,-4-23 56,0 0 0,0 0 1,0-1-1,1 1 1,-1 0-1,1 0 0,0-1 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 0,0-1 1,-1 1-1,1-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,1-1-1,-1 0 0,5 0 1,0-1-3,-1 0 0,1 0-1,-1 0 1,0-1 0,10-4 0,-10 4-1062,1-1-1,-1 1 0,1 1 1,0-1-1,10 0 1,-1 2-3067,-1 0-2020</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2111.28">1255 381 1969,'0'0'9580,"0"-6"-8505,0-3-947,1 7-16,-1 0 1,1 0 0,-1 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 1 1,0-1 0,1 0-1,-1 1 1,0-1 0,-2 1 0,-2-2-93,0 1 1,0 1 0,-1-1-1,1 1 1,0 0 0,-13 2-1,17-1-20,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 1-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 1 1,1-1-1,-1 0 0,1 0 1,-1 1-1,1-1 1,-1 4-1,-2 4 28,0 0 1,1 0-1,1 0 0,-1 0 1,2 1-1,-1-1 0,1 1 1,1-1-1,0 1 0,1-1 1,3 21-1,-4-29-19,1 0-1,0 0 1,0 0 0,-1 0 0,1-1-1,1 1 1,-1 0 0,0 0 0,0-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,4 0 0,-5 0 2,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,1 1 0,-1-1 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,0 0 1,0-3-1,5-14-6,0 0-1,-1-1 1,-2 1-1,1-1 0,-2 0 1,0-29-1,-2 48-35,0 13-347,0 2 369,1 0 0,0 0 0,7 25-1,-8-36 23,1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,6 4 0,-7-5 9,-1-1 1,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0-1,1-1 1,-1 0 5,1-1 1,0 1-1,-1-1 0,1 0 0,-1 0 0,0 0 0,0-1 1,0 1-1,1-5 0,2-3-4,-1 0 0,-1-1 0,0 0 0,-1 1-1,2-16 1,-3-175-177,-1 198 155,0 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,-1 0-1,0 1 1,-3-6-1,4 9-14,1 0 1,-1 0-1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,-1 1 0,1-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,-5 27-17,5-25 10,-7 33 109,3 1 1,1-1 0,1 1-1,2-1 1,8 62 0,-7-93-79,1-1 0,-1 1-1,1 0 1,0 0 0,0-1 0,1 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,1-1 0,0 0 0,0 0-1,7 5 1,-8-7 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1-1-1,1 1 1,0-1-1,0 0 1,0 1-1,-1-1 1,1 0-1,0-1 1,0 1-1,0 0 0,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1-1 1,1 1-1,-1-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-2 1,0 1-1,0 0 1,1-3-1,4-5 29,0 0 1,-1 0-1,-1-1 0,1 0 0,4-17 0,-8 22-31,0 0-1,0 0 0,-1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,-2-1-1,1 1 0,0 0 1,-1 0-1,-2-8 0,-3 7-157,3 18-26,1 16 78,26 23 99,-21-45 3,0-1 1,0 2-1,-1-1 0,1 0 0,-1 0 0,0 1 0,-1-1 0,1 1 1,-1 0-1,0-1 0,0 9 0,-2-13 2,-1 0 1,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-3 0 1,-16 1-732,20-25-11333,0 15 6555</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2111.27">1255 381 1969,'0'0'9580,"0"-6"-8505,0-3-947,1 7-16,-1 0 1,1 0 0,-1 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 1 1,0-1 0,1 0-1,-1 1 1,0-1 0,-2 1 0,-2-2-93,0 1 1,0 1 0,-1-1-1,1 1 1,0 0 0,-13 2-1,17-1-20,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 1-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 1 1,1-1-1,-1 0 0,1 0 1,-1 1-1,1-1 1,-1 4-1,-2 4 28,0 0 1,1 0-1,1 0 0,-1 0 1,2 1-1,-1-1 0,1 1 1,1-1-1,0 1 0,1-1 1,3 21-1,-4-29-19,1 0-1,0 0 1,0 0 0,-1 0 0,1-1-1,1 1 1,-1 0 0,0 0 0,0-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,4 0 0,-5 0 2,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,1 1 0,-1-1 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,0 0 1,0-3-1,5-14-6,0 0-1,-1-1 1,-2 1-1,1-1 0,-2 0 1,0-29-1,-2 48-35,0 13-347,0 2 369,1 0 0,0 0 0,7 25-1,-8-36 23,1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,6 4 0,-7-5 9,-1-1 1,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0-1,1-1 1,-1 0 5,1-1 1,0 1-1,-1-1 0,1 0 0,-1 0 0,0 0 0,0-1 1,0 1-1,1-5 0,2-3-4,-1 0 0,-1-1 0,0 0 0,-1 1-1,2-16 1,-3-175-177,-1 198 155,0 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,-1 0-1,0 1 1,-3-6-1,4 9-14,1 0 1,-1 0-1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,-1 1 0,1-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,-5 27-17,5-25 10,-7 33 109,3 1 1,1-1 0,1 1-1,2-1 1,8 62 0,-7-93-79,1-1 0,-1 1-1,1 0 1,0 0 0,0-1 0,1 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,1-1 0,0 0 0,0 0-1,7 5 1,-8-7 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1-1-1,1 1 1,0-1-1,0 0 1,0 1-1,-1-1 1,1 0-1,0-1 1,0 1-1,0 0 0,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1-1 1,1 1-1,-1-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-2 1,0 1-1,0 0 1,1-3-1,4-5 29,0 0 1,-1 0-1,-1-1 0,1 0 0,4-17 0,-8 22-31,0 0-1,0 0 0,-1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,-2-1-1,1 1 0,0 0 1,-1 0-1,-2-8 0,-3 7-157,3 18-26,1 16 78,26 23 99,-21-45 3,0-1 1,0 2-1,-1-1 0,1 0 0,-1 0 0,0 1 0,-1-1 0,1 1 1,-1 0-1,0-1 0,0 9 0,-2-13 2,-1 0 1,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-3 0 1,-16 1-732,20-25-11333,0 15 6555</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2680.04">1489 372 2497,'0'0'9949,"1"-6"-8469,1-16 1,-1 17 149,-1 14-1376,0 23 40,2 58 254,-1-83-525,0 0 0,0 0 0,1 0 1,0 0-1,1 0 0,-1-1 0,1 1 0,1-1 0,-1 1 0,6 6 0,-9-12-12,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0 0 0,-1-1 0,1 1 0,0-1 0,-1 1-1,1 0 1,0-1 0,0 1 0,0-1 0,0 0 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,0 0 3,-1-1 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,0-1 0,15-61 185,-14 56-211,3-39-4,-2 55-14,0 0-1,0 0 1,0 0-1,1 0 1,0-1-1,0 1 1,1-1-1,0 0 1,0 0-1,1-1 1,6 7 0,-11-12 34,1 1 1,-1-1-1,1 0 1,-1 1 0,1-1-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1-1-1,0 1 1,0 0 0,-1-1-1,1 1 1,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,5-1-1,-4 0 22,1-1 0,-1 1 1,0-1-1,0 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,3-3 0,0-4 48,0 0 0,0 0-1,-1-1 1,-1 1 0,1-1-1,-2 1 1,1-15 0,-1 15-173,-1-13 378,0 23-330,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 1,-1-1-1,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 1,0 0-1,11 14-8337,12-9 3972,3 0-410</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3609.93">1953 369 1777,'0'0'11901,"-6"-9"-10348,-18-31-507,24 39-1026,-1 0 1,0 1-1,0-1 0,0 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 1-1,0 0 0,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,-2 2-1,-23 18 55,23-14-59,-1-1 1,1 1-1,0 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,1 1 0,-1-1 0,1 1 0,0-1 0,1 1 1,0 13-1,0-19-10,0 0-1,1-1 1,-1 1 0,0 0 0,1 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,0 0 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 0 0,0 1 0,0-1-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,-1 1 0,1 0 0,1-2-1,2 2 21,0-1-1,0-1 0,-1 1 0,1 0 1,-1-1-1,1 0 0,-1 1 1,0-1-1,6-5 0,-6 3 62,0 0 1,0-1-1,-1 1 0,1-1 0,-1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0-7 0,-1 11 36,0 27-406,1-20 287,-1 0-1,1 0 1,1-1 0,-1 1-1,1-1 1,0 1 0,4 9 0,-5-14 3,-1 1 1,1-1-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,-1-1-1,0 1 1,1-1-1,0 0 1,1-1 9,-2 0 0,1 0 1,0 0-1,0 0 0,-1 0 0,1-1 1,-1 1-1,1 0 0,-1-1 1,0 1-1,0-1 0,0 0 0,0 1 1,0-5-1,5-30-7,-5 35-82,-1 6 71,-1 3 0,1 0 0,0 0 0,1 0 0,0 0-1,0 0 1,0 0 0,3 7 0,-3-12 5,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,2 0 0,-1 1 0,0-1 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0-1 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 1,0-1-1,1-2 0,-1 2-13,0 0-1,0 0 1,0 0 0,1 1-1,-1-1 1,1 1-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 0 0,6-2-1,0 2 22,-1-2 0,0 1 0,0-1 0,0 0 1,-1 0-1,1-1 0,-1 0 0,0 0 0,0-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,0 0 0,0 0 0,0 0 1,2-8-1,-2 14 120,1 10-165,3 13-40,11 52 69,-4 1-1,-3 1 0,4 138 1,-16-207-1,0 1 0,-1 0 0,0 0 0,0-1 0,-1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-2 0 0,1 0 0,-1 0 0,-8 11 0,9-14 9,-1 0 1,0 0-1,0-1 1,-1 1 0,1-1-1,-1 0 1,0 0-1,1-1 1,-1 1-1,0-1 1,-1 0-1,1 0 1,0-1 0,0 1-1,-1-1 1,1 0-1,-1-1 1,1 1-1,-11-2 1,13 1 6,0 0-1,0-1 1,0 1 0,1-1 0,-1 0-1,0 1 1,0-1 0,0-1-1,1 1 1,-1 0 0,1-1 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1 0-1,0 0 1,-2-3 0,0 0 8,1 0 1,-1-1-1,1 0 1,0 0 0,1 0-1,0 0 1,0 0-1,-2-7 1,1-5-16,0 0 1,1 0 0,1 0 0,1 0-1,2-22 1,-1 34-94,0 1 0,1-1-1,0 0 1,0 0 0,0 1-1,0-1 1,1 1 0,0-1-1,0 1 1,1 0 0,-1 0-1,1 1 1,0-1 0,0 1-1,1 0 1,5-4 0,4-3-1741,1 0 0,1 2-1,0 0 1,18-7 0,4-1-7014</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4526.64">2684 315 4898,'0'0'10891,"-1"-8"-9744,-1 0-1009,-1-14 491,1 40-118,2 199 1348,0-217-1856,0 0-1,0 0 1,0 1 0,-1-1-1,1 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,-1 0 0,1 1-1,0-1 1,0 0-1,0 0 1,-1 1 0,1-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 1 0,-1-1-1,1 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,-11-6 41,11 5-62,0-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0-1,-1 1 1,1-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,0-1 0,-1 0 0,1 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,3-3 0,6-4-400,0-1-1,1 1 1,18-10-1,-14 9-158,4-3-108,40-30-1887,-57 39 2474,1 1 1,-1-1-1,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0-6 0,0-3-40,-3-26 1636,2 38-1391,0 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1 0,1-1-1,-1 0 1,0 0-1,0 1 1,1-1-1,-1 0 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,-2 0 1,2 1-94,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 1,1-1-1,-1 0 0,1 1 0,-1 0 0,1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 2 0,0-3 7,-1 164 1410,1-164-1417,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,0 1 1,1-1 0,-1 1-1,0-1 1,1 1 0,-1-1-1,1 1 1,-1-1 0,0 0-1,1 1 1,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,-1 1 0,2-1-1,20-7 235,23-27-138,-41 30-121,21-10-7,-24 14 16,0-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,-1 1 1,1-1-1,-1 0 0,1 1 1,0 0-1,1 1-11,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 5-1,-1-4 14,1-1 0,-1 0 0,1 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,0-2 0,-1 1 0,1 0 0,3 3 0,-4-5 5,1-1 0,0 1-1,-1 0 1,1 0-1,0-1 1,0 1 0,-1-1-1,1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,-1 0-1,1-1 1,0 1 0,0 0-1,0-1 1,0 1-1,-1-1 1,1 0 0,0 0-1,-1 1 1,1-1-1,0 0 1,-1 0 0,1-1-1,-1 1 1,0 0 0,1 0-1,-1-1 1,0 1-1,0-1 1,2-2 0,2-2-9,-1 1 1,0-1-1,0 0 1,0-1-1,-1 1 1,1-1-1,2-11 1,-5 14-20,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,-1 0 0,-1-8 0,2 11 15,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 1 1,-2 0-1,1 1 8,0-1-1,0 1 1,1-1 0,-1 1 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,1 0 1,-1 0 0,0 0 0,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1 0,0 0 0,0 3 0,0-2-222,0-1 0,-1 1 0,1 0 0,0-1 1,0 1-1,1 0 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0 0 0,0-1 1,0 0-1,0 1 0,0-1 0,1 0 1,-1 1-1,1-1 0,2 2 0,15 6-3886</inkml:trace>
@@ -12548,7 +12548,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2505.05">387 1649 1201,'0'0'5477,"0"-4"-1958,-1 7-915,-47 329-2036,44-304-207,-14 50 0,6-27-115,9-40-31,1-2-328,3-12-661,2-35-2726,-3 2-1190</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3136.6">369 1549 2113,'0'0'5090,"0"-2"-4588,-4-3-278,-4 11-178,-5 9-25,-1 6 75,-2 1 129,1 1 0,1 1 0,1 0 0,-9 27 1,20-48 871,3-5-449,4-13-282,15-25-426,-12 29 71,1 1 0,0 0 0,0 0 0,2 1 0,-1 1 0,1-1 0,0 2 0,0 0 0,19-9 0,-29 16 2,1-1 1,0 1 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 1 0,-1-1-1,1 0 1,-1 1 0,1-1 0,0 1-1,-1-1 1,1 1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0-1 0,-1 1-1,1 1 1,4 9 208,0 1-1,-1 0 1,2 18 0,1-4-102,-4-19-565,5 20 1222,-7-15-7088</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3910.72">2 1262 3522,'0'0'5333,"0"-9"-4832,0-21 82,0 27-306,0 5-45,0 23-96,0 23 75,-1-14-87,1-1 0,1 0 0,12 64 0,-12-95-94,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,2 1 1,0-1 7,0 1 1,0-1 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 1-1,0-1 1,4-1 0,4-2 5,-1-1 1,1 0-1,-1-1 1,11-7-1,-8 4-102,-1 1 0,1 0-1,19-9 1,0 11-4375,-25 6 178</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4309.77">303 1321 3282,'0'0'6573,"0"-8"-6226,-6 116 827,8-107-1158,1 0 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 1,4-1-1,-4-1 7,0 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,-1-1 1,1 0 0,-1 1-1,1-8 1,1-60 129,-3 51-134,0 20-42,0-1 0,0 1 0,0 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,-12 13-2068,11 0-441,1-2-971</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4309.76">303 1321 3282,'0'0'6573,"0"-8"-6226,-6 116 827,8-107-1158,1 0 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 1,4-1-1,-4-1 7,0 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,-1-1 1,1 0 0,-1 1-1,1-8 1,1-60 129,-3 51-134,0 20-42,0-1 0,0 1 0,0 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,-12 13-2068,11 0-441,1-2-971</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4451.33">290 1321 2289</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4650.57">290 1321 2289,'150'-31'2414,"-120"24"-1216,-31 8-1093,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,1 0 1,0 0-1,-1 1 1,1-1-1,0 0 1,-1 0-1,1 1 0,0-1 1,0 2-1,-3 32 391,2-19-310,1-13-154,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,1-1 1,-1 1-1,3 5 0,-2-7-24,0 1 0,0-1 0,0 0-1,0 0 1,1 0 0,-1-1 0,0 1 0,1 0-1,-1 0 1,0-1 0,1 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,2 0-1,-2-1 14,0 1-1,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1-1 0,1 1 0,0-1 0,-1 1 1,1-1-1,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 1,-1 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 1,-1 1-1,1-2 0,1-3 11,-1 1-1,0-1 1,0 1-1,0-1 1,-1 1-1,0-1 1,0 0-1,-2-12 1,1 18-21,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,-2-1 1,3 1-146,0 0 1,-1-1 0,1 1-1,-1 0 1,1 0-1,-1-1 1,1 1 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 1-1,1-1 1,0 0 0,-1 0-1,1 0 1,-1 1 0,1-1-1,0 0 1,-1 1-1,1-1 1,0 0 0,-1 1-1,1-1 1,0 0-1,-1 2 1,1 4-3203</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4898.57">584 1190 3298,'0'0'6122,"0"18"-5716,0 197 485,3-188-393,2-15-1689,5-9-5122,-4-6 3707</inkml:trace>
@@ -12564,7 +12564,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12349.75">3023 1656 4562,'36'-44'1745,"36"-36"3271,-73 82-4955,1 1 1,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,2 1 0,-1-1-1,0 1 1,1 2 0,0 4 21,-1 178 2232,0-186-1301,0-11 211,0-230-783,0 239-447,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0-1-1,1 1 1,-1 0 0,1 1 0,-1-1-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,2 0 0,-1 0-13,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 1,-1 0-1,1 0 0,1 2 0,6 10 111,-1 1 0,0 0 0,-1 0 1,0 0-1,-2 1 0,0 0 0,6 32 0,0 52-1798,-10-32-3991,-4-64 1149,-12-4-303</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12505.15">3119 1663 6195,'0'0'6259,"84"-97"-6259,-42 76-48,-6 1-993,-6 3-2240</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17110.88">6940 1359 1553,'0'0'9031,"0"-5"-6706,0 6-1001,2 29-1079,2 0 1,11 48-1,0 2 441,-14-78-675,21 147 1144,3 192 0,-7-227-349,-14-111-1100,-4-13-1458,-10-12-2733,-2-7-1139</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17440.19">6982 1435 2689,'0'0'5819,"-3"8"-5296,-35 66 603,42-95 214,-4 19-1338,0-1-1,0 1 0,0 0 0,0-1 1,1 1-1,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,0-1 0,0 1 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,0 1 0,-1-1 1,1 1-1,0 0 0,0 0 0,3-2 1,1 1-473,0 1 1,0-1 0,1 1 0,-1 0 0,0 1 0,0 0 0,8 0 0,-6 0-1260,11 0-1925</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17440.18">6982 1435 2689,'0'0'5819,"-3"8"-5296,-35 66 603,42-95 214,-4 19-1338,0-1-1,0 1 0,0 0 0,0-1 1,1 1-1,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,0-1 0,0 1 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,0 1 0,-1-1 1,1 1-1,0 0 0,0 0 0,3-2 1,1 1-473,0 1 1,0-1 0,1 1 0,-1 0 0,0 1 0,0 0 0,8 0 0,-6 0-1260,11 0-1925</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18025.94">7283 1435 2993,'0'0'8428,"0"13"-8041,0 147 5253,0-164-4976,0-14-555,1 1-1,1-1 1,1 1-1,0 0 0,1 0 1,8-21-1,-9 29-139,1 1 1,-1-1-1,2 1 0,-1 0 0,1 0 1,1 1-1,-1 0 0,1-1 0,0 2 1,1-1-1,0 1 0,0 0 0,13-8 0,-19 13 13,-1 0 0,1 1-1,0-1 1,-1 1 0,1-1 0,0 1-1,0-1 1,0 1 0,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 1-1,-1-1 1,1 0 0,0 1-1,0-1 1,-1 1 0,1 0-1,0-1 1,-1 1 0,1 0-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1 0 0,0 0 0,1 1-1,0 1-31,-1 1 1,1-1-1,-1 0 0,0 0 0,0 1 1,0-1-1,0 0 0,-1 0 0,1 1 1,-1-1-1,0 0 0,-1 5 0,-3 0-145,0 1 0,-1-1 0,0 0 1,0 0-1,-1 0 0,0-1 0,-1 0 0,1-1 0,-1 0 0,0 0 0,-16 9 0,23-15 483,25 0-267,-15 1 26,1 0 0,-1 1 0,0-1 0,0 2 0,14 5 0,11 2-1488,1-5-4902,-17-5 242</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18461.28">7667 1348 96,'0'0'12000,"0"11"-11231,0 229 807,-43-235-831,25-5-722,31-1-737,-2 1 605,0 0-1,-1-1 1,1-1 0,0 0 0,17-5 0,8-13-2154,-33 17 1672,0 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,3-6 0,-2-7-3699</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18574.41">7654 1348 7379</inkml:trace>
@@ -12677,7 +12677,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">25 137 1281,'0'0'1392,"-24"0"-2304</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="336.94">25 137 2945,'25'57'1521,"-20"-45"4562,4-11-5974,40 7 48,90 4 0,-45-5-161,-92-7-62,-1 0 1,1 0 0,-1 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,1 1-1,-1-1-156,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 1 0,0-1 0,1 0 1,-1 0-1,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 0,-1 0 1,1 0-1,0 1 0,-1-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,-1 1 0,-13 9-2565</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="599.82">92 412 3586,'0'0'5728,"-16"0"-5117,105-1-789,171-25 1,-219 22-3657,-38 4 963</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="599.81">92 412 3586,'0'0'5728,"-16"0"-5117,105-1-789,171-25 1,-219 22-3657,-38 4 963</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1078">139 38 5330,'0'0'7196,"-7"-6"-6473,-21-19-510,28 25-215,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,1 1 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0 0,12 1-25,-10-1 18,48 9-35,81 25 0,-31-7-276,-70-20 240,-3-2-64,-1 1 0,0 2 0,0 1-1,39 18 1,-63-25 139,-1-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0 4 0,-5 43 61,-2-22-4,-1 0 0,-2 0-1,-1-1 1,-1-1 0,-1 0-1,-19 28 1,17-29 29,-42 73 259,2-6 154,-82 184 1,130-260-641,2 0 0,0 1 0,1-1 0,1 1 0,0 0 0,0 25 0,2-40-25,1 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 0 1,0 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,1 0 1,25 0-3933</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1649.31">1159 319 4194,'0'0'7699,"-4"-6"-6917,-8-10-449,6 15-111,4 34-58,2-15-179,0 7 22,6 158 588,-3-155-959,1 0-1,2-1 0,0 0 0,16 41 1,1-7-5066,-21-45 1215</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1868.03">1128 576 560,'0'0'2668,"-6"-23"-760,-4-12-1214,-32-129 4084,41 158-4667,-1 1 0,1-1 1,1 1-1,-1-1 0,1 1 1,0-1-1,0 1 1,0-1-1,1 1 0,0 0 1,0-1-1,0 1 1,1-1-1,-1 1 0,2 0 1,-1 0-1,0 0 0,1 0 1,0 1-1,0-1 1,0 1-1,1-1 0,6-6 1,8-2-142,-1 0 1,2 0-1,0 2 1,0 0-1,1 2 1,0 0-1,1 1 0,0 1 1,0 1-1,0 1 1,1 1-1,0 0 1,39 0-1,-58 4-92,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 1-1,-1-1 1,0 1-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0-1,2 4 1,0 1-512,-1 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,-1 0-1,0 14 0,0 27-2732</inkml:trace>
@@ -12776,7 +12776,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">42 519 1617,'0'0'4677,"-2"-9"-4205,-1-4-327,1 8 56,1-1 1,0 1-1,0-1 1,0 1-1,1-1 1,-1-6-1,-1-6 2660,2 17-2800,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 1,-1 0-1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0-1 0,1 1 0,55-12-496,0 3 0,0 2-1,0 2 1,68 4-1,-124 1 314,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 1,1-1-1,-1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 0 1,-1 1-1,-9 16-2680</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="267.84">0 643 1265,'0'0'7987,"9"0"-7029,11-2-830,-1-2-1,1 0 1,-1 0-1,-1-2 1,26-10-1,28-9-108,-10 5 17,8-2-3455,-58 18 762,-5-2 8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="688.85">167 73 5202,'0'0'7897,"-10"-12"-7347,-30-36-459,40 48-93,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0-1 0,0 1 0,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0-1-1,1 1 1,-1 0 0,0 0 0,0-1 0,0 1-1,0 0 1,1 0 0,-1-1 0,0 1 0,0 0 0,1 0-1,11 1 4,-11-1-7,18 4 12,-1 0 0,0 1 0,0 1 0,-1 1 0,23 11 0,85 52 24,-118-65-32,24 13 23,-3-2-98,-2 0-1,0 2 1,29 25 0,-49-37 54,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1-1,-1 1 1,0 0 0,0 1 0,0-1 0,-1 1 0,0 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,0 11 0,0-8 21,-1-1 1,-1 1 0,1-1 0,-2 1 0,1 0-1,-2-1 1,1 0 0,-1 0 0,-1 0-1,0 0 1,-7 12 0,-27 45 36,-3 1 63,3 2 0,4 2 0,-31 89 0,61-145-550,1 0-1,1 1 1,0 0 0,1-1-1,1 18 1,0-31 331,2 10-3652,8-8-2242</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="688.84">167 73 5202,'0'0'7897,"-10"-12"-7347,-30-36-459,40 48-93,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0-1 0,0 1 0,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0-1-1,1 1 1,-1 0 0,0 0 0,0-1 0,0 1-1,0 0 1,1 0 0,-1-1 0,0 1 0,0 0 0,1 0-1,11 1 4,-11-1-7,18 4 12,-1 0 0,0 1 0,0 1 0,-1 1 0,23 11 0,85 52 24,-118-65-32,24 13 23,-3-2-98,-2 0-1,0 2 1,29 25 0,-49-37 54,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1-1,-1 1 1,0 0 0,0 1 0,0-1 0,-1 1 0,0 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,0 11 0,0-8 21,-1-1 1,-1 1 0,1-1 0,-2 1 0,1 0-1,-2-1 1,1 0 0,-1 0 0,-1 0-1,0 0 1,-7 12 0,-27 45 36,-3 1 63,3 2 0,4 2 0,-31 89 0,61-145-550,1 0-1,1 1 1,0 0 0,1-1-1,1 18 1,0-31 331,2 10-3652,8-8-2242</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -13017,15 +13017,15 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">101 290 9652,'0'0'6777,"-16"14"-5793,-46 51-55,59-61-876,1-1 0,0 0 1,0 0-1,0 1 0,0 0 0,0-1 1,1 1-1,-1 0 0,1 0 1,0-1-1,0 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,1 7 0,0 7 15,0-16-64,-1 0-1,1 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,0 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,4-1 1,-1 2-2,1-1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 0 1,-1-1-1,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 1,4-4-1,-3 0-75,-1 0 0,1 0-1,-1 0 1,-1-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,0 1 0,-3-13 0,3 19 103,0 0 1,-1 0 0,1-1-1,-1 1 1,0 1-1,1-1 1,-1 0 0,0 0-1,0 1 1,0-1 0,0 1-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 1 0,-1-1-1,1 1 1,-1-1 0,1 1-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,1 1 0,-3 0-1,4 0-23,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0 1 0,3 31-14,-1-31-14,0 0 0,-1-1 0,1 1 0,0-1 1,1 1-1,-1-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 1,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,5-1 0,-3 1-36,0 0 0,1-1 0,-1 0-1,1 0 1,-1 0 0,1-1 0,-1 0 0,0 0 0,1 0-1,-1-1 1,0 0 0,9-4 0,-7 1 9,0 0 0,-1 0 0,1-1 1,-1 0-1,0-1 0,-1 1 0,0-1 1,0 0-1,0 0 0,-1-1 0,0 0 0,0 1 1,-1-1-1,0 0 0,0-1 0,2-14 0,0-10 246,-1 0 0,-2 0 0,-1-34 0,-2 44 148,-3-3 138,0 17-97,2 14 71,-22 623 907,24-608-1356,0 10 16,2-1 0,6 39 0,-7-59-7,1-1 0,0 1-1,0-1 1,1 0-1,0 0 1,1 0-1,0 0 1,0 0 0,1-1-1,-1 0 1,2 0-1,9 11 1,-14-17-19,1 0 1,-1 1-1,1-1 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1 0 0,1-1 1,-1 0-1,2-2 0,5-6-10,0 0-1,-1 0 0,-1 0 0,0-1 1,6-13-1,-4 4-106,0-1 0,-1 0 0,-1-1 1,-1 1-1,-1-1 0,-1 0 0,-1 0 0,-1 0 0,0 0 0,-4-25 0,2 43 112,1 0 0,-1 0 0,0 1 0,0-1 0,-1 0 0,1 1-1,-1-1 1,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,0 1 0,0-1 0,0 1 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 1 0,0 0 0,1-1-1,-1 1 1,-6 0 0,-6-2 136,-1 1 0,0 1-1,0 0 1,0 1 0,-18 3 0,-2 9 247,37-12-378,-1 1 0,0-1 0,1 0-1,-1 0 1,0 1 0,1-1-1,-1 0 1,1 1 0,-1-1-1,0 1 1,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,0 1 1,-1-1 0,1 1 0,-1-1-1,1 1 1,0 0 0,0-1-1,-1 1 1,1 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1 0,2 1-6,0 0 0,0-1 0,-1 0 0,1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 0 0,0 1 0,6-1 0,46-3 98,-45 2-95,1 0-26,0-1-1,0-1 1,0 0-1,0-1 1,0 0-1,0 0 1,-1-1-1,0-1 1,12-7-1,24-18-2733,-22 14-503,1 0-3149</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="635.35">915 187 9060,'0'0'8802,"0"7"-8629,5 266 2183,-5-272-2295,0-15 259,-5-324-8,5 330-308,0 0 0,1 0-1,0 0 1,0 0-1,1 0 1,0 0 0,4-8-1,-5 14-8,0 0 0,-1 0 0,1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,3 0 0,-4 0 0,0 0 1,0 1 0,0-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0 0 0,-1-1 0,1 1-1,0 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 2 1,3 32-10,-3-30 13,0 0 1,0 12 2,0 1 0,-1 0 0,0-1 1,-2 1-1,0-1 0,-8 27 1,7-33-39,0 0 1,1 0 0,0 0 0,1 1 0,0-1 0,0 16 0,4-25-8,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,4 1-1,4 2-85,-8-3 84,-1 1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1 0,-1-1 0,0 1-1,0-1 1,4 4 0,-6-4 70,1-1 1,-1 1-1,0 0 1,1-1-1,-1 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 1,0-1-1,0 1 1,0-1-1,-1 1 1,1 0-1,-2 2 115,-1 0 1,1-1-1,0 0 0,-1 1 1,1-1-1,-1 0 0,0-1 1,1 1-1,-1 0 0,0-1 1,0 1-1,0-1 0,-1 0 0,-4 1 1,-22 9 311,21-8-678,0 1 0,0-1-1,0-1 1,-1 0 0,-10 1 0,43-8-13038</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="635.34">915 187 9060,'0'0'8802,"0"7"-8629,5 266 2183,-5-272-2295,0-15 259,-5-324-8,5 330-308,0 0 0,1 0-1,0 0 1,0 0-1,1 0 1,0 0 0,4-8-1,-5 14-8,0 0 0,-1 0 0,1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,3 0 0,-4 0 0,0 0 1,0 1 0,0-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0 0 0,-1-1 0,1 1-1,0 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 2 1,3 32-10,-3-30 13,0 0 1,0 12 2,0 1 0,-1 0 0,0-1 1,-2 1-1,0-1 0,-8 27 1,7-33-39,0 0 1,1 0 0,0 0 0,1 1 0,0-1 0,0 16 0,4-25-8,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,4 1-1,4 2-85,-8-3 84,-1 1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1 0,-1-1 0,0 1-1,0-1 1,4 4 0,-6-4 70,1-1 1,-1 1-1,0 0 1,1-1-1,-1 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 1,0-1-1,0 1 1,0-1-1,-1 1 1,1 0-1,-2 2 115,-1 0 1,1-1-1,0 0 0,-1 1 1,1-1-1,-1 0 0,0-1 1,1 1-1,-1 0 0,0-1 1,0 1-1,0-1 0,-1 0 0,-4 1 1,-22 9 311,21-8-678,0 1 0,0-1-1,0-1 1,-1 0 0,-10 1 0,43-8-13038</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="980.23">1173 286 8996,'0'0'9058,"0"10"-8509,-1 9-283,0-6-172,1 0 0,0 0 0,0-1-1,1 1 1,1 0 0,0-1 0,6 19 0,-7-29-91,0-1 1,0 1 0,0-1-1,1 1 1,-1-1-1,0 0 1,1 1 0,-1-1-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0-1-1,-1 1 1,1 0-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0 0,0 1-1,0-1 1,0-1 0,0 1-1,0 0 1,-1 0-1,1-1 1,2 0 0,1 0 14,-1 0 0,0 0 0,1 0 0,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,5-6 0,-4 2 107,-1 0-1,1-1 1,-1 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,-1 0-1,1-1 1,-2 1 0,1-1-1,-1 1 1,0-1 0,-1 1-1,1-1 1,-1 0 0,-1 0 0,-2-12-1,3 20-153,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 1 0,0-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1-1-1,0 1 1,-1 0 0,1-1-1,0 1 1,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0-1,-1 0 1,1 0 0,-2-1-1,2 2-127,-1-1 0,1 0 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1 0-1,1-1 1,0 1 0,0-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,1 0-1,-1 14-4041,0-3-865</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1261.76">1358 320 2481,'0'0'9639,"17"9"-8337,53 29-416,-67-37-809,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 1-1,-1-1 1,1 1 0,0-1-1,-1 1 1,0-1 0,0 1-1,0 0 1,0 0 0,0-1-1,0 1 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,-2 5-1,1 8 414,1-16-456,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 0 1,-8-12 1142,3-1-1044,2 0 0,0-1 0,1 1 1,0-1-1,1 0 0,0 1 0,1-1 0,4-26 1,-4 38-207,1 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 1 0,1-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,0 1 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 1 0,1-1-1,-1 1 1,0-1 0,5 1-1,66-1-8023,-53 1 3584,2 0-1175</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2109.99">1701 267 1121,'0'0'15089,"-18"5"-13763,-57 18-318,71-22-945,0 1 0,0 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 1 1,1 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1 1-1,0-1 1,-1 1-1,2 0 1,-3 5-1,1 0-62,1 0 0,1 0 0,-1 0 0,1 0 0,1 17 0,0-23-14,0-2-8,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,1-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 1,0 1-1,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,1-1 0,-1 0 1,0 1-1,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 1 1,2-1-1,22-1-383,19-16-285,35-46 198,-78 63 496,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 1 0,1 0 28,9 31 115,-2 0 0,0 1 0,-3 0 0,0 0 0,-2 0 0,-2 1 0,-1-1 0,-5 34 0,4-58-110,0-1 0,-1 1 0,-1-1 0,1 0 0,-2 0-1,1 0 1,-8 13 0,10-19-7,0 0 1,0 1-1,-1-1 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,0-1-1,0 1 0,0 0 0,0-1 1,-1 0-1,1 1 0,0-1 0,-1 0 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1 0 0,-1-1 0,1 0 1,-1 0-1,1 1 0,-1-1 0,0-1 1,1 1-1,-4-1 0,5-1 11,0 0 1,0 0-1,0 0 0,0-1 0,1 1 1,-1 0-1,1 0 0,-1-1 0,1 1 1,0 0-1,0-1 0,0 1 0,1-4 0,-1 4-12,0-9-20,1 1 0,0 0 0,1 0 0,0 0 0,1 0 0,-1 1 0,2-1-1,0 1 1,0 0 0,6-10 0,8-9-255,38-46 0,-40 57 170,-1-2 0,-1 0-1,-1 0 1,-1-1 0,15-32 0,-27 51 84,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 1 0,-1-1 1,0 1-1,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,0 0 0,1 0 0,-3-2 0,-1 1 3,0 1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1-1,0 1 1,0 0 0,-6 1 0,1-1-20,7 0 13,0 0-1,1 1 1,-1-1-1,0 1 0,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,1 0-1,-1 2 0,-5 51-155,9-54 156,0 0-1,0-1 1,0 1-1,0 0 1,0-1 0,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,3-1-1,-5 1-1,7-2 19,0 0 0,0-1-1,0 0 1,0-1 0,0 1 0,-1-2-1,1 1 1,-1-1 0,0 0 0,7-7-1,29-17 83,-43 29-83,0 0 1,1 0-1,-1-1 0,0 1 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 1 0,-1-1 1,0 0-1,1 0 0,-1 0 0,0 0 1,1 0-1,-1 1 0,0-1 1,0 0-1,1 0 0,-1 0 0,0 1 1,1-1-1,-1 0 0,0 0 1,0 1-1,0-1 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 1 1,5 19 189,-4-16-32,2 9 36,-1-3 25,0-1 1,1 1-1,0 0 1,8 15-1,-10-23-210,0-1 0,-1 1 0,1-1 0,0 1 1,1-1-1,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 1,-1-1-1,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 1,0 0-1,2-2 0,12-5-84,-1 0 0,1-2-1,-1 0 1,-1 0 0,20-17 0,-23 17-1409,-1-1 0,1 0 0,16-21 0,-13 11-6542</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3083.34">2676 578 1713,'0'0'10287,"5"0"-9596,-1 0-593,0-1 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1-1 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1-1,-1 1 1,0-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0-4 0,4-28 1107,-2-1 0,-1-37 0,-2 70-572,-1 48-595,0-20-6,0 1 1,6 37-1,-5-56-35,2 1-1,-1-1 0,1 0 1,0 0-1,0 1 1,0-1-1,1-1 1,0 1-1,0 0 1,1-1-1,-1 1 1,1-1-1,1 0 1,6 6-1,-10-9 14,0-1-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0 0 0,-1-1 1,1 1-1,0-1 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 0,0 1 1,-1-1-1,1 1 0,0-1 1,-1 0-1,3-1 0,2-3 23,0 1-1,0-1 0,0-1 0,-1 1 0,6-9 1,-5 7-51,1 2 113,-1-1-542</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3739.52">2932 203 1361,'0'0'15481,"-3"-14"-14261,-12-44-401,15 57-806,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 0 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 1 0,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,1 0 1,-3 1-1,1 0-3,0 0-1,0 1 1,0-1 0,0 0-1,1 1 1,-1-1 0,0 1-1,1 0 1,-1 0-1,1 0 1,-1-1 0,0 4-1,-7 15 49,2 1 0,0 0-1,2 0 1,0 0 0,-3 40 0,5 113 479,3-111-426,1-40-230,0 1 0,2-1 0,0 0-1,1 0 1,2 0 0,15 40-1,-16-43-1653,-5-12-3126</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4013.53">2781 640 7075,'0'0'9863,"4"-15"-9334,-1 6-499,-3 4-32,1 1 1,0-1 0,1 0-1,-1 1 1,1-1-1,0 1 1,0-1-1,0 1 1,1 0 0,0 0-1,-1 0 1,1 0-1,1 1 1,-1-1-1,0 1 1,1 0-1,0-1 1,0 2 0,0-1-1,4-2 1,116-37-413,-86 31-748,66-29 0,-102 39 1164,-1 0 0,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,0-1 1,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0 0,-1-1-1,1 1 1,-1-4-1,0-9 524,1 15-740,-1 0 0,1-1 1,-1 1-1,0 0 0,1-1 1,-1 1-1,1 0 0,-1-1 1,0 1-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,-1 1 0,-2-1-3143,-1 0-754</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4541.98">3095 384 6659,'0'0'8289,"-6"17"-6984,6-17-1304,-8 22 460,2 1-1,0 0 1,1 1 0,-3 44 0,8-66-455,0-1 1,-1 1-1,1-1 1,0 0-1,1 1 1,-1-1 0,0 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 1 1,1 0-1,-1-1 13,1-1-1,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0-1 0,0 1 1,3-1-1,-1-1 10,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,-1-1 0,1 0-1,-1 0 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,-1-1-1,0 0 1,0 0 0,0 0-1,0-1 1,-1 1-1,1 0 1,-1 0 0,1-8-1,-1 7-21,1-1 0,-2 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1 1-1,-1-1 1,0 0 0,-1 1 0,1-1 0,-1 1 0,-4-6 0,-5 0-225,10 10 6,0 0-1,1-1 1,-1 1 0,0-1-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1-2-1,10 3-2478,18 3 2514,-20 0 178,1 1 1,-1 0 0,1 0 0,-1 1-1,0-1 1,0 1 0,0 1-1,-1-1 1,0 1 0,5 5 0,47 58 292,-52-61-223,4 4 200,-1 1 0,-1 0 1,0 0-1,0 1 0,5 14 1,-12-32 4949,-1-34-4451,-2 21-705,1 0-1,0 0 1,2 0 0,0 0-1,1 0 1,1 1 0,6-29-1,-7 41-183,1-1-1,-1 1 1,1-1-1,1 1 1,-1 0-1,0 0 1,1 0-1,0 0 1,1 0-1,-1 1 1,1-1-1,0 1 1,0 0-1,0 0 0,0 0 1,1 1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,1 1 1,-1 1-1,1-1 1,-1 1-1,11-1 1,46 1-7286,-37 1 592</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4821.48">3845 237 10165,'0'0'11151,"-4"-5"-10534,4 4-605,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,1-1 1,-1 1-1,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,-1 0 0,0 27 232,1 2-104,-12 117 801,1-13-1406,9-46-3007,5-73-1877,10-9-3693</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4541.97">3095 384 6659,'0'0'8289,"-6"17"-6984,6-17-1304,-8 22 460,2 1-1,0 0 1,1 1 0,-3 44 0,8-66-455,0-1 1,-1 1-1,1-1 1,0 0-1,1 1 1,-1-1 0,0 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 1 1,1 0-1,-1-1 13,1-1-1,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0-1 0,0 1 1,3-1-1,-1-1 10,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,-1-1 0,1 0-1,-1 0 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,-1-1-1,0 0 1,0 0 0,0 0-1,0-1 1,-1 1-1,1 0 1,-1 0 0,1-8-1,-1 7-21,1-1 0,-2 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1 1-1,-1-1 1,0 0 0,-1 1 0,1-1 0,-1 1 0,-4-6 0,-5 0-225,10 10 6,0 0-1,1-1 1,-1 1 0,0-1-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1-2-1,10 3-2478,18 3 2514,-20 0 178,1 1 1,-1 0 0,1 0 0,-1 1-1,0-1 1,0 1 0,0 1-1,-1-1 1,0 1 0,5 5 0,47 58 292,-52-61-223,4 4 200,-1 1 0,-1 0 1,0 0-1,0 1 0,5 14 1,-12-32 4949,-1-34-4451,-2 21-705,1 0-1,0 0 1,2 0 0,0 0-1,1 0 1,1 1 0,6-29-1,-7 41-183,1-1-1,-1 1 1,1-1-1,1 1 1,-1 0-1,0 0 1,1 0-1,0 0 1,1 0-1,-1 1 1,1-1-1,0 1 1,0 0-1,0 0 0,0 0 1,1 1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,1 1 1,-1 1-1,1-1 1,-1 1-1,11-1 1,46 1-7286,-37 1 592</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4821.47">3845 237 10165,'0'0'11151,"-4"-5"-10534,4 4-605,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,1-1 1,-1 1-1,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,-1 0 0,0 27 232,1 2-104,-12 117 801,1-13-1406,9-46-3007,5-73-1877,10-9-3693</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5197.39">4049 290 12502,'0'0'8273,"-13"9"-8065,-43 40-389,-79 87-1,136-167-701,1 27 914,-1-1 0,1 0 0,0 1 0,1-1 0,-1 1 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,1 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,7-1 0,-10 3-25,0-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 0,0 1 0,0-1 1,-1 1-1,1-1 0,1 3 0,19 47 104,-8-21-132,-12-27-144,1 0 1,0 1 0,1-1 0,-1 0-1,1 0 1,-1 0 0,1-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 0-1,1 0 1,4 2 0,-3-2-909,1-1-1,-1 0 1,0 0 0,1 0 0,0 0-1,-1-1 1,1 0 0,-1 0 0,8-2-1,11-2-4742</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5883.02">4243 389 3666,'0'0'11640,"-4"-11"-10234,-14-34-609,17 45-784,1-1 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1-1,0 1 1,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0-1,-1 1 1,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-21 25 168,20-24-156,-5 10-8,0 1-1,0 0 1,1 0-1,1 1 1,0-1-1,1 1 1,1 0-1,0 0 1,1 0-1,0 26 1,1-40-23,1 1 1,-1 0-1,0-1 0,0 1 1,1 0-1,-1-1 1,0 1-1,0-1 0,1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 0,-1 0 1,1 1-1,-1-1 1,1 1-1,-1-1 0,1 0 1,-1 1-1,1-1 1,-1 0-1,1 1 0,0-1 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 1 1,0-1-1,-1 0 1,1 0-1,0 0 0,-1-1 1,1 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 0,-1-1 1,1 0-1,33-18-317,-24 9 207,-1-1-1,1 0 1,-2-1-1,0 0 1,0-1-1,-1 1 1,0-1-1,7-22 1,-15 53 220,1 1 0,0-1 0,2 1 0,3 19 0,-5-37-104,0-1 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,1 1-1,-1-1 1,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1-1,1-1 1,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0-1,1 1 1,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,2 1-1,17-17 81,11-34-16,-26 40-53,2-2 3,-2 1 1,1-1 0,-1 0-1,-1 0 1,0 0 0,-1-1-1,1-20 1,-3 33-133,10 33-943,-6-23 1230,0 0 1,1 0-1,0-1 1,0 1-1,1-1 1,1-1-1,-1 1 1,15 13 0,-18-21-206,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,6-1 0,15-1-7465,-14 0 1618</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6810.52">4537 354 4322,'0'0'12443,"0"-7"-11811,0 138 1433,0-131-2064,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,1 0 0,-1 1-1,0-1 1,0 1 0,1-1-1,-1 0 1,0 1 0,1-1-1,-1 0 1,0 1 0,1-1-1,-1 0 1,0 1 0,1-1-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 1 0,-1-1-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1-1 0,23-25 40,-7-4-24,-6 10 38,0 0 1,24-30 0,-35 50-43,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,5 15 160,-2 15-80,-3-24-120,0 0-1,0 0 0,1-1 1,-1 1-1,1 0 0,1-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,5 8 0,-6-11-120,1 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,1-1-1,-1 1 0,1-1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,0-1-1,1 1 0,3-3 0,2 0-209,-1 0-1,1-1 1,-1 0-1,1-1 1,-2 0-1,1 0 1,0 0-1,-1-1 0,0 0 1,0 0-1,-1 0 1,9-13-1,-11 14 727,1 0-1,-1 0 0,-1 0 0,1-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,-1 0 0,0 0 1,1-8 1280,-9 15-170,4 0-1429,-1 1 1,0-1 0,1 1-1,0 0 1,-1 0 0,1 0 0,0 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,1 0 0,-1 0 0,-2 5-1,-26 48 113,30-55-204,1-1 1,0 0-1,-1 1 1,1-1-1,0 0 0,0 1 1,0-1-1,-1 1 1,1-1-1,0 0 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 1 1,0-1-1,0 1 1,1-1-1,-1 0 1,0 1-1,1-1 1,14-4-590,17-19-703,39-39-3233,-72 75 7705,1-6-3004,1 0 0,0 0 0,-1 0 0,2 0 1,3 13-1,-3-17-126,-1-1 0,1 1 1,0-1-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,4 0-1,-3-1 23,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,0 0 0,-1 0 0,5-4 0,1-1 91,0 0-1,-1 0 0,0-1 1,-1-1-1,1 1 1,-1-1-1,-1 0 0,0-1 1,0 1-1,5-14 1,-6 4 67,-1-1 1,0 1 0,-2-1-1,0 0 1,-1 0 0,-3-36-1,1 9 122,-5 30 572,6 17-871,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 1-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,0-1-1,0 1 1,-5 11-8,1 1 0,0-1-1,1 1 1,0 0 0,1 0 0,-1 16 0,2 87 11,1-72-53,-1-1-249,0-23-1117,1 0 1,3 32 0,0-43-2586</inkml:trace>
@@ -13061,7 +13061,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1481.47">980 291 6243,'0'0'9087,"16"-10"-8434,52-33-218,-63 40-391,-1-1-1,1 0 1,-1 0-1,0 0 0,0 0 1,0-1-1,-1 0 1,0 1-1,0-1 1,0 0-1,0-1 1,-1 1-1,0 0 1,0-1-1,2-8 0,-2-1 94,0 0 0,-1 0 0,-1 0 0,-2-18 0,1-2 412,-7 12 252,0 20-221,-1 15-400,1 12-107,0 0 0,2 0 0,1 1 0,1 0 0,-1 34 0,5 135 114,3-89-87,-3 227 842,0-337-928,6-231 218,-2 195-234,2 1 0,1-1 0,23-69 0,-29 106-5,0 1 0,0-1 0,0 0 0,1 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0 0 1,1 0-1,-1 1 0,1-1 0,-1 1 0,1 0 0,0 0 1,-1 0-1,1 0 0,7 0 0,-9 1-2,-1 0 1,1 1-1,-1 0 0,1-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1-1 1,0 1-1,0 0 0,1 2 0,2 58-94,-3-54 79,0-2-7,-1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0-1 1,0 1-1,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1-1 0,0 1 0,-4 4 0,5-6 14,1-1 0,-1 1 1,0-1-1,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 1,1-1-1,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,1 0 1,-1-1-1,1 0 0,-1 1 0,0-1 0,1 0 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1 1 0,-5-3 0,-7-8 46,5 4 34,21 24-8,-6-11-52,0 0 0,0 0 0,1-1 0,0 1 0,0-1 1,1-1-1,0 1 0,-1-1 0,1 0 0,1 0 0,-1 0 0,0-1 0,13 4 0,-15-6 4,0 0 0,0 0-1,1 0 1,-1-1 0,1 0-1,-1 0 1,0 0-1,1-1 1,-1 1 0,0-1-1,1 0 1,-1 0 0,0 0-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1-1 1,1 1-1,-1-1 1,6-6 0,-3 2 17,-1 0 1,0 0-1,0 0 1,-1 0-1,0-1 1,0 0-1,-1 0 1,0 0-1,0 0 0,-1 0 1,0-1-1,0 1 1,0-17-1,13-47-102,-14 71 60,0 0 1,0 0-1,0 0 0,0 0 1,-1 1-1,2-1 0,-1 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,1 1 1,-1-1-1,0 1 0,1 0 1,-1 0-1,0-1 0,0 1 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 1 0,0-1 1,0 0-1,3 2 0,37 15-38,-35-13 37,-1 0-1,0 1 0,0-1 0,0 1 1,-1 0-1,1 0 0,-1 0 1,-1 1-1,1-1 0,-1 1 1,3 6-1,22 70 45,-22-62 18,-6-18-39,0 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,4 1 0,-4-2 4,1 0-1,-1 0 1,1 0 0,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,0 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,2-3 0,5-6 33,0-1 1,0 0 0,-1-1 0,6-14-1,-7 13-36,0-2 0,-1 1 1,0-1-1,-1 1 0,-1-1 0,0 0 0,-1 0 0,0-26 0,-2 40 85,0 4-196,-2 45 37,1-22 120,0 0 1,5 37-1,-3-62-86,-1 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 1,0 0-1,-1-1 0,1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,-1 0 0,1-1 1,0 1-1,0-1 0,1 0 1,2-1-541,0 1 0,0-1 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 0-1,-1 0 1,4-4 0,13-25-7025</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1632.41">1792 154 4082,'0'0'11429,"-15"13"-13222,15 10-816,5-1-1249</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1885.66">1899 310 5651,'0'0'14934,"-112"106"-14245,107-78-257,5 0-288,0-6-96,0 0-48,0-5-64,10-8 0,9-7-576,6-2-641,9-5-1264,0-18-3074,-5-4-3121</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2225.26">1886 323 9716,'114'47'1900,"-91"-38"3340,-2-15-4106,-17 2-1042,-1 0 0,1 1 0,-1-1 1,1-1-1,-1 1 0,0 0 1,-1-1-1,1 1 0,-1-1 0,3-8 1,-4 12-72,-1-1 1,0 1-1,0 0 0,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-2-2 1,0 2 11,1 0 1,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,-2 1 0,2-1-14,-1 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0 1 1,-26 58 212,26-57-192,-4 11 12,1 0 0,0 0 0,1 1 0,1-1 0,1 1-1,0 0 1,1 0 0,1 0 0,1 0 0,2 20 0,-2-36-55,-1 0 1,1 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1-1 0,0 1 0,3-1-1,2 0-13,0-1 0,1 0-1,-1 0 1,0 0 0,0-1-1,8-5 1,11-9-599,0-2-1,28-27 1,6-19-5763,-37 28-751</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2225.25">1886 323 9716,'114'47'1900,"-91"-38"3340,-2-15-4106,-17 2-1042,-1 0 0,1 1 0,-1-1 1,1-1-1,-1 1 0,0 0 1,-1-1-1,1 1 0,-1-1 0,3-8 1,-4 12-72,-1-1 1,0 1-1,0 0 0,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-2-2 1,0 2 11,1 0 1,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,-2 1 0,2-1-14,-1 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0 1 1,-26 58 212,26-57-192,-4 11 12,1 0 0,0 0 0,1 1 0,1-1 0,1 1-1,0 0 1,1 0 0,1 0 0,1 0 0,2 20 0,-2-36-55,-1 0 1,1 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1-1 0,0 1 0,3-1-1,2 0-13,0-1 0,1 0-1,-1 0 1,0 0 0,0-1-1,8-5 1,11-9-599,0-2-1,28-27 1,6-19-5763,-37 28-751</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -13123,7 +13123,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">0 168 8996,'0'0'9012,"0"-5"-7985,1-10-58,1 33-399,6 30-487,5 5 125,-7-23-175,1-1 1,2 0-1,0 0 0,2-1 0,2-1 0,15 28 1,-27-54-36,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,1-1 0,0 0 6,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,2-4-1,20-57 166,-20 54-171,8-32 41,-1 0 0,-2 0 0,-2-1 0,3-74 0,-9 113-250,1-25 709,-1 27-558,1 0-1,-1 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,0 0 0,0 1-1,1-1 1,-1 0 0,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 1 1,0-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0-1,0 0 1,1 0-1,-1 0 1,0-1 0,1 1-1,-1 0 1,0 0 0,0 0-1,0-1 1,1 1-1,-1 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,1 1 1,-1 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0-1 0,12 19-4322,-1 9-253</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="702.02">366 351 8404,'0'0'4543,"15"-9"-3972,49-30 8,-60 36-490,0 1 0,0-1 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,4-6 0,-5 8 15,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,-1 0 1,1 0-1,0-1 0,0 1 0,-1 0 0,1 0 0,-1 0 1,0 0-1,-1-3 0,1 4-77,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 1-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,0 1-1,-1-1 1,-1 1-1,1-1-7,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,0 0 0,0 1 0,0 0 0,-3 2 0,1 7 31,-1-1 0,1 0-1,1 1 1,0 0 0,1-1 0,0 1 0,0 0 0,1 0 0,1 0 0,0 1 0,1 11 0,-1-4-38,0-16-43,0-1 0,0 1 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,0-1-1,1 1 0,-1 0 0,0-1 0,1 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,1-1 0,-1 1 0,1-1 0,0 0 0,-1 0 1,1 1-1,0-2 0,0 1 0,0 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,0 0 0,4 0 0,2 0-642,-1-1 1,1 0-1,0 0 0,0-1 0,-1 0 0,0-1 0,1 1 1,-1-2-1,0 1 0,0-1 0,14-10 0,-15 9-85,0-1 0,0 0 0,0 0 0,-1-1 0,0 0 0,-1 0-1,1 0 1,-1-1 0,-1 1 0,5-11 0,1-16 2642,-6-5 8568,-4 42-9887,-2 37 372,0-25-660,1 0 1,1 0-1,1 0 1,0 0 0,3 16-1,-4-30-274,0 0 1,1-1-1,-1 1 0,1 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,1 0 1,0-1-1,-1 1 0,1-1 1,0 1-1,-1-1 0,1 0 1,0 1-1,0-1 0,-1 0 1,1 1-1,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0-1 0,0 1 1,-1 0-1,1-1 0,0 1 1,0 0-1,-1-1 0,1 1 1,1-1-1,29-21 112,4-18-315,-28 30 147,1 1 1,0 0 0,0 0-1,1 0 1,17-12 0,-25 21 72,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,0 1-1,0-1 1,-1 0-1,1 0 1,0 1-1,0-1 1,-1 0 0,1 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,-1-1 1,1 1-1,-1-1 1,1 1-1,0 1 1,17 23 548,-12-16-410,-2-4-160,-1 1 0,1-1-1,0 0 1,1-1 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,8 4-1,-8-6-395,1 0 0,0-1 0,-1 0 0,1 1 0,0-2-1,0 1 1,9-1 0,-6 0-411,0 1-429,0-2 0,-1 1 0,1-1 0,14-3 0,7-10-4148</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1697.88">1168 254 3522,'0'0'11194,"-12"8"-10185,-38 30-233,47-36-725,1 1 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,1 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,1-1 0,0 1 1,0-1-1,0 1 0,1 7 0,-1 2-65,3-12 26,0 0 1,-1 0 0,1-1-1,-1 1 1,1-1-1,0 1 1,-1-1 0,1 0-1,0 0 1,-1 0 0,1-1-1,0 1 1,-1-1 0,5-1-1,-1-1-43,-1 0 0,0 0-1,0-1 1,-1 1 0,1-2 0,-1 1-1,0 0 1,0-1 0,0 1-1,0-1 1,-1 0 0,0-1 0,0 1-1,0 0 1,-1-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,2-7 0,1-16-3,-1 1 1,-1-55 0,-2 66 74,0-48 1672,-14 140-6,14-61-1591,-3 21 9,2 0 0,6 69 0,-4-100-186,0-1-1,0 0 1,1 0-1,-1 1 1,1-1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 0-1,4-1 1,1 1-440,0 0 0,-1-1 0,1 1 0,-1-2 0,1 1 0,-1-1 0,1 0-1,-1-1 1,0 1 0,0-2 0,0 1 0,-1-1 0,10-6 0,-13 7 249,0 0 0,1 0-1,-1-1 1,0 0 0,-1 1-1,1-1 1,-1 0 0,0 0-1,0-1 1,0 1-1,0 0 1,1-7 0,-1-1 874,0 0 1,-1-1 0,-1-17 0,1 30-494,-1 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0 0,-8 10 1339,-6 22-1009,15-32-450,-4 14 113,0 0 1,1 1 0,1-1-1,1 0 1,0 1 0,1 28-1,1-42-124,-1 1 0,0-1 1,0 0-1,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 1,0 0-1,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 0,0 0 0,1 0 0,-1-1 0,0 1 1,1 0-1,-1 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 1,0 0-1,3-1 4,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,-1 1 0,1-1 1,0 0-1,-1 0 0,0-1 0,1 1 0,2-5 0,-3 2 22,0 0 0,0 1 0,-1-1-1,0 0 1,0 0 0,-1 0 0,1-1 0,-1 1-1,-1 0 1,1-1 0,-1 1 0,0 0 0,-1-9 0,0 13-9,0 0 1,1-1-1,-1 1 1,0 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 1-1,-1-1 1,0 0 0,0 1-1,0-1 1,0 1-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 1-1,-1-1 1,1 1-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1 0-1,1 1 1,0-1-1,-6 2 1,7-2-83,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 0 0,-1 0 1,1 1-1,0-1 0,0 2 0,2-2-100,0-1 1,-1 1-1,1-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0-1 0,2 1 0,0 0 78,12 0 104,-5-1-28,0 1-1,1 0 0,-1 1 0,0 1 1,22 5-1,-29-6 59,0 1 1,-1 0-1,1 0 1,0 0-1,-1 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,0 0-1,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,0 0-1,-1 0 1,1 0-1,1 6 1,1 1 330,-1 0 0,-1 0 0,0 0 1,1 17-1,-3-23-214,1-1 0,-1 0-1,-1 0 1,1 0 0,0 1 0,-1-1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,-1 0 0,0 0 0,-3 4-1,4-7 341,1-7 498,1-23-916,1 1-1,1-1 0,2 1 0,1 0 0,1 0 0,19-49 0,-18 58-176,1-1 0,1 2 0,1-1-1,0 1 1,1 1 0,1 0 0,1 1 0,0 0 0,32-26 0,-46 42 57,1-1-1,-1 1 1,0-1-1,0 1 1,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,1 0-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,0 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,0 1-1,1-1 1,-1 0-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,-2 32-4170,-6-10-1155</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2222.72">1909 90 11397,'0'0'7601,"9"-14"-7380,32-41-197,-39 53-24,1 0 0,-1 0-1,1 0 1,0 0 0,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 2 0,1-1-1,-1 0 1,0 0 0,1 1-1,5 0 1,-8 0-7,1-1 0,0 1 1,-1 0-1,1 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 1,1 1-1,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,0-1 0,0 0 0,1 1 0,0 1 0,0 10 25,0 0 0,-1 0 0,-1 1-1,0-1 1,-1 0 0,0 0-1,-1 1 1,0-1 0,-1 0-1,-6 16 1,-17 33 804,19-50-599,1 0-1,1 1 1,0 0-1,1 0 0,0 0 1,0 1-1,2-1 0,0 1 1,0 0-1,1 19 0,35-33-5525,-19 0-2600</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2222.71">1909 90 11397,'0'0'7601,"9"-14"-7380,32-41-197,-39 53-24,1 0 0,-1 0-1,1 0 1,0 0 0,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 2 0,1-1-1,-1 0 1,0 0 0,1 1-1,5 0 1,-8 0-7,1-1 0,0 1 1,-1 0-1,1 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 1,1 1-1,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,0-1 0,0 0 0,1 1 0,0 1 0,0 10 25,0 0 0,-1 0 0,-1 1-1,0-1 1,-1 0 0,0 0-1,-1 1 1,0-1 0,-1 0-1,-6 16 1,-17 33 804,19-50-599,1 0-1,1 1 1,0 0-1,1 0 0,0 0 1,0 1-1,2-1 0,0 1 1,0 0-1,1 19 0,35-33-5525,-19 0-2600</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2393.3">2099 581 4946,'0'0'21994,"0"-3"-21722,0-11-272,0 0-560,-10 0-1521,-14 3-2657</inkml:trace>
 </inkml:ink>
 </file>
@@ -13276,9 +13276,9 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6762.46">9636 316 8100,'0'0'4895,"-3"20"-3966,-14 277 2253,17-297-3176,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0-1,0 0 1,0-1 0,0 1 0,1 0 0,-1 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,13-13 165,0-15-124,18-54 0,-21 55-319,0 0-1,20-37 1,-30 63 274,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,1 1 0,20 50 388,-19-46-367,1 3-67,0 2 46,1 0 0,0 0 0,1 0 0,10 16 0,-14-24-258,1-1-1,0 1 0,1-1 0,-1 0 0,0 1 1,1-1-1,-1 0 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,1 0 0,-1-1 1,0 1-1,0-1 0,5 0 0,25-1-4078,1-3-534</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7299.26">10016 310 5282,'0'0'7479,"-18"4"-6527,-56 16 96,72-19-991,-1 0-1,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,1-1 0,-2 3 0,1 4 43,0 0 0,1 0 0,0 0 0,1 12 0,0-3-41,-1-16-57,0 0 0,0 0 0,0 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 0-1,-1 0 1,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,2-1 0,4-1 7,0 1 0,-1-1 0,0 0 0,1-1 0,-1 1 0,0-2 0,-1 1 0,1-1 0,9-6 0,1-7-19,0 0-1,-2-1 1,0 0-1,-1-2 1,-1 1-1,-1-2 1,-1 0 0,0 0-1,-2-1 1,-1 0-1,0 0 1,-2-1-1,6-36 1,-8 28 209,-4 24 107,-4 21-288,-7 35 45,5-26 20,1 1 0,1-1 0,-2 41 0,6-61-80,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,0-1 1,0 0-1,5 4 0,-3-2-13,1-1 0,0 0 0,0 0 0,0-1 1,1 0-1,-1 1 0,0-2 0,1 1 1,11 1-1,-11-1-57,1-2 1,0 1 0,-1-1 0,1 1-1,0-2 1,-1 1 0,1-1-1,0 0 1,-1 0 0,1-1 0,-1 0-1,0 0 1,1-1 0,-1 0-1,0 0 1,-1 0 0,1 0 0,7-7-1,-9 5 46,0 0 0,0 0-1,-1-1 1,0 1 0,0-1-1,0 1 1,-1-1 0,0 0-1,0 0 1,0 0 0,-1 0-1,0 0 1,0-1 0,-1 1-1,0-10 1,0 15 35,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,-1-1-1,1 1 1,0 0-1,-1 0 1,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,-2 0-1,0 0 61,0 0-1,0-1 1,0 2-1,0-1 1,-1 0-1,1 1 1,0-1 0,0 1-1,-7 0 1,5 0-9,1 1 1,-1-1 0,0 1-1,0 0 1,0 0 0,0 0-1,1 1 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 1 0,-6 6-1,5-2-35,0 0 0,1 1 0,1-1 0,-1 1 0,1 1 0,0-1 0,1 0-1,0 1 1,0 0 0,1 0 0,0 0 0,1 0 0,0 0 0,0 10 0,1-14-83,0 1 0,0-1 0,1 1 0,0-1 0,0 1 1,0-1-1,1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,0 0 0,0-1 0,0 1 0,1-1 1,-1 0-1,1 0 0,0 0 0,0-1 0,0 1 0,1-1 1,-1 0-1,9 4 0,0-3-935,0 1 0,1-2-1,0 0 1,0 0 0,0-1 0,0-1 0,0 0 0,0-1-1,20-3 1,21-4-3662</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7610.03">10651 318 208,'0'0'17312,"-11"8"-17213,-11 9 20,1 2 0,1 0-1,0 1 1,2 1 0,0 1 0,-17 28 0,21-32-125,13-18-1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,7-40-739,-2 27 731,0 1 1,1-1 0,0 1-1,1 1 1,1-1 0,15-17-1,-22 26 33,1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,3 2 0,10 9-106,-2 1-1,1 0 1,-2 1 0,0 0 0,0 1 0,-2 0-1,0 1 1,-1 0 0,0 1 0,-2-1-1,0 2 1,-1-1 0,-1 1 0,4 20 0,-9-9-3453,-4-4-1866</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9537.88">8346 1643 2689,'0'0'6945,"-4"-1"-6030,-12-9 4909,2-31-5237,12 68-240,-9 45 0,0-3-17,0 310 1020,11-267-683,0-111-480,0-20 5,-1 1-213,-1 0-1,0 0 1,-7-20 0,-6-42-268,12 38 84,-7-139-801,10 154 826,1 1-1,2-1 1,0 0 0,12-41 0,-13 61 164,1 0 1,0 0-1,0 0 1,0 1-1,1-1 1,0 1 0,6-8-1,-10 13 13,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 1-1,0-1 1,1 1-1,-1 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,1 0 1,-1 1 0,0-1-1,0 1 1,1-1-1,-1 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 2-1,2 4 18,0 1 0,0 0 0,-1 0 0,1 0 0,-2 0 0,1 0 0,-1 1 0,-1-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,0 0 0,-1 1 0,0-1 0,0 0 0,-1 0 0,1-1 0,-2 1 0,1 0 0,-10 12 0,-39 31 61,86-41-190,-13-4 162,-1 1 1,0 0-1,-1 2 1,37 21 0,70 56-407,-68-44-1374,-56-40 977,1 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 1,0 0-1,0-1 0,7 2 1,5-2-5456</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9537.87">8346 1643 2689,'0'0'6945,"-4"-1"-6030,-12-9 4909,2-31-5237,12 68-240,-9 45 0,0-3-17,0 310 1020,11-267-683,0-111-480,0-20 5,-1 1-213,-1 0-1,0 0 1,-7-20 0,-6-42-268,12 38 84,-7-139-801,10 154 826,1 1-1,2-1 1,0 0 0,12-41 0,-13 61 164,1 0 1,0 0-1,0 0 1,0 1-1,1-1 1,0 1 0,6-8-1,-10 13 13,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 1-1,0-1 1,1 1-1,-1 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,1 0 1,-1 1 0,0-1-1,0 1 1,1-1-1,-1 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 2-1,2 4 18,0 1 0,0 0 0,-1 0 0,1 0 0,-2 0 0,1 0 0,-1 1 0,-1-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,0 0 0,-1 1 0,0-1 0,0 0 0,-1 0 0,1-1 0,-2 1 0,1 0 0,-10 12 0,-39 31 61,86-41-190,-13-4 162,-1 1 1,0 0-1,-1 2 1,37 21 0,70 56-407,-68-44-1374,-56-40 977,1 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 1,0 0-1,0-1 0,7 2 1,5-2-5456</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9688.18">8701 1955 4498,'0'0'10965,"-43"-72"-10965,57 72-5635,6 6-319</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9968.45">8978 1571 3650,'0'0'7243,"-21"2"-6227,6-1-830,9-1-127,1 0-1,-1 0 0,0 0 1,1 1-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 1-1,1 0 1,0 0-1,0 1 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1 1 1,0 0-1,0 0 0,0 0 1,-4 8-1,-1 7 231,1 1-1,1 0 1,0 0-1,2 0 1,1 1-1,0 0 1,1 0-1,2 0 1,0 0 0,1 0-1,1 0 1,5 28-1,-4-41-261,0-1-1,1 1 0,-1-1 1,1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,1-1 1,-1 0-1,2 0 1,-1 0-1,1-1 0,0 1 1,0-1-1,0-1 0,0 1 1,10 4-1,-7-4-38,0-1-1,0 0 1,1 0 0,0-1-1,0 0 1,0-1 0,0 0-1,0 0 1,0-1 0,0 0-1,1-1 1,-1-1 0,17-2-1,-20 1-722,0-1-1,0 1 0,-1-2 1,1 1-1,-1-1 0,0 0 0,0 0 1,-1-1-1,8-7 0,-4 4-1106,11-9-3323</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9968.44">8978 1571 3650,'0'0'7243,"-21"2"-6227,6-1-830,9-1-127,1 0-1,-1 0 0,0 0 1,1 1-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 1-1,1 0 1,0 0-1,0 1 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1 1 1,0 0-1,0 0 0,0 0 1,-4 8-1,-1 7 231,1 1-1,1 0 1,0 0-1,2 0 1,1 1-1,0 0 1,1 0-1,2 0 1,0 0 0,1 0-1,1 0 1,5 28-1,-4-41-261,0-1-1,1 1 0,-1-1 1,1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,1-1 1,-1 0-1,2 0 1,-1 0-1,1-1 0,0 1 1,0-1-1,0-1 0,0 1 1,10 4-1,-7-4-38,0-1-1,0 0 1,1 0 0,0-1-1,0 0 1,0-1 0,0 0-1,0 0 1,0-1 0,0 0-1,1-1 1,-1-1 0,17-2-1,-20 1-722,0-1-1,0 1 0,-1-2 1,1 1-1,-1-1 0,0 0 0,0 0 1,-1-1-1,8-7 0,-4 4-1106,11-9-3323</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10386.84">9355 1934 4530,'0'0'12376,"-7"0"-11677,-12-6-443,27-2-52,44-14 3,-43 19-204,20-9-173,25-9-349,-20 15-4341,-34 8 2471,0 0 1887,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1-1,-1 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0-1-1,-1 3 1,-24 20-1692,-43 17 6261,47-29-1412,19-11-2331,0 0-1,0 0 0,0 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 1 1,0-1-1,0 1 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,0 1-1,-1 4 0,4-7-327,0 0-1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 1,0 0-1,0 1 0,0-1 0,0-1 0,5 0 0,-4 1 1,5 0-260,-1-1 0,1 0 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 0 0,0-1 0,0 0 0,9-6 0,-9 5-469,0 0 0,-1-1 0,0 1 0,0-1 0,0-1-1,0 1 1,-1-1 0,0 0 0,-1 0 0,5-9 0,-2-12-1361</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10584.3">9520 1764 416,'0'0'13043,"-12"-12"-11877,-35-36-928,40 37-190,15 10 0,6 2 14,0 1 1,0 0-1,0 1 0,-1 1 1,1 0-1,-1 1 1,0 0-1,0 1 1,18 11-1,-14-6 71,0 0 1,-1 1-1,0 0 1,-1 1-1,0 1 0,16 20 1,-28-30-104,1 0 0,-1 1 1,0-1-1,-1 1 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,0 0 0,0 1 1,0-1-1,0 0 0,-1 1 1,0-1-1,0 0 0,-1 1 1,0-1-1,-1 8 0,-1-5-7,0-1 0,-1 1 0,1-1 1,-1 0-1,-1 0 0,1 0 0,-1-1 0,0 0 0,-1 0 0,0 0 0,0 0 0,-9 6 0,-129 90-38,42-44-3651,51-34-1526</inkml:trace>
 </inkml:ink>
@@ -13365,7 +13365,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">114 1 5330,'0'0'3602,"-3"9"-3591,-5 13 128,-1 0 0,-21 38 0,18-40-75,2 0 0,0 0 1,1 1-1,2 1 0,-8 30 1,15-50 285,2-11-186,21-61-150,-11 42-18,-9 19 9,0 0 0,1 0 0,1 0-1,-1 0 1,1 1 0,1 0 0,10-13 0,-15 21-17,-1-1 0,1 1 1,-1 0-1,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 1,-1 1-1,1-1 1,-1 0-1,0 1 0,1-1 1,-1 1-1,1-1 0,-1 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 1 1,0-1-1,1 2 0,11 28 34,-11-25-43,16 42-393,36 120 1290,-49-145-2232,0 1 0,-1 0 0,-1 25 0,-2-45-1483</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="156.21">114 308 2801,'0'0'3314,"73"-25"-3314,-39 22-16,0 0-128,5-2-881,-5-1-607,0-5 47</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="156.2">114 308 2801,'0'0'3314,"73"-25"-3314,-39 22-16,0 0-128,5-2-881,-5-1-607,0-5 47</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="802.17">523 105 1297,'0'0'920,"-19"15"-704,-56 50-112,72-63-101,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 1 1,1-1-1,0 1 0,-1 0 0,1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,1 4 0,1 9 79,-2-15-79,0-1 0,0 0 1,0 0-1,1 1 0,-1-1 0,0 0 1,0 1-1,0-1 0,0 0 1,1 0-1,-1 1 0,0-1 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1-1 0,0 1 1,1 0-1,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0-1-1,1 1 0,-1 0 0,0 0 1,0 0-1,0-1 0,1 1 1,-1 0-1,0 0 0,0-1 1,0 1-1,0 0 0,1-1 1,-1 1-1,0 0 0,0-1 1,15-14 613,-15 14-513,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 1 0,1-1 0,-1 1-92,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 1-1,5 12-2,-1 0-1,0-1 0,-1 1 0,-1 1 0,0-1 0,-1 1 1,0-1-1,-1 1 0,-1-1 0,-2 21 0,2-5 22,-1-24-11,1-1 0,-1 1 0,-1 0 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,0 0-1,-6 9 1,8-12 66,0-1 0,-1 1 0,1 0 0,-1 0-1,1-1 1,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,0-1 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,-1-1 0,1 1 0,0 0-1,0-1 1,0 1 0,-1-1 0,1 0 0,0 0-1,-3-1 1,3 0-65,0 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1-1-1,1 1 1,0 0 0,0-1-1,0 1 1,1-1 0,-1 1-1,0-1 1,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,0 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1-1 0,1-3-1,0-2-66,1 0-1,-1 1 1,1-1-1,1 1 1,0 0 0,0 0-1,10-13 1,9-4-799,2 2-1,50-37 1,23-19-1643,-88 69 2319,0-1-1,-1 0 1,0 0 0,-1-1 0,-1 0 0,13-22 0,-20 32 211,1 0 0,0 0-1,-1-1 1,1 1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0-1-1,0 1 1,1 0 0,-1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1-1-1,0 1 1,-2-2 0,1 2 14,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-2 1-1,-1-1 33,0 1 0,0 0 0,-1 0 0,1 1 0,0-1 1,0 1-1,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-6 7 0,7-6-28,0 1-1,0-1 1,0 1 0,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 1 0,0-1-1,1 5 1,-1-7-45,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,0 1 1,0 0 0,1-1-1,-1 1 1,0-1 0,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0-1-1,3 2 1,7 0 88,2 0 0,-1-1-1,0 0 1,0-1 0,19-2 0,-26 2-257,-1-1 1,1 0-1,-1 0 0,1-1 1,-1 1-1,0-1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,-1-1 1,1 1-1,-1-1 1,5-5-1,3-10-3517</inkml:trace>
 </inkml:ink>
 </file>
@@ -13427,7 +13427,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="810.12">9543 545 896,'0'0'5390,"0"-9"-4758,0-22 522,0 65 42,-2-1-771,-10 58-1,-2 9-46,5 620 116,12-425-347,-5-55-35,13 447 256,-10-672-374,19 207 122,-14-176-11,3 0-1,23 76 1,-29-113-112,0-3-13,-1 0-1,0 1 0,0-1 1,-1 1-1,1 9 0,12-30-2158,-2-14-1730,6-14-1128</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1559.96">10303 691 800,'0'0'534,"0"-17"-299,0-117 1006,0-24 6271,0 158-7437,0 3-206,-12 244 43,0-33 200,10-69-82,-31 703 180,24-745-190,-30 603 160,38-627-121,3 83 146,-2-160-199,0 0-1,0 0 0,0 0 1,0 0-1,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 1,0-1-1,-1 1 0,1 0 0,0-1 1,0 1-1,2 2 0,-2-4-3,-1 0-1,1 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0-1 0,-1 1 0,1 0 1,0 0-1,-1-1 0,1 1 0,-1 0 1,1 0-1,0-1 0,0 0 0,4-3-103,1-1-1,-1 0 1,-1 0-1,1 0 1,-1 0-1,6-9 1,7-15-2539,24-54-1,-7 8-2472</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2071.03">11117 236 1553,'0'0'1857,"-6"23"-1220,-51 264 964,9 577-53,47-833-1538,-2 896 702,17-746-231,67 318-1,-66-421-117,-15-77-354,0 0 0,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 1,1 1-1,9-32-1144,-8 20 673,13-48-2940,3-17-1005</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2490.18">11840 295 1617,'0'0'2017,"1"2"-2055,2 14 195,-1 0 0,0 1 0,-1-1 0,0 1 0,-2-1 0,-3 23 0,2-7 270,-31 388 1132,-9 252-743,41-614-791,-3 160 212,28 235 0,15-166-11,20 182-60,-60-468-183,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,0 0 0,-1-1-1,1 1 1,0-1 0,0 1 0,0 0-1,1 0 1,0-2-111,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 1,0 0-1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-3 0,17-40-4224</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2490.17">11840 295 1617,'0'0'2017,"1"2"-2055,2 14 195,-1 0 0,0 1 0,-1-1 0,0 1 0,-2-1 0,-3 23 0,2-7 270,-31 388 1132,-9 252-743,41-614-791,-3 160 212,28 235 0,15-166-11,20 182-60,-60-468-183,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,0 0 0,-1-1-1,1 1 1,0-1 0,0 1 0,0 0-1,1 0 1,0-2-111,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 1,0 0-1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-3 0,17-40-4224</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2957.16">12673 256 3810,'0'0'4220,"0"-9"-3889,0-17-314,0 20-63,0 20-77,-14 609 1023,0 116 140,25-566-861,63 328 1,0-33 98,-74-467-385,4 19 337,-4-20-272,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,12-12-3212</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3370.38">13568 273 3025,'0'0'1761,"-5"21"-1056,-19 74 341,-48 226 837,36 16-644,14 568 0,57-438-440,-18-281-24,-7-127-562,0 15-252,-4-70-2532,2-3-5903</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5487.51">9096 0 2401,'0'0'5715,"10"4"-4576,-11 45-1118,-3-1-1,-1 1 1,-23 93 0,25-131-12,2 0 1,0 0-1,0 0 1,1 11-1,0-14-8,0-7 9,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,0 1-1,-1-1 1,1 1 0,-1-1-1,1 1 1,0-1 0,0 0-1,-1 1 1,1-1 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0-1 0,1 1-1,0-1 73,6 1 8,0-2-1,0 1 0,0-1 1,0 0-1,0-1 1,0 0-1,-1 0 1,1-1-1,13-8 1,28-13-153,-43 24-172,3-2-4435,-5 0 675</inkml:trace>
@@ -13438,14 +13438,14 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11352.07">12199 4104 2577,'0'0'5507,"0"-1"-5067,-6 70 529,3-50-783,0 1 0,2-1-1,0 0 1,2 1 0,3 26 0,-4-45-181,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 1,1 1-1,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,1 1 1,1-2-1,2 1 17,0-1-1,1 0 1,-1-1 0,0 1 0,0-1 0,-1 0 0,9-6-1,-7 2-9,-1 0-1,0 0 1,0-1-1,0 0 1,-1 1-1,0-1 1,-1-1-1,0 1 0,0 0 1,0-1-1,-1 0 1,-1 1-1,1-1 1,-2 0-1,1 0 1,-1 0-1,-1-9 1,1 11 8,-1 0 1,0 0 0,0 0-1,0 1 1,-1-1 0,0 0 0,-1 1-1,1 0 1,-1-1 0,0 1 0,-1 0-1,0 0 1,0 1 0,0-1-1,0 1 1,-1 0 0,0 0 0,0 0-1,0 1 1,-1 0 0,1 0 0,-11-6-1,15 9-28,0 1 0,-1-1-1,1 0 1,0 1-1,0-1 1,-1 0 0,1 1-1,0 0 1,-1-1 0,1 1-1,-1 0 1,1-1-1,0 1 1,-1 0 0,1 0-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 1-1,-1-1 1,1 1-1,0-1 1,-1 1 0,1-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1-1-1,0 1 1,0 0 0,0 0-1,1 1 1,-1-1 0,-1 2-1,0 2-571,0 1-1,0-1 1,1 1 0,0-1-1,0 1 1,0 0 0,1-1-1,0 8 1,0 4-3243</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12296.2">12540 4239 3826,'0'0'6493,"-28"-3"-4313,28 3-2182,-27 3 549,26-3-538,1-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1 1 0,1 0-1,0-1 1,-1 1 0,1-1-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 1-1,0-1 1,1 1 0,-1-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 1 0,1-1-1,-1 1 1,1-2 0,0 2-21,-1-1 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 1 1,-1-1-1,1 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,-1-1 1,1 0-1,0 0 0,0 1 1,0-1-1,0 1 1,-1-1-1,1 0 0,0 1 1,0 0-1,-1-1 1,1 1-1,0-1 0,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 1,-1 0-1,0 0 0,1-1 1,-1 1-1,0 0 1,1 0-1,-1 0 0,0 0 1,1 1-1,-1 8 30,0-9-9,1 0 1,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1-1-1,1 1 1,0 0 0,-1 0-1,0 0 1,1-1 0,-1 1-1,1 0 1,-1-1 0,0 1-1,0 0 1,1-1 0,-1 1-1,0-1 1,0 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-3 0 1,2 0 153,6-20-267,-4 20 94,-1 0 1,1 0-1,0 0 0,0 0 1,-1 1-1,1-1 0,0 0 1,-1 0-1,1 1 0,0-1 1,-1 0-1,1 1 1,-1-1-1,1 0 0,0 1 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1 0 0,0-1 1,1 1-1,-1-1 1,1 1-1,-1 0 0,0-1 1,0 1-1,1 0 0,-1-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 1,-1 1-1,1 1 0,0 4-15,0-5 430,0-35 68,0 34-494,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1 0-1,0-1 1,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,2 1-1,2 9 13,-1 0-1,0 0 1,0 0-1,-1 0 0,-1 0 1,0 0-1,0 1 0,-1-1 1,-2 20-1,1 5 7,0-27-269,0-1 1,-1 1-1,1-1 0,-2 0 0,1 1 0,-1-1 0,0 0 0,-1 0 1,0-1-1,0 1 0,0-1 0,-1 0 0,0 0 0,-1 0 0,0-1 1,0 0-1,0 0 0,-11 7 0,-3 3-4502</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13736.18">12876 3965 1857,'0'0'7531,"-1"-13"-6541,1 5-725,-5-49 779,4 53-674,0 0-1,0 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,-3-2 0,5 6-325,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 1 1,0-1-1,-6 11 347,1 24-811,4-30 601,-8 135 362,7 142 1,4-132-15,-2-150-632,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 0 0,3-4-721,0 0 1,0 0 0,-1 0 0,1-1 0,-1 1-1,5-11 1,-3 8-327,18-31-4730</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13989.85">13066 3890 3362,'0'0'10258,"0"-10"-9237,0-20-749,0 53 75,0 72 771,0 96-801,0-110-3779,0-44-775</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13989.84">13066 3890 3362,'0'0'10258,"0"-10"-9237,0-20-749,0 53 75,0 72 771,0 96-801,0-110-3779,0-44-775</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14370.48">13466 4338 9861,'0'0'7408,"-13"-1"-7301,8 1-95,-6-1 21,-1 0 0,1 1 1,-1 1-1,1 0 1,-1 0-1,-13 4 0,24-5-22,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1-1,0 0 1,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0-1 0,-1-40-34,1 35 13,1 6-6,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 0-1,1 1 0,0-1 1,-1 1-1,1-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1-1 0,0 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,1 1-1,-1 0 3,1-1 0,-1 0 1,1 0-1,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 1,-1 1-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,2 3 0,0 5-42,0 1-1,-2 0 1,1 0 0,-1 0-1,0 0 1,-1-1-1,0 1 1,-1 0 0,0-1-1,-1 1 1,1-1 0,-2 1-1,1-1 1,-2 0-1,1 0 1,-1-1 0,0 0-1,-1 1 1,0-2-1,0 1 1,-9 8 0,13-14-189,1-1-191,0 0-1,-1 0 1,1 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,1 1 0,-1-1-1,0 1 1,1 0 0,-1-1-1,0 4 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14915.45">13809 4049 4770,'0'0'3919,"0"-17"-2409,0 3-1147,1 2-38,0 0 0,-1 1-1,0-1 1,-1 1 0,0-1 0,-1 1-1,-1 0 1,0 0 0,0-1 0,-6-11-1,9 22-293,-1-1 0,0 1 0,1-1-1,-1 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0 0 0,-1-1 0,1 1-1,0 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 1-1,-1-1 1,0 0 0,1 1 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 1-1,0-1 1,1 1 0,-1 0 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 0-1,-1 1 1,-2 3 66,0 0 0,-1 0 0,2 0-1,-1 1 1,1 0 0,0-1 0,0 2 0,0-1 0,-2 7 0,1-1-107,0 0 1,1 1 0,0 0-1,1-1 1,1 1 0,0 0-1,1 1 1,0-1-1,1 0 1,0 0 0,3 17-1,-2-28-3,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1-1,0 1 1,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,2-1 0,-1 1 4,0-1-1,0 1 1,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0-1-1,0 1 1,3-5 0,6-30 76,-10 33-37,-1 0 0,1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,0 0 0,2-3 0,1 26 176,9 328-38,-14-339-153,0 0 0,-1 0-1,0 0 1,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-7 11 0,7-16-11,0 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,-4-1 0,8 0-112,-1 0 0,1-1 0,-1 1 1,0 0-1,1-1 0,-1 1 0,1-1 1,-1 1-1,1 0 0,-1-1 1,1 1-1,-1-1 0,1 0 0,0 1 1,-1-1-1,1 1 0,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 1,0-27-3008,0 23 2042,0-32-5475</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15460.29">14007 3845 6211,'0'0'4573,"8"-17"-4291,28-50-119,-35 65-155,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 1,1-1-1,-1 1 0,3-1 0,-4 1-8,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,0 0 0,1-1 0,-1 3 1,0 79 967,-18 131 0,12-180-940,2 0 0,2 1 0,1-1-1,4 37 1,-3-69-29,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,-1 0 1,1-1 0,0 1-1,0-1 1,1 1-1,-1-1 1,0 1-1,0-1 1,0 0-1,2 1 1,-1-1 9,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 0 0,1 1-1,-1-1 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0 0,0 0-1,0-1 1,1 1-1,-1 0 1,0 0 0,0-1-1,0 1 1,-1 0-1,1-1 1,1-1 0,4-20-8,0 2-288,-4 35-219,-24 372 523,21-376-6,-1 0 0,0 0 1,-1 0-1,0 0 0,-1 0 1,0-1-1,0 1 0,-1-1 1,0 0-1,-1-1 0,0 1 1,0-1-1,0 0 0,-1-1 1,-1 0-1,1 0 1,-1 0-1,-1-1 0,1 0 1,-1 0-1,0-1 0,-13 5 1,11-5-611,0-1 1,-1-1 0,1 0-1,-1-1 1,0 0 0,0-1-1,-14 0 1,-18-1-4788</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17268.79">12064 245 912,'0'0'3869,"0"-4"-3456,0-19 3896,-11 25-3871,-5 16-318,1 1 0,0 0 1,2 1-1,0 0 1,2 1-1,-12 26 1,9-19-12,-17 33 115,2 2 0,-23 77 0,46-130-349,14-19-1761,15-12-745,10-8-1027</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17642.43">12176 283 800,'0'0'6110,"2"-6"-5014,4-18-453,-4 18-459,-5 9-304,-22 35 415,1 0-1,2 1 1,-32 81-1,-32 137 815,73-215-1046,5-17-80,0 1 1,2-1 0,0 1-1,-2 45 1,25-73-2222,-10-1 1730,-1 0 1,1-1 0,-1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,5-7 0,28-28-2951</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17946.74">12496 236 4082,'0'0'4167,"-14"24"-3767,-3 5-258,-68 131 418,-44 146 984,15-33-714,-13 55-694,117-298-1355,12-22-1859,11-16 228,10-17 41</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18285.61">12496 683 2609,'0'0'4130,"-8"27"-3196,1-4-705,-57 173 1268,-162 319 1814,11-30-2692,209-467-747,0 0 0,1 1 0,-6 36 1,8-6-3820,8-48 274,4-2 2588,2-1-2676</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18285.6">12496 683 2609,'0'0'4130,"-8"27"-3196,1-4-705,-57 173 1268,-162 319 1814,11-30-2692,209-467-747,0 0 0,1 1 0,-6 36 1,8-6-3820,8-48 274,4-2 2588,2-1-2676</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18925.23">13024 189 1265,'0'0'1392,"-73"97"-495,44-44 527,4 8-175,-4 6-209,0 3-223,5 2-321,4 1-256,1-1-112,4-5-112,10-9 32,-5-13-48,10-12-16,0-8-208,0-13-1457,0-10-1408,5-2-913</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19235.38">13278 240 160,'0'0'5952,"-6"16"-5450,-134 312 3446,37-98-2731,44-91-1068,-66 169-248,122-296-385,-1-1 0,1 1 0,1 0 0,0 0 0,1 0 0,0 15 0,4-24-2584,14-3-544</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19547.44">13408 456 3682,'0'0'1841,"-9"23"-942,-6 14-504,-79 223 2454,-1 40-774,-57 196-677,117-384-924,-7 36 152,42-126-213,0-14-5415,8-22 1659</inkml:trace>
@@ -13464,7 +13464,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-200771.56">93 7141 1217,'0'0'1371,"-11"18"-835,-35 55-114,37-48 81,16-14 43,-5-10-464,0 0 1,0-1-1,1 1 0,-1-1 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,3-1-1,1 1 84,22-2 377,0 0 0,-1-2 0,0-1 0,1-1 0,-2-1 0,53-22 0,178-81 490,-146 58-2035,165-51 0,-255 98-2055,-7 4-398</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-200446.01">337 7611 6163,'0'0'4765,"23"-10"-3994,323-150 371,-239 110-1111,112-46-577,-190 89-2816</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-198048.51">255 7581 2001,'0'0'6555,"-6"0"-5688,-20 0-120,19 0 808,19-1-1493,155-38 1673,26-5-1392,19 13-276,149-31 34,-354 60-102,12 1 320,-15 25-143,6 332 1331,-11-351-1495,1-1 1,-1 1-1,0-1 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,-1-1-1,0 1 1,0-1-1,0 0 1,0 0-1,-5 1 1,-14 6 18,0-1 1,0-2-1,-32 6 1,44-10-23,-77 11 70,-2-5 0,1-4 0,-96-7 1,35 1 99,148 1-177,1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0-1 1,-1 1 0,2-3-1,-5-37-45,4 14 33,0 0 0,2 0 1,1 0-1,1 0 0,11-35 1,-11 47 9,18-42 50,-22 56-177,1 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 1 0,-1 0 1,1 0-1,0-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,-1 1 0,1-1 1,0 0-1,0 1 0,22 11-4136,-8-1-29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-195484.24">1742 7729 1713,'0'0'7043,"15"-4"-6117,88-25 562,1 3 0,196-20 1,223 15-1254,-291 22-82,874-88 7,130 21-110,-1025 72-53,692-2-12,-604 23 30,49 2-1,-248-20-1,51-1 50,0 7 1,162 26-1,-235-19 437,0-2-1,100-1 1,-18-15-420,-160 2-44,0 0-1,0 0 0,-1 0 1,1 1-1,-1-1 0,0 0 1,-2-6-1,-31-50-18,22 42-7,1-1 1,-9-24-1,48 136-256,-24-77 307,0 0-1,-1 0 1,0 0 0,-2 1-1,0-1 1,-2 27 0,0-40-35,0-1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,1 1 0,-1-1 0,0 0 0,0-1 1,0 1-1,-1 0 0,1-1 0,0 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,-3 0 0,-62 19-1700,57-18 723,-44 8-3377,-15-3-3105</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-195484.25">1742 7729 1713,'0'0'7043,"15"-4"-6117,88-25 562,1 3 0,196-20 1,223 15-1254,-291 22-82,874-88 7,130 21-110,-1025 72-53,692-2-12,-604 23 30,49 2-1,-248-20-1,51-1 50,0 7 1,162 26-1,-235-19 437,0-2-1,100-1 1,-18-15-420,-160 2-44,0 0-1,0 0 0,-1 0 1,1 1-1,-1-1 0,0 0 1,-2-6-1,-31-50-18,22 42-7,1-1 1,-9-24-1,48 136-256,-24-77 307,0 0-1,-1 0 1,0 0 0,-2 1-1,0-1 1,-2 27 0,0-40-35,0-1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,1 1 0,-1-1 0,0 0 0,0-1 1,0 1-1,-1 0 0,1-1 0,0 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,-3 0 0,-62 19-1700,57-18 723,-44 8-3377,-15-3-3105</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-194650.49">4513 7210 6003,'0'0'7024,"-1"-12"-6189,-2-39-50,2 39-233,1 24-496,-1 152 355,-2-8 601,21 188 1,-13-308-1555,11 104 2282,-14-99-4218,-4-9-3768,6-63 1363</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-193127.38">4452 7110 7603,'0'0'3407,"26"-12"-2894,-14 7-444,20-9 173,-1 1 0,2 2 1,-1 1-1,56-8 0,397-18 1236,4 32-1413,-202 4-39,1174-99-1027,-1430 95 984,752-93-371,-699 87 360,113 0 0,-196 11 27,0-1 0,1 1 1,-1 0-1,0 0 0,1 0 0,-1-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 0,-1-1 1,1 0-1,0 1 0,-1-1 0,1 0 0,-1 1 1,0-1-1,1 3 0,11 43 267,-10-36-110,4 25 214,-2 0-1,-1 1 1,-4 56 0,0 6 178,26 246 762,-20-244-1069,-2 204 802,-3-299-1004,-1 0 1,0 0-1,0-1 1,-1 1 0,0 0-1,0 0 1,0-1 0,0 1-1,-1-1 1,0 0-1,0 0 1,0 0 0,-1 0-1,-7 7 1,4-5-8,0-1 1,-1 0-1,0-1 0,0 0 1,0 0-1,-1 0 0,0-1 1,-13 4-1,-6 0-18,0-2 1,0-1-1,-1-1 0,0-1 0,-35-2 1,-106-1-177,-586 5-354,4 35 359,391-2 169,-528 27 165,836-68-8,0-2 1,-81-18-1,-24-4 27,-83 2 1562,82 16-1184,158 9-550,13-3-3610,44 2-2246,-26-3 1182</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85210.43">3714 8959 5234,'0'0'5555,"-3"-17"-4547,-11-51-60,6 40 311,3 23-38,1 33-887,8 104-208,6 1-1,35 169 0,129 830 337,-145-884-6,30 419 710,-60-498-683,6 123 164,-1-244-552,1-1 1,3 0 0,2-1 0,17 49 0,-28-104-254,0 0 1,1-1 0,0 1-1,1-15 1,1-10-1103,-2-95-6108,0 45 52</inkml:trace>
@@ -13472,7 +13472,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-81500.22">567 8689 256,'0'0'8385,"-12"-15"-7379,-39-49-347,48 61-603,1 0 0,-1-1 0,0 1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 1 1,0-1-1,0 1 0,-1-1 0,1 1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-4 6 0,-1 3-58,0 0 0,1 0 0,0 0-1,1 1 1,0 0 0,1 0 0,0 1-1,1-1 1,1 1 0,0-1 0,1 20 0,0-33 1,1 1 1,0 0 0,0 0-1,0 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,0 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,-1 0 0,0-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,-1 0-1,1 1 1,1-1 0,1 1-18,-1-1 0,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,3-2 0,-1 0-53,1 0 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,8-9 0,-4-1-78,-1 0 0,-1-1 0,0 0 0,-1 0 0,0 0-1,4-20 1,16-96-736,-20 99 675,16-187-1342,-14 103 1511,-5 92 1257,-2 32-805,-1 48-459,0-42 249,-2 54 182,0-42-294,1 0 0,1 0 0,1 0 0,2 0 0,8 37 0,-9-58-78,0 0-1,0 0 1,1 0-1,0 0 1,0-1 0,0 0-1,1 1 1,-1-1-1,1 0 1,1-1-1,-1 1 1,1-1-1,0 0 1,0 0-1,9 6 1,-10-9-2,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 0 0,1-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 0-1,0-1 0,-1 1 1,1-1-1,0 1 1,-1-1-1,1 0 0,0 0 1,-1-1-1,1 1 1,-1-1-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,4-6 1,0 2-1,-1 0 1,0-1-1,0 0 1,-1 0 0,0 0-1,0-1 1,-1 0-1,0 0 1,0 0 0,-1 0-1,0-1 1,3-13-1,-2-5 113,-1 1-1,-1-54 0,-2 77-97,-9 196 333,8-158-172,2 0 0,1 1 1,2-1-1,1 0 0,2 0 0,2-1 0,17 47 0,-24-76-158,0-1 0,0 0-1,0 0 1,0-1 0,1 1 0,0 0 0,3 3 0,-6-6-23,1-1 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,1 1 0,-1-1 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,1 0 0,-1-1 1,0 1-1,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1-1 0,3-18 18,-2 12-77,-1 1-1,0-1 0,-1 1 1,1 0-1,-1-1 1,0 1-1,-1 0 1,0-1-1,0 1 0,0 0 1,-1 0-1,0 1 1,0-1-1,0 1 1,0-1-1,-1 1 1,0 0-1,0 0 0,-1 0 1,0 1-1,1 0 1,-1 0-1,-1 0 1,1 0-1,0 1 0,-1 0 1,0 0-1,-7-3 1,9 6 31,30-3-9,0-1 0,-1-1 0,1-1 1,-1-1-1,25-11 0,-44 16 24,48-18 52,51-27-1,-40 11-4059,-55 31-673</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-80151.04">4447 8511 1953,'0'0'9175,"-2"-5"-7935,1 3-1110,0 0-1,-1 0 1,1 0-1,-1-1 1,0 1-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,-1-1 0,1 1-1,0 0 1,-1 0-1,-2-1 1,-3-1-30,-1 1 1,1 0 0,-1 1 0,1 0-1,-14-1 1,12 2-111,0 0-1,1 1 1,-1 0 0,0 0 0,0 1-1,1 0 1,-1 1 0,1 0 0,0 0-1,-15 8 1,21-8-1,0-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,1 0 1,0 1 0,0-1-1,0 0 1,1 1-1,-1-1 1,1 1 0,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 0 1,1 0 0,0 0-1,0-1 1,0 1-1,1 0 1,1 7-1,-1-10 10,0 0 0,0 1-1,0-1 1,0 1-1,0-1 1,0 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1-1 0,1 0-1,0 1 1,-1-1-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0 0,2-1-1,4 0-20,-1 0 1,1 0-1,-1 0 1,1-1-1,11-5 0,-10 2-42,-1 0-1,-1-1 1,1 1-1,-1-2 1,0 1-1,0-1 1,-1 0-1,0-1 1,0 1-1,0-1 1,-1 0-1,-1 0 0,1-1 1,-1 0-1,5-15 1,3-16-188,-2 0 1,8-55-1,-12 59 197,4-62-872,-11 168 846,-2-44 126,2 1 1,1 0 0,1-1-1,2 1 1,0-1-1,2 0 1,9 29 0,-13-51-40,1 0 1,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0-1 0,0 1-1,1 0 1,-1-1 0,1 1 0,0-1 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 0 0,-1-1-1,0 1 1,0-1 0,1 1 0,-1-1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0-1 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,0-1 0,4-3 0,4-6 9,-1 0 0,0 0 1,-1-1-1,0 0 0,-1-1 0,-1 0 1,0 0-1,-1 0 0,0-1 1,-1 0-1,-1 0 0,0-1 1,-2 1-1,3-25 0,-20 210 27,1 7 607,14-163-566,-1 10 40,2-1-1,7 47 1,-7-64-113,0 0-1,1 0 1,0 0 0,0 0-1,1 0 1,-1-1-1,1 1 1,0-1-1,1 1 1,-1-1-1,1 0 1,0-1 0,1 1-1,-1-1 1,1 1-1,6 3 1,-10-7-3,0 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1-1,1 1 1,1-1 0,-2 0-24,0-1 1,0 1-1,0 0 1,0 0-1,0-1 0,-1 1 1,1-1-1,0 1 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 0 1,0 1-1,0-3 0,0-4-88,-1 0 0,1 1 0,-2-1 0,1 0 0,-1 1 0,-1-1 0,1 1 0,-5-10 0,-4 3-60,0-1 0,0 2 0,-2 0 0,-13-12 0,-20-22 608,46 47-436,-1-1 1,1 1-1,0-1 0,0 0 1,-1 1-1,1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 1,0 0-1,0 1 0,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,0 1 0,1 0 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 1,2-1-1,28-13-118,-24 11 119,352-128-95,-223 86-538,-124 41 63,9-2 289,-5 5-5415</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77476.33">2033 9160 5090,'0'0'5259,"-4"-5"-4696,4 5-559,0-1 0,0 1 0,0-1 1,-1 1-1,1-1 0,0 1 0,0-1 1,-1 1-1,1-1 0,0 1 0,-1 0 1,1-1-1,-1 1 0,1-1 0,0 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1-1 1,-1 1-1,1 0 0,-1 0 0,1 0 0,-1 1 1,0-1-1,-3 21 130,15 54 235,-9-63-249,125 611 2113,-94-510-1973,-19-73-188,-2 2-1,11 68 1,-23-108-60,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,0 0 0,-1 3 0,1-5-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 1,0-1-1,0 1 0,1 0 0,-1-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,1-1 0,-1 0 0,1 1 1,-1-1-1,0 1 0,1-1 0,0 0 0,-1 1 0,0-2 1,-39-61 236,39 62-254,-42-84 26,25 46-34,-26-40 0,39 73-11,6 59-401,1-42 428,0 0-1,1 0 0,1 0 1,0 0-1,0-1 0,1 1 1,1-1-1,-1 0 0,2-1 1,-1 1-1,9 7 1,-11-11 3,1-1 1,0 0-1,0-1 1,1 1-1,-1-1 1,1 0 0,0-1-1,0 1 1,1-1-1,-1 0 1,0-1 0,1 1-1,0-1 1,0-1-1,-1 1 1,1-1 0,0 0-1,0-1 1,8 0-1,-12-1-3,1 1 0,-1-2 0,1 1-1,-1 0 1,0-1 0,0 0 0,1 1-1,-1-1 1,-1 0 0,1-1-1,0 1 1,0-1 0,-1 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0-1-1,0 1 1,-1 0 0,1 0-1,-1-1 1,0 1 0,0 0 0,1-7-1,4-9-900,-2-1 0,-1 1 0,2-24 0,-4-1-4825,-1 32 1647</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76531.35">2076 11245 2609,'0'0'8340,"-1"-5"-7596,-6-15-298,6 15-174,45 5 1078,-40 0-1319,1 0-1,-1 0 1,1 0 0,-1-1 0,1 1-1,-1-1 1,1 0 0,-1-1-1,0 1 1,1-1 0,-1 0 0,0 0-1,7-4 1,-8 3-21,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,0-1 1,0 1-1,0-1 1,0 0-1,-1 1 1,0-1-1,1 0 1,-1 1-1,-1-6 1,1-76 65,0 84-123,6 25-249,-5-22 303,0-1-1,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 1,0 0-1,4-1 0,-3 0 1,0 0 0,0 0 0,-1-1 0,1 0 0,0 1 1,0-1-1,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,4-5 0,0-1-8,-1-1 0,0 0 0,0 0 1,-1-1-1,0 1 0,-1-1 0,0 0 0,1-12 1,-1-12-134,-1-1 1,-1 0 0,-8-58 0,0 67 58,3 18-38,2 19-283,2 6 371,-1 11 45,1 0 0,1 0 0,1 0 0,2 0 0,0 0 0,2-1 0,12 36 0,-8-38 152,1 0 0,0 0 0,28 39 0,-35-57-347,0-1 0,0 0-1,1 0 1,-1 0-1,1-1 1,0 1-1,1-1 1,-1 0 0,1 0-1,0-1 1,0 0-1,0 0 1,0 0-1,0-1 1,1 0-1,-1 0 1,1-1 0,-1 0-1,13 1 1,-8-2-3498</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76531.36">2076 11245 2609,'0'0'8340,"-1"-5"-7596,-6-15-298,6 15-174,45 5 1078,-40 0-1319,1 0-1,-1 0 1,1 0 0,-1-1 0,1 1-1,-1-1 1,1 0 0,-1-1-1,0 1 1,1-1 0,-1 0 0,0 0-1,7-4 1,-8 3-21,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,0-1 1,0 1-1,0-1 1,0 0-1,-1 1 1,0-1-1,1 0 1,-1 1-1,-1-6 1,1-76 65,0 84-123,6 25-249,-5-22 303,0-1-1,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 1,0 0-1,4-1 0,-3 0 1,0 0 0,0 0 0,-1-1 0,1 0 0,0 1 1,0-1-1,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,4-5 0,0-1-8,-1-1 0,0 0 0,0 0 1,-1-1-1,0 1 0,-1-1 0,0 0 0,1-12 1,-1-12-134,-1-1 1,-1 0 0,-8-58 0,0 67 58,3 18-38,2 19-283,2 6 371,-1 11 45,1 0 0,1 0 0,1 0 0,2 0 0,0 0 0,2-1 0,12 36 0,-8-38 152,1 0 0,0 0 0,28 39 0,-35-57-347,0-1 0,0 0-1,1 0 1,-1 0-1,1-1 1,0 1-1,1-1 1,-1 0 0,1 0-1,0-1 1,0 0-1,0 0 1,0 0-1,0-1 1,1 0-1,-1 0 1,1-1 0,-1 0-1,13 1 1,-8-2-3498</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76330.79">2273 10828 6371,'0'0'2945,"39"-6"-4754,-10 20-1120,0 0-1649</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76017.55">2603 10892 3522,'0'0'6779,"-10"14"-6275,-29 46-224,38-58-260,-1 1-1,1-1 1,0 0 0,0 0-1,0 1 1,0-1 0,1 1-1,-1-1 1,1 1 0,-1-1-1,1 1 1,0 3-1,0-5-13,0 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1 0 0,0-1-1,0 1 1,-1-1-1,3 2 1,2-1 5,-1 1 1,1-1 0,0 0 0,-1 0 0,1-1 0,0 1-1,0-1 1,6-1 0,-6 1 17,-4 0-23,0 0 0,0-1 0,0 1 1,0 0-1,-1-1 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 1,1 1-1,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 0,0-42 61,-1 33 19,1 10-98,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,0 1 0,2-1-71,0 1 0,-1-1-1,1 0 1,0 0 0,0 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,1 1 1,-1-1 0,0 0-1,0 1 1,0-1 0,0 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,1 0 0,-1 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 1 1,1-1 0,15 5-3015,7-1-629</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-75782.14">2765 10875 1809,'0'0'8748,"-5"2"-7844,2-1-826,0 0 0,0 1-1,0-1 1,1 1 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 0 0,0 1-1,1 0 1,-1-1 0,1 1-1,0 0 1,-1 0 0,1 0-1,-1 4 1,0 5 277,-1-1-1,1 1 1,1 0 0,0 21-1,1-32-336,0 1-1,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,2 1 0,1-1 8,0 1-1,0 0 0,0-1 1,0 0-1,1 0 0,-1 0 1,0 0-1,6 0 0,2-1-29,0 0 0,0-1 0,1 0 0,-1-1 0,16-4 0,-19 3-547,0 0 0,0-1-1,-1 0 1,0 0 0,1-1 0,-1 0-1,-1 0 1,11-10 0,-10-2-3490</inkml:trace>
@@ -13480,9 +13480,9 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-73865.71">2629 12955 0,'0'0'6016,"3"-9"-4559,3-10-218,-2 0 1,0-1-1,-1 0 1,1-38-1,-4 58-1204,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 1-1,1-1 1,-2 0-1,-25 8 66,23-3-71,1-1-1,-1 1 1,1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,0 1-1,-3 10 1,-8 53 532,10-53-429,1-1 1,1 1-1,1 0 1,0-1 0,4 26-1,-3-34-119,1-1 1,0 0-1,0 0 0,0 0 1,1-1-1,0 1 0,0 0 1,1-1-1,-1 0 0,1 0 1,0 0-1,1 0 0,-1-1 1,1 1-1,0-1 0,8 5 1,-6-5-3,-1 0 0,1-1 0,1 0 1,-1 0-1,0 0 0,1-1 1,-1 0-1,1-1 0,0 1 1,0-2-1,-1 1 0,16-1 0,-22 0 24,0-5-25,0 1 0,-1-1 0,0 0-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0 0 0,-1-1-1,1 1 1,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0-1,0 1 1,0-1 0,0 1 0,-6-6 0,3 6 5,-1 1 0,1-1 1,-1 1-1,1 1 0,-1-1 1,0 1-1,0 0 0,1 1 1,-1 0-1,0 0 0,0 0 1,0 1-1,-7 1 0,10-1-225,0 0 0,0 0-1,0 0 1,0 1 0,0 0-1,0-1 1,1 1-1,-1 1 1,-6 4 0,8-6-235,1 1 1,-1 0-1,0 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,1 0 1,-1 1 0,1-1-1,0 0 1,-1 1-1,1 2 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-73335.2">2673 12746 288,'0'0'6102,"-18"-13"-4971,-58-39-205,74 50-857,-1 1 0,1-1 1,-1 0-1,0 1 0,0 0 0,1-1 1,-1 1-1,0 0 0,0 1 1,0-1-1,0 0 0,-1 1 1,1 0-1,0-1 0,0 1 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,1 1 1,-6 3-1,2 1-6,0 1 1,0 0-1,1 0 1,0 0-1,1 1 1,-1-1-1,-4 13 1,4-9-5,-6 12 215,2 1 0,1 0-1,0 1 1,2-1 0,1 1 0,1 0 0,1 1 0,1-1 0,1 1 0,2-1 0,4 31 0,-2-41-207,2 1 1,0-1 0,0 0 0,2-1 0,0 1 0,0-1 0,2-1 0,-1 0 0,2 0 0,0 0 0,0-1 0,1-1 0,1 0 0,0 0-1,0-1 1,1 0 0,0-2 0,1 1 0,-1-2 0,2 1 0,-1-2 0,1 0 0,0-1 0,0 0 0,19 2 0,-20-5-49,1-1 0,0 0 0,0-1 0,0-1 0,0 0 0,16-4 1,-23 3-10,0 0 1,0-1-1,-1 0 1,1-1 0,-1 1-1,1-1 1,-1-1 0,0 0-1,-1 0 1,1 0 0,-1-1-1,7-7 1,-3 2-3,-1-1 1,0-1-1,0 1 0,-1-1 1,-1-1-1,0 0 1,-1 0-1,0 0 0,-2 0 1,1-1-1,-2 0 1,0 0-1,0 0 0,-2 0 1,0-1-1,-1 1 1,0 0-1,-1-1 0,-1 1 1,0 0-1,-5-16 1,1 11-11,0 1 0,-1 0 0,-1 1-1,-1 0 1,0 0 0,-1 1 0,-1 0 0,-1 1 0,0 0 0,-1 1 0,-1 0 0,-1 1 0,0 0 0,0 2 0,-28-18 0,38 26-4,0 1 0,-1 0 0,1 0-1,-1 1 1,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 1 0,0-1-1,0 1 1,0 0 0,0 0 0,0 1 0,-7 1 0,8 0-193,1 0-1,0 0 1,-1 0 0,1 1-1,0 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 1 1,1-1 0,0 1-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,0 1-1,0-1 1,1 1 0,-2 6-1,-7 21-3190,0-5-2536</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-70712.98">8217 8569 1313,'0'0'3756,"-22"14"-2844,-69 46-127,83-54-653,1-1 0,0 1 1,0 1-1,0-1 0,1 1 1,-1 0-1,2 1 0,-1-1 0,1 1 1,0 0-1,1 0 0,0 1 1,0 0-1,1-1 0,0 1 0,-4 19 1,6-24-110,0-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1 0-1,1 0 1,-1 0-1,2 7 1,-2-9-14,1-1 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 0-1,0 0 1,1 1-1,-1-1 1,0 0 0,1 0-1,-1 0 1,3-1-1,0 1 8,0 0-1,0 0 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0-1 0,0 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,2-4 1,0 1-4,-1-1 1,0 0-1,0 0 1,-1-1 0,0 1-1,-1-1 1,1 0-1,1-9 1,2-8 6,-2 0 0,0-1-1,-2 0 1,0-43 0,-3-94 2172,0 229-2290,3 1 1,3-1-1,3 0 1,23 86-1,-18-114-2104,0-8-1731</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-69636.85">8316 8845 592,'0'0'7713,"1"0"-7598,0 1-1,0-1 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,0 1 1,2-1-1,1-1-48,0-1 0,-1 0-1,1 0 1,0-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 0 1,-1 0-1,1-1 1,-1 1 0,2-5-1,1-4-37,0 0 0,-1 0 0,3-18 0,-5 18-6,-1 1 0,0-1-1,-2-21 1,0-10 30,1 42-84,-6 11-217,5-9 245,0 1 1,0 0-1,1 0 0,-1-1 1,0 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 1,2 14-657,1-27 199,5-15-104,-5 5 611,-4 17 671,1 16-440,0 144 1001,0-154-1257,0 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,1-1 1,-1 1-1,0-1 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,2 0 1,4 1 63,1 0 0,-1-1 0,1 0 0,-1 0 0,14-1 0,-16 0-70,-3-1-1,-1 1 1,0-1-1,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 0,0 1 0,0-1 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,1-3 0,21-60 101,-20 55-112,7-35-81,-1 0-1,-2-1 1,-2 0-1,-2-79 1,-13 142-265,2 7 315,1 0-1,1 0 1,2 1 0,-4 46 0,8 105 148,0-155-95,2 0-1,0 0 1,2 0 0,0-1-1,1 0 1,1 0 0,1 0-1,1 0 1,1-1 0,0-1-1,1 1 1,2-1 0,-1-1-1,16 16 1,-27-33-15,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,0-1-1,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0-1-1,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 1-1,1-1 0,-1 0 0,-9-22 104,-1 10-147,0 1-1,-1 0 1,0 0 0,-1 1-1,0 1 1,-1 0 0,-17-9 0,-10-4-172,-50-19 0,79 38 192,-22-11 96,33 13-79,0 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 1,1 1-1,-1-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 1,1 0-1,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 1,25-13-107,-1 1 1,1 1 0,1 1 0,30-7 0,24-9-1583,-20 4-1106,-1-3-2238</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-69636.86">8316 8845 592,'0'0'7713,"1"0"-7598,0 1-1,0-1 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,0 1 1,2-1-1,1-1-48,0-1 0,-1 0-1,1 0 1,0-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 0 1,-1 0-1,1-1 1,-1 1 0,2-5-1,1-4-37,0 0 0,-1 0 0,3-18 0,-5 18-6,-1 1 0,0-1-1,-2-21 1,0-10 30,1 42-84,-6 11-217,5-9 245,0 1 1,0 0-1,1 0 0,-1-1 1,0 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 1,2 14-657,1-27 199,5-15-104,-5 5 611,-4 17 671,1 16-440,0 144 1001,0-154-1257,0 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,1-1 1,-1 1-1,0-1 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,2 0 1,4 1 63,1 0 0,-1-1 0,1 0 0,-1 0 0,14-1 0,-16 0-70,-3-1-1,-1 1 1,0-1-1,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 0,0 1 0,0-1 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,1-3 0,21-60 101,-20 55-112,7-35-81,-1 0-1,-2-1 1,-2 0-1,-2-79 1,-13 142-265,2 7 315,1 0-1,1 0 1,2 1 0,-4 46 0,8 105 148,0-155-95,2 0-1,0 0 1,2 0 0,0-1-1,1 0 1,1 0 0,1 0-1,1 0 1,1-1 0,0-1-1,1 1 1,2-1 0,-1-1-1,16 16 1,-27-33-15,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,0-1-1,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0-1-1,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 1-1,1-1 0,-1 0 0,-9-22 104,-1 10-147,0 1-1,-1 0 1,0 0 0,-1 1-1,0 1 1,-1 0 0,-17-9 0,-10-4-172,-50-19 0,79 38 192,-22-11 96,33 13-79,0 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 1,1 1-1,-1-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 1,1 0-1,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 1,25-13-107,-1 1 1,1 1 0,1 1 0,30-7 0,24-9-1583,-20 4-1106,-1-3-2238</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-69255.24">9114 8316 1601,'0'0'7323,"-20"-2"-7053,-63 0-108,77 3-150,0 0 1,0 0-1,0 1 0,0-1 0,1 1 0,-1 1 0,1-1 0,-1 1 1,1 0-1,0 0 0,0 1 0,0-1 0,0 1 0,1 0 0,-7 8 1,4-4-2,0 1 1,1 0-1,0 0 1,0 0-1,1 1 1,-6 16-1,4-5-7,2 1 0,0-1 0,1 1-1,-2 36 1,6 94 362,2-73 535,-3-78-864,1 1 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,1-1 1,-1 0-1,0 0 0,0 1 0,1-1 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 1,1 0-1,0-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 0 0,0 0 1,0 1-1,-1-1 0,1-1 0,0 1 1,0 0-1,-1 0 0,4-1 0,3-1-19,-1-1 0,0 1 0,0-1 0,-1 0 0,1-1-1,0 1 1,-1-1 0,0-1 0,9-7 0,0-5-1652,-7 3-3997,-7 8 354</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-68943.67">8729 8892 2897,'0'0'9477,"-15"0"-9477,25 0-4434,0 0-1041</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-68943.68">8729 8892 2897,'0'0'9477,"-15"0"-9477,25 0-4434,0 0-1041</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-68008.59">8716 8892 3522,'105'21'3270,"-103"-21"-3182,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,-1-1 0,1 1-1,0-1 1,0 0 0,0 1 0,0-1-1,-1 0 1,1 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,0 0 1,-1-1 0,2-8 437,6-6-330,0 1 0,2-1 0,-1 1-1,12-13 1,-11 14-175,0 1-1,0-1 1,-1-1-1,-1 1 1,7-21 0,-4-2-7,-2-1 0,-1 0 1,-2 0-1,-2 0 0,-1 0 1,-4-51-1,2 85-28,0 2 11,0 1-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,-1 1 1,1-1 0,0 1 0,-2-1 0,2 3-7,0-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1-1,1 1 1,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,1 1 0,-1 1-4,-7 70 475,6 111 1,1-180-447,0-1 1,1 1 0,-1 0-1,1-1 1,0 1 0,1-1-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 0 0,0 0-1,1 0 1,0 0 0,0-1-1,0 1 1,0-1 0,0 0-1,7 5 1,-5-5 6,1 0 1,-1-1-1,1 1 1,-1-1-1,1-1 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 0,0 0 1,0 0-1,8-2 0,-10 1-8,0 0-1,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 0-1,-1 0 0,0-1 1,1 1-1,-1-1 1,0 0-1,3-3 1,34-46 65,-34 43-67,12-17-188,-1-1-1,-1-1 1,-2 0-1,-1-2 1,-1 1-1,-2-1 1,-1-1-1,-1 0 1,-2 0-1,-1 0 1,-1-1-1,-1-33 1,-2 43 37,-1-69-243,-1 85 353,0-1 1,0 0 0,0 1-1,-1 0 1,0-1 0,0 1-1,-1 0 1,0 0 0,0 0-1,0 0 1,-5-5 0,7 9 21,1 1 0,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 0,-1 1 1,1-1-1,0 1 0,0-1 0,-1 1 0,1 0 1,0 0-1,-1-1 0,1 1 0,-1 0 1,1 0-1,0 0 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,-1 1 1,1 0-1,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 1 0,0-1 0,0 0 1,1 0-1,-2 2 0,-3 5-8,0 0 1,1 0-1,0 1 0,0-1 0,-4 18 1,0 18 161,1-1-1,2 1 1,3 1 0,4 66 0,-1-34 130,-1-49-136,2 0-1,1 0 0,11 48 0,-10-60-100,1-1 0,0 1 1,2-1-1,-1 0 0,2-1 0,0 0 0,17 24 0,-22-35-35,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,5 2 0,-8-3 2,1 1 1,-1-1-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,-1 0 1,2-3-1,2-9 22,-1 0-1,-1 1 0,0-1 0,0 0 0,-1-25 1,-1 35-18,0 0 0,0-1 1,0 1-1,0 0 1,-1-1-1,0 1 1,1 0-1,-1 0 1,0-1-1,0 1 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,0 1-1,0-1 1,0 0-1,0 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,1 0-1,-1 1 0,-6-4 1,8 8-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 1 1,1-1-1,2 5 0,-2-8-85,0 1 1,0-1 0,1 0 0,-1 1 0,0-1-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,0-1 0,1 1 0,-1-1 0,1 0-1,26-19-3081,-17 12 645,8-6-2061</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-67868.55">9544 8566 2673,'0'0'4354,"0"20"-4354,10-20-4546</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-67499.83">9925 8018 4818,'0'0'2263,"-22"-5"-1709,-65-16 247,84 20-756,0 1 1,0-1 0,0 1-1,0 0 1,0-1 0,1 1-1,-1 1 1,0-1-1,0 0 1,0 1 0,0-1-1,0 1 1,1 0-1,-1 0 1,0 0 0,0 0-1,1 1 1,-1-1-1,1 1 1,-1-1 0,1 1-1,0 0 1,-4 4 0,2 0-21,-1 0 1,1 0-1,1 1 1,-1 0-1,1 0 1,-4 11 0,1-2 103,-6 16 64,1 1-1,1 0 1,2 0-1,2 1 1,-4 41-1,3 173 1245,7-220-1217,0 2-76,1 0-1,11 57 1,-10-76-108,1-1 0,0 1 0,0-1 1,1 0-1,0 0 0,1 0 0,0-1 0,1 0 0,0 0 0,0 0 0,12 11 1,-17-18-13,0-1 1,0 0-1,0 1 1,1-1-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0-1 0,-1 1-1,1-1 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 1,0-1 0,0 1-1,-1-1 1,1 0-1,-1 0 1,1 1-1,-1-1 1,3-2 0,2-3-506,0 0 0,0 0 1,0-1-1,-1 0 0,9-13 1,-1 0-2584,10-7-2883</inkml:trace>
@@ -13497,7 +13497,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-31544.58">11928 13714 5042,'0'0'5763,"34"58"-10453,-20-22 736</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-30323.67">12088 14051 816,'0'0'8615,"0"17"-7388,0 148 2783,0-114-2729,1-51-1283,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,25-12 156,-17 3-72,-1-1-1,0 0 0,12-22 1,21-29 91,-41 62-170,0 0 0,1-1 0,-1 1-1,0 0 1,0-1 0,0 1 0,1 0 0,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,0 0 0,1 0-1,-1 0 1,0-1 0,1 1 0,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 1 0,-1-1 0,0 0-1,1 0 1,-1 1 0,10 18 136,1 24 129,-9-30-222,1 0-1,0 1 1,0-1-1,11 22 1,-13-32-158,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,0-1 0,1 1 0,-1 0 1,0-1-1,1 0 0,-1 1 0,1-1 0,-1-1 0,7 2 0,1-1-734,0 0 1,0-1 0,0 0 0,0-1-1,0 0 1,0-1 0,17-5 0,-24 6 706,-1 0 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,0-1 1,0 0-1,0 1 1,-1-1-1,1 0 0,0 0 1,-1-1-1,0 1 1,0 0-1,0-1 1,0 1-1,-1-1 1,1 0-1,-1 0 0,0 1 1,0-1-1,1-7 1,-1 3 425,0 0 1,-1 0 0,0 0 0,0 0-1,-1 0 1,0 0 0,0 0-1,-1 0 1,0 0 0,0 0 0,-5-10-1,5 16-95,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0 0 0,1-1 0,-4 2 0,2 1-156,1-1 0,-1 0 0,1 1 0,0 0-1,0 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,0 0 0,0 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,1 4 0,-1-8-43,-1-1 1,1 1-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,1-1 0,-1 1-1,0-1 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 1-1,2-1 1,34-18-36,-25 7-28,0-1 0,-1 0 1,0 0-1,-1-1 0,0 0 0,-2 0 1,1-1-1,-2-1 0,0 1 0,-1-1 0,0-1 1,3-18-1,-1-8 47,-1-1 1,-3 0-1,0-66 0,-4 131 85,-1 24 361,3 0 0,8 56 0,-8-89-356,0-1 1,1 0-1,0 0 1,1 0-1,0 0 1,0 0-1,1-1 0,1 0 1,0 0-1,0 0 1,1-1-1,0 0 1,1 0-1,11 11 1,-17-18-57,0 0 1,1 0-1,-1 0 1,0 0-1,1-1 1,0 1 0,-1-1-1,1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,0-1 1,0 1 0,0-1-1,0 0 1,0 1-1,0-2 1,0 1-1,0 0 1,0 0 0,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1-1 1,1 1 0,-1-1-1,1 0 1,-1 1-1,1-1 1,-1-1-1,0 1 1,0 0-1,0 0 1,0-1 0,-1 1-1,1-1 1,-1 0-1,1 1 1,-1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0-4-1,2-7 12,-1 1 0,0 0-1,0-20 1,-2 30-17,0 1 0,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,0 1 0,0-1 0,0 0 0,-3-1 0,4 2-6,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,1 1 0,-1 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 2 0,-5 43 36,5-39-80,0 7 29,0 0 0,0 0 0,1-1 0,1 1 0,0-1 0,7 20 0,-8-29-201,1-1-1,0 1 0,0-1 0,0 1 0,0-1 1,1 0-1,0 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,-1-1 0,1 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,0-1 1,0 1-1,0-1 0,0 0 0,7 0 0,-4-1-137,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-2 0,0 1 0,0-1 0,-1 1 0,1-2 0,-1 1 0,0 0-1,0-1 1,0 0 0,0 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,4-12-1,2-3 903,-2-1-1,0 0 1,-1 0-1,-1 0 0,3-43 1,-7 51-199,1-14 4312,-2 16-564,-3 26-3277,-16 104-1195,-6-43-5381,25-76 5553,0 1 0,0 0-1,0 0 1,0-1 0,-1 1 0,1 0-1,0-1 1,0 1 0,-1-1 0,1 1 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 1 0,-1-1-1,0 1 1,1-1 0,-1 0 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0 0,1 0-1,-1 1 1,0-1 0,-1 0 0,-9-14-2129,-1-33 3315,11 45-840,-8-29 2632,-1-17 5175,18 47-7177,69 11-1960,-30-2-1948,-4-4-2515</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-29995.63">13297 13588 7235,'0'0'6096,"20"-11"-5228,0-1-636,1 1 0,24-8 0,-41 18-186,0 0 1,0 0-1,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 1-1,-1-1 1,0 1-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 1 1,0 0-1,-1 0 1,1 1-1,0-1 1,-1 1-1,1-1 1,-1 1-1,0 0 1,0 1-1,4 4 1,-1-2 16,7 8 95,0 2 0,-1-1 0,-1 1-1,0 1 1,-1 0 0,-1 0 0,-1 1-1,0 1 1,-2-1 0,0 1 0,-1 0-1,5 36 1,-2 17 240,-3 0 0,-6 85 0,0-66-145,3-41-143,0-36-92,-1 0-1,-1 0 1,0 0 0,0 0 0,-2-1-1,0 1 1,0 0 0,-8 21-1,9-32-4,-1-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,-1-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,1-1 1,-1 1-1,0-1 0,-5 0 0,-8 1 34,-1-1 0,-27-3 1,32 2-87,-227-29-5909,158 25 1491</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-29221.98">10464 13526 5731,'0'0'2155,"-18"-8"-1608,-1 0-429,1 1 0,-40-10 0,50 15-102,-1 0 0,0 1 0,1 1 0,-1-1 0,0 1 1,1 1-1,-1-1 0,0 1 0,1 1 0,-1 0 0,1 0 0,-14 6 0,10-3 9,0 1 0,0 1 1,1 0-1,0 0 0,0 1 0,1 1 0,0-1 0,-11 14 0,16-16 17,0 1-1,1 0 1,0 0-1,0 0 1,0 1-1,1-1 1,0 1-1,1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,0 1-1,1 9 1,1 55 571,3 0 1,15 75-1,20 248 2730,-34 5-158,-5-360-2816,23-41-324,-7-4 1,-1 0 0,0-1-1,0-1 1,0 0 0,21-12 0,15-7-78,-3 5-874,58-15 0,-86 29-645,1 2-1,0 1 1,22-1 0,-15 3-3603</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-29221.99">10464 13526 5731,'0'0'2155,"-18"-8"-1608,-1 0-429,1 1 0,-40-10 0,50 15-102,-1 0 0,0 1 0,1 1 0,-1-1 0,0 1 1,1 1-1,-1-1 0,0 1 0,1 1 0,-1 0 0,1 0 0,-14 6 0,10-3 9,0 1 0,0 1 1,1 0-1,0 0 0,0 1 0,1 1 0,0-1 0,-11 14 0,16-16 17,0 1-1,1 0 1,0 0-1,0 0 1,0 1-1,1-1 1,0 1-1,1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,0 1-1,1 9 1,1 55 571,3 0 1,15 75-1,20 248 2730,-34 5-158,-5-360-2816,23-41-324,-7-4 1,-1 0 0,0-1-1,0-1 1,0 0 0,21-12 0,15-7-78,-3 5-874,58-15 0,-86 29-645,1 2-1,0 1 1,22-1 0,-15 3-3603</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-26672.58">11060 13577 5699,'0'0'3172,"-15"-18"-2377,-2-7-586,9 12-65,-1 1 1,0 1-1,-1-1 0,0 2 1,-19-17-1,24 24-93,1-1 0,-1 1 0,0 0 1,0 1-1,0-1 0,-1 1 0,1 0 0,0 1 0,-1-1 1,1 1-1,-1 0 0,0 0 0,1 1 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,1 0 0,-1 0 1,1 1-1,-1 0 0,1 0 0,0 0 0,-8 4 0,-8 6-53,0 0-1,1 1 1,1 1-1,-30 27 1,27-20 32,0 1 1,2 1-1,0 0 1,2 2-1,1 0 1,1 1-1,1 1 1,1 0-1,1 1 1,2 0-1,0 1 1,3 0-1,-8 43 1,3-9 86,3 1 0,3 0 1,3 0-1,2 1 1,4-1-1,10 70 0,-5-99-70,1 0-1,2-1 0,2 0 0,1-1 0,1-1 0,2 0 0,1-1 0,2 0 0,1-2 0,41 48 0,-50-66-42,0-1-1,1 0 1,1-1-1,0 0 1,0-1-1,0 0 1,1-1-1,0 0 1,0-2-1,1 1 1,0-2-1,20 4 1,-24-6 6,0-1 0,0 0-1,0-1 1,0 0 0,0-1 0,0 0-1,0-1 1,0 0 0,0-1 0,-1 0-1,1 0 1,-1-1 0,0-1 0,0 0-1,0 0 1,-1-1 0,17-12 0,0-6 30,0-2 0,-2-1 0,-1 0 0,-1-2 0,-1 0 0,-2-2 0,-1 0 0,-2-1 0,0-1 0,-3 0 0,12-40 0,-3-7-66,-3-1-1,-4-1 0,8-142 0,-21 191-9,-1 1 0,-2 0 0,-1 0 0,-1 0 0,-2 0 0,-13-45 0,14 65 44,0-1-1,-1 0 0,-1 1 0,0 0 0,-1 1 0,0-1 1,-1 1-1,0 1 0,-1-1 0,0 1 0,-1 1 0,0 0 1,0 0-1,-1 1 0,0 0 0,0 1 0,-24-11 1,27 14-67,-1 1 1,1 0 0,-1 1 0,0-1-1,0 1 1,0 1 0,0 0 0,0 0-1,0 1 1,0 0 0,-1 1 0,1 0-1,0 0 1,0 1 0,-16 5 0,2 3-877,0 0 0,1 2 1,0 1-1,-28 20 0,-22 17-4272</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-25503.4">8901 16177 2145,'0'0'2076,"-2"-18"-105,1-8-1197,1 11-154,-1 1 1,0-1-1,-1 0 1,-6-16 0,5 22 1869,1 12-1055,-1 24-685,3 50-434,12 77 268,8 0-1,58 226 0,-74-362-666,-1-3-221,1 0 0,0 0 0,10 21 0,-12-33 16,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 0-1,0 1 1,0-1-1,7 1 1,15-1-4657</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-24942.57">8877 16050 2049,'0'0'5845,"11"-19"-3300,-6 9-2457,1 1 1,0-1-1,1 1 0,0 1 0,0-1 0,0 1 0,1 0 0,1 1 0,-1 0 0,1 0 0,1 1 0,-1 0 0,1 1 0,0 0 0,0 0 0,19-5 0,392-88 926,14 30-523,878-63-6,-1252 126-395,10-2 69,1 4 1,132 10 0,-198-7-125,1 2 0,-1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 1 1,-1 0-1,1 0 0,-1 1 0,0-1 0,0 1 0,0 0 0,-1 1 0,1-1 1,-1 1-1,0 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0 0 0,-1 0 1,0 0-1,0-1 0,1 8 0,2 16 198,-1 0 0,-1 1 0,-1-1 0,-4 46 0,1-24 118,-9 156 274,0-42-372,9-104-207,-7 114 48,5-151-79,0-1 1,-2 0 0,0 0 0,-1 0 0,-12 25 0,12-37-10,-1 0 0,0 0-1,-1 0 1,0-1 0,0-1 0,-1 1 0,0-2 0,-1 1 0,0-1-1,-1 0 1,1-1 0,-1-1 0,-1 1 0,1-2 0,-18 7-1,-22 6 30,0-3 0,-73 13 0,80-18-22,-1108 199 95,1031-189-96,81-13 3,-512 75-57,399-66 272,-247-7-1,387-9-158,0-1 0,-1-1-1,1 0 1,0 0 0,0-1 0,0-1 0,-22-10-1,32 13-61,-1-1-1,1 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,1-1 0,-1 0 1,1 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,1-1-1,0 1 1,0 0-1,0-1 0,0 1 1,1-1-1,-1 1 1,1-1-1,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 1,1 1-1,0 0 1,2-7-1,2 0-260,0-1 0,1 2 1,0-1-1,1 1 0,0 0 0,0 0 0,1 1 0,0 0 1,0 0-1,1 1 0,0 0 0,11-6 0,4-6-1265,38-31-3737</inkml:trace>
@@ -13511,15 +13511,15 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55386.74">12571 4763 5907,'0'0'8838,"-2"70"-6546,-15 13-1957,11-60-185,1 1-1,1 0 1,-1 35 0,34-58 554,-22-1-610,-1-1 0,1 0 0,0 0 1,-1-1-1,0 0 0,1 0 0,-1-1 0,0 0 0,0 0 0,0 0 0,7-5 0,-5 3-731,0 0 0,1 0 0,0 1-1,11-3 1,0 3-7470,-6-1 1677</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55725.34">12906 4763 5715,'0'0'9140,"-5"-5"-8342,3 3-764,1 0 0,0 0 0,-1 1 0,0-1 0,1 1 0,-1 0 1,0-1-1,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,-3 0-1,3 1-19,0 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0 0 0,1-1 0,-1 2 0,0-1 0,0 0 0,1 0 0,-1 0 1,0 1-1,1-1 0,-1 1 0,1-1 0,-2 3 0,-5 6 109,-1 0 0,1 1 0,0 0 0,1 0-1,1 1 1,0 0 0,0 0 0,1 1 0,1-1-1,0 1 1,0 0 0,2 0 0,0 0 0,0 1 0,1-1-1,1 15 1,0-26-122,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,1-1 1,-1 1 0,0-1-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0-1 0,0 0-1,0 1 1,0-1 0,2 0-1,13 2 60,0-1 0,0 0 0,18-2 1,-13 0 2,3-2 559,-13 1-2069,-1 1-5924,-19 1 1511</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56848.23">10485 5390 4674,'0'0'3989,"-6"3"-3538,-3 1-272,1 1 1,0 0-1,0 1 1,1 0-1,0 0 1,0 0-1,0 1 1,1 0 0,0 1-1,-8 12 1,-52 96 1544,50-83-1150,-3 2-78,-66 135 1421,72-138-1556,1 1 1,1 0-1,-9 49 0,18-71-314,1-4-1655,5-11-646,6-7 1072,18-15-2433,5-8-1000</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57348.22">10841 5471 2209,'0'0'6744,"-4"-2"-5943,2 1-718,0-1 1,0 1 0,0 0-1,0 1 1,-1-1 0,1 0 0,0 1-1,0-1 1,0 1 0,-1 0-1,1 0 1,0-1 0,-1 2-1,1-1 1,0 0 0,0 0-1,-1 1 1,1-1 0,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 1-1,1-1 1,-1 1 0,0-1-1,-2 5 1,-206 317 3844,130-191-3064,68-113-776,4-9-30,1 1 0,0-1 0,1 1 0,1 0-1,-1 1 1,2-1 0,0 1 0,0 0 0,-2 14 0,6-26-379,2 0-754,7-1 335,0-1 0,-1-1 0,0 1 0,0-1 0,0-1 0,0 1-1,0-2 1,-1 1 0,14-10 0,-15 9 58,43-30-5060</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57348.21">10841 5471 2209,'0'0'6744,"-4"-2"-5943,2 1-718,0-1 1,0 1 0,0 0-1,0 1 1,-1-1 0,1 0 0,0 1-1,0-1 1,0 1 0,-1 0-1,1 0 1,0-1 0,-1 2-1,1-1 1,0 0 0,0 0-1,-1 1 1,1-1 0,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 1-1,1-1 1,-1 1 0,0-1-1,-2 5 1,-206 317 3844,130-191-3064,68-113-776,4-9-30,1 1 0,0-1 0,1 1 0,1 0-1,-1 1 1,2-1 0,0 1 0,0 0 0,-2 14 0,6-26-379,2 0-754,7-1 335,0-1 0,-1-1 0,0 1 0,0-1 0,0-1 0,0 1-1,0-2 1,-1 1 0,14-10 0,-15 9 58,43-30-5060</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57903.44">11492 5386 880,'0'0'6473,"-8"8"-5379,-153 175 3100,12-11-1970,-36 8-881,95-96-902,3 4 0,-79 105 0,87-68 149,58-87-346,-2-1-1,-40 49 0,62-85-253,13-5-1829,20-19-1908,34-32 0,-63 52 3462,40-35-4360</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58361.36">11577 5782 3426,'0'0'7806,"-7"8"-6896,-453 460 5131,212-231-5157,193-182-727,3 3-1,3 2 0,2 2 1,-57 101-1,103-163-155,-4 9 0,0 1 1,1-1 0,-1 1-1,2 0 1,-5 16 0,8-24-189,8-11-2003,53-45-4243,-18 17 2122</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58822.48">11604 6345 2449,'0'0'7430,"6"-3"-6472,-2 0-715,-2 1-167,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0-1,0 1 1,0-1 0,3 0 1931,-6 6-1815,-1-1 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1-1,0-1 1,0 0 0,-4 3 0,-4 6 143,-203 204 1758,-24 28-1037,25 5-473,204-233-2366,23-18-3555,12-9-824,-14 4 5008,17-14-4197</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59153.4">11663 6718 4882,'0'0'4848,"6"-4"-4176,20-10-72,-19 10-66,-10 21 957,-3-5-972,0 0 0,-1-1 0,-1 0 0,0 0 0,-15 15 0,-14 19 380,31-37-777,-118 161 2061,122-167-2189,-1 1-20,1 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,-1 8-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60428.09">10300 4891 3714,'0'0'12894,"0"3"-12838,-20 406 3743,20-399-3427,-2-24-1003,-1-29-6527,3 26 1587</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60973.01">10480 5175 6611,'0'0'10229,"0"-2"-10165,0 18 112,0 7 160,-10-1-80,1 3-64,-1 3-112,-5-6 48,1 3-128,9-8-96,5-6-1056,0-8-2178</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61436.79">10756 5039 4370,'0'0'10992,"0"-7"-10043,0-21-252,0 27-660,1 0 1,-1 1 0,0-1 0,1 1-1,-1-1 1,0 0 0,1 1-1,-1-1 1,0 1 0,1-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,-1 1 0,1 0 0,0-1-1,-1 1 1,1 0 0,-1 0-1,1-1 1,0 1 0,-1 0-1,1 0 1,0 0 0,-1-1-1,1 1 1,0 0 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,24 6-8,-22-2-20,0 0-1,0 1 0,0-1 1,-1 0-1,0 1 1,1-1-1,-2 1 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 0,-1 7 1,1-3 42,0 0-1,-1 1 1,0-1 0,0 0 0,-1 0 0,0 0-1,-1 0 1,-4 10 0,-6-1 102,10-15-50,1 0-1,-1 0 1,1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 4 0,27-9-147,-12-2-57,-1 0-1,0-1 1,0 0-1,0-1 1,19-10 0,28-18-3271,-38 21 357,-4-1-1415,-2 0-1942</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63113.22">11273 7640 5923,'0'0'9935,"-4"0"-8604,3 0-1262,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 1,1 1-1,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 1,-1 1-1,0-2 0,1 1-51,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 1,1 0-1,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 0 0,0 1 1,-1-1-1,1 1 0,0 0 1,0-1-1,1 0 0,4-2 43,-1-1 1,1 1-1,0 1 0,1-1 0,-1 1 0,0 0 0,1 0 1,-1 1-1,1 0 0,-1 0 0,1 0 0,10 1 0,-14 1-52,0-1-1,1 0 1,-1 1-1,0 0 1,0-1-1,-1 1 1,1 0-1,0 1 1,0-1-1,0 0 0,-1 1 1,1 0-1,-1 0 1,1-1-1,-1 1 1,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,-1-1 0,1 1 1,-1 0-1,1 0 1,-1-1-1,0 1 1,0 0-1,1 4 1,0 2 6,0-1 0,-1 0 0,-1 1 0,1-1 1,-1 1-1,0-1 0,-1 1 0,0-1 0,-1 0 0,1 1 1,-2-1-1,1 0 0,-1 0 0,0 0 0,-1 0 1,0-1-1,0 1 0,-6 7 0,-9 9-7,0-1 1,-2-2-1,-41 36 1,36-35-8,14-12-24,-6 3 169,19-10-70,10-6-41,12-5-15,1-1 0,-2-1 0,1 0 0,-1-2 0,21-15 0,-35 19-3196,-5 7 264,4 1-1661,6 0-2264</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61436.78">10756 5039 4370,'0'0'10992,"0"-7"-10043,0-21-252,0 27-660,1 0 1,-1 1 0,0-1 0,1 1-1,-1-1 1,0 0 0,1 1-1,-1-1 1,0 1 0,1-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,-1 1 0,1 0 0,0-1-1,-1 1 1,1 0 0,-1 0-1,1-1 1,0 1 0,-1 0-1,1 0 1,0 0 0,-1-1-1,1 1 1,0 0 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,24 6-8,-22-2-20,0 0-1,0 1 0,0-1 1,-1 0-1,0 1 1,1-1-1,-2 1 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 0,-1 7 1,1-3 42,0 0-1,-1 1 1,0-1 0,0 0 0,-1 0 0,0 0-1,-1 0 1,-4 10 0,-6-1 102,10-15-50,1 0-1,-1 0 1,1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 4 0,27-9-147,-12-2-57,-1 0-1,0-1 1,0 0-1,0-1 1,19-10 0,28-18-3271,-38 21 357,-4-1-1415,-2 0-1942</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63113.21">11273 7640 5923,'0'0'9935,"-4"0"-8604,3 0-1262,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 1,1 1-1,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 1,-1 1-1,0-2 0,1 1-51,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 1,1 0-1,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 0 0,0 1 1,-1-1-1,1 1 0,0 0 1,0-1-1,1 0 0,4-2 43,-1-1 1,1 1-1,0 1 0,1-1 0,-1 1 0,0 0 0,1 0 1,-1 1-1,1 0 0,-1 0 0,1 0 0,10 1 0,-14 1-52,0-1-1,1 0 1,-1 1-1,0 0 1,0-1-1,-1 1 1,1 0-1,0 1 1,0-1-1,0 0 0,-1 1 1,1 0-1,-1 0 1,1-1-1,-1 1 1,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,-1-1 0,1 1 1,-1 0-1,1 0 1,-1-1-1,0 1 1,0 0-1,1 4 1,0 2 6,0-1 0,-1 0 0,-1 1 0,1-1 1,-1 1-1,0-1 0,-1 1 0,0-1 0,-1 0 0,1 1 1,-2-1-1,1 0 0,-1 0 0,0 0 0,-1 0 1,0-1-1,0 1 0,-6 7 0,-9 9-7,0-1 1,-2-2-1,-41 36 1,36-35-8,14-12-24,-6 3 169,19-10-70,10-6-41,12-5-15,1-1 0,-2-1 0,1 0 0,-1-2 0,21-15 0,-35 19-3196,-5 7 264,4 1-1661,6 0-2264</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63449.28">11616 7843 7668,'0'0'9791,"5"-2"-9210,-3 2-536,-1-1-1,1 1 0,-1 0 0,1-1 1,-1 1-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 1 0,0-1 0,-1 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1 0 0,1 0 0,1 1 1,-1 1 10,0-1 1,0 1 0,0-1 0,0 1-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 4-1,0-3-6,0 1 0,0 0-1,0 0 1,-1-1-1,0 1 1,0 0 0,0 0-1,0 0 1,-1-1-1,0 1 1,0 0 0,0 0-1,0-1 1,-1 1-1,-3 5 1,1-5-26,0 1 0,-1-1 0,1-1 0,-1 1 0,0-1 0,-1 0-1,1 0 1,-1 0 0,1-1 0,-10 4 0,2 0-43,10-4-44,-1-1 0,1 0 0,-1 0 0,0-1 1,0 1-1,1-1 0,-1 0 0,-7 2 0,9-3-1056,4-9-6588,6-10-936</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63743.25">11767 7682 8612,'0'0'10287,"0"9"-9684,0 239 2059,0-138-8883</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64086">12116 7604 8324,'0'0'10437,"20"58"-9685,-1-10-160,1-1-224,-1 6-272,-9-3-48,-5-3-48,-5 1-80,-25-4-352,-23-2-928,-11-3-2066,-9-6-2048,-10-5-4371</inkml:trace>
@@ -13697,7 +13697,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">18 141 3025,'0'0'10082,"-5"-8"-2880,3 6-7899,1 2 641,-7 52-1799,7-49 1844,1-1-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,0 1-1,1-1 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,1 2-1,2-2-50,-1-1-1,0 0 1,0 0 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1-1 1,7-1 0,-9 1 62,-1 0 1,0-1-1,1 1 1,-1 0-1,0-1 1,1 0-1,-1 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1-1 1,-1 1-1,1 0 1,0 0-1,0-4 0,0 0 15,0-1-1,0 1 1,0 0-1,-1-1 1,0 1-1,-1-1 0,1 1 1,-1 0-1,0-1 1,-4-9-1,4 14-15,-1 1 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 1 0,-1-1 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,-2 1 0,-40 1-146,43-1 104,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 3 0,0 19-7828</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="720.76">243 47 4034,'0'0'7886,"21"-1"-7603,-18 4-278,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 1 0,0-1-1,1 1 1,-1 0-1,0-1 1,-1 1 0,1 0-1,-1 0 1,0 0 0,2 9-1,0 2 47,-1 0 0,1 31 0,-2-37 1095,3-17-1246,12-18-439,32-9 237,-38 29 314,0 0 0,-1-1 1,1-1-1,8-9 0,-17 16-1,-1-1-3,0 2 24,0 21-301,0 51 698,0-42-6402</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="890.05">506 2 5491,'0'0'6514,"12"-2"-9891,-4 11 752,0 6-1793</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1721.68">699 74 3394,'0'0'7808,"-4"0"-7362,-3 0-430,1 0-1,0 1 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,1 2 1,-1-1 0,-6 4-1,9-4-53,0-1 0,1 1 0,-1 1-1,1-1 1,-1 0 0,1 0 0,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,1 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,1-1-1,0 0 1,-1 7 0,1-10 3,1 0 1,-1 1-1,0-1 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,1 1 1,-1-1-1,0 0 0,1 0 1,-1 1-1,0-1 0,1 0 1,-1 0-1,0 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,1-1 1,1 0 69,0 0 1,-1 1-1,1-2 1,-1 1-1,1 0 1,-1 0 0,1 0-1,-1-1 1,0 1-1,1-1 1,-1 1-1,1-3 1,4-13 513,4-9 1237,-5 27-1310,0 17-798,1 15 361,-1 1 0,-3-1 0,0 1 0,-6 64 0,3-96-30,1 0 1,-1 0-1,0 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,-1-1-1,1 1 1,0-1-1,0 1 1,-3 1-1,3-2-7,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1-7-142,0 0-1,1 0 0,0 0 1,1 0-1,-1 0 0,2 0 0,-1 0 1,1 0-1,0 1 0,7-12 0,0 4-199,0 1-1,1 1 0,0 0 0,15-13 0,-23 23 320,5-4 48,0 0 0,-1 0 0,0-1 0,0 0 1,-1 0-1,0-1 0,0 0 0,-1 0 0,0 0 1,4-12-1,-7 16 3455,-15 72-4286,16-66-2114</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1721.67">699 74 3394,'0'0'7808,"-4"0"-7362,-3 0-430,1 0-1,0 1 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,1 2 1,-1-1 0,-6 4-1,9-4-53,0-1 0,1 1 0,-1 1-1,1-1 1,-1 0 0,1 0 0,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,1 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,1-1-1,0 0 1,-1 7 0,1-10 3,1 0 1,-1 1-1,0-1 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,1 1 1,-1-1-1,0 0 0,1 0 1,-1 1-1,0-1 0,1 0 1,-1 0-1,0 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,1-1 1,1 0 69,0 0 1,-1 1-1,1-2 1,-1 1-1,1 0 1,-1 0 0,1 0-1,-1-1 1,0 1-1,1-1 1,-1 1-1,1-3 1,4-13 513,4-9 1237,-5 27-1310,0 17-798,1 15 361,-1 1 0,-3-1 0,0 1 0,-6 64 0,3-96-30,1 0 1,-1 0-1,0 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,-1-1-1,1 1 1,0-1-1,0 1 1,-3 1-1,3-2-7,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1-7-142,0 0-1,1 0 0,0 0 1,1 0-1,-1 0 0,2 0 0,-1 0 1,1 0-1,0 1 0,7-12 0,0 4-199,0 1-1,1 1 0,0 0 0,15-13 0,-23 23 320,5-4 48,0 0 0,-1 0 0,0-1 0,0 0 1,-1 0-1,0-1 0,0 0 0,-1 0 0,0 0 1,4-12-1,-7 16 3455,-15 72-4286,16-66-2114</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2344.99">953 80 7043,'0'0'3492,"0"12"-3121,4 102 1043,0-111-1123,6-9 1,5-8 134,30-59 70,-44 73-498,-1-1 1,1 1-1,-1-1 1,1 1-1,-1 0 1,1-1-1,0 1 0,-1 0 1,1-1-1,-1 1 1,1 0-1,0 0 0,-1 0 1,1 0-1,0-1 1,0 1-1,-1 0 1,1 0-1,0 0 0,-1 1 1,1-1-1,0 0 1,-1 0-1,1 0 0,0 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 1-1,-1-1 0,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 0,0 2 1,25 22 117,-18-16 185,-4-5-245,0 0 0,0 0 0,1 0 0,-1-1-1,1 1 1,0-1 0,0 0 0,0-1-1,9 3 1,11-2-4036</inkml:trace>
 </inkml:ink>
 </file>
@@ -34688,7 +34688,7 @@
       <c r="C4" s="7">
         <v>100</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>64</v>
       </c>
       <c r="E4" s="7">
@@ -34842,10 +34842,10 @@
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B23" s="12">
+      <c r="B23" s="10">
         <v>44958</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="11">
         <v>120</v>
       </c>
       <c r="E23" s="14"/>
@@ -34857,10 +34857,10 @@
       <c r="K23" s="14"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B24" s="12">
+      <c r="B24" s="10">
         <v>44959</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="11">
         <v>200</v>
       </c>
       <c r="E24" s="14"/>
@@ -34872,18 +34872,18 @@
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <v>44960</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="11">
         <v>150</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <v>44961</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="11">
         <v>180</v>
       </c>
       <c r="E26">
@@ -34892,18 +34892,18 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B27" s="12">
+      <c r="B27" s="10">
         <v>44962</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="11">
         <v>220</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <v>44963</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="11">
         <v>170</v>
       </c>
       <c r="E28">
@@ -55646,8 +55646,8 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -55786,102 +55786,102 @@
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -55896,7 +55896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65F423C-4131-4500-AE43-217D44B98427}">
   <dimension ref="B2:B235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+    <sheetView topLeftCell="A199" workbookViewId="0">
       <selection activeCell="T206" sqref="T206"/>
     </sheetView>
   </sheetViews>
@@ -57460,55 +57460,55 @@
       </c>
     </row>
     <row r="13" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="13" t="s">
         <v>472</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
       <c r="K13" s="7" t="str">
         <f>INDEX(Dataset!A1:B501,MATCH('Vlookup Hlookup'!C19,Dataset!A1:A501,0),MATCH("Sport",Dataset!A1:B1,0))</f>
         <v>Athletics</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B18" s="6"/>
@@ -57622,51 +57622,51 @@
       <c r="B35" s="6"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B43" t="s">

</xml_diff>